<commit_message>
II Core, II Windows 1.2.2: 12 Lead Colors & Grid - Localizations updated - 12L ECG color schemes added: Light and Dark   - Options added to Menu drop-down - 12L ECG option to show background grid   - Pink/red 12L ECG background implemented
</commit_message>
<xml_diff>
--- a/II Core/Localization Strings.xlsx
+++ b/II Core/Localization Strings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibi\Documents\Infirmary Integrated\II Core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D1A758-1E3A-429A-B726-EF198859DCE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C737C2D-1D78-40D1-8B4C-2F37F0371AB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="203" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9304" uniqueCount="3471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9400" uniqueCount="3519">
   <si>
     <t>Temperature</t>
   </si>
@@ -10438,6 +10438,150 @@
   </si>
   <si>
     <t>تغییر اندازه خودکار</t>
+  </si>
+  <si>
+    <t>MENU:MenuColorSchemeDark</t>
+  </si>
+  <si>
+    <t>MENU:MenuColorSchemeLight</t>
+  </si>
+  <si>
+    <t>Dark</t>
+  </si>
+  <si>
+    <t>Light</t>
+  </si>
+  <si>
+    <t>Colori scuri</t>
+  </si>
+  <si>
+    <t>Dunkle Farben</t>
+  </si>
+  <si>
+    <t>Colores oscuros</t>
+  </si>
+  <si>
+    <t>Couleurs sombres</t>
+  </si>
+  <si>
+    <t>צבעים כהים</t>
+  </si>
+  <si>
+    <t>गहरे रंग</t>
+  </si>
+  <si>
+    <t>어두운 색</t>
+  </si>
+  <si>
+    <t>Cores escuras</t>
+  </si>
+  <si>
+    <t>Темные цвета</t>
+  </si>
+  <si>
+    <t>Rangi nyeusi</t>
+  </si>
+  <si>
+    <t>ደማቅ ቀለሞች</t>
+  </si>
+  <si>
+    <t>ألوان داكنة</t>
+  </si>
+  <si>
+    <t>暗色</t>
+  </si>
+  <si>
+    <t>رنگهای تیره</t>
+  </si>
+  <si>
+    <t>رنگ های روشن</t>
+  </si>
+  <si>
+    <t>الوان فاتحة</t>
+  </si>
+  <si>
+    <t>ቀላል ቀለሞች</t>
+  </si>
+  <si>
+    <t>浅色</t>
+  </si>
+  <si>
+    <t>Helle Farben</t>
+  </si>
+  <si>
+    <t>Colores claros</t>
+  </si>
+  <si>
+    <t>Couleurs claires</t>
+  </si>
+  <si>
+    <t>צבעים בהירים</t>
+  </si>
+  <si>
+    <t>हल्के रंग</t>
+  </si>
+  <si>
+    <t>Colori chiari</t>
+  </si>
+  <si>
+    <t>밝은 색상</t>
+  </si>
+  <si>
+    <t>Cores claras</t>
+  </si>
+  <si>
+    <t>Светлые цвета</t>
+  </si>
+  <si>
+    <t>Rangi nyepesi</t>
+  </si>
+  <si>
+    <t>MENU:MenuShowGrid</t>
+  </si>
+  <si>
+    <t>Show Grid</t>
+  </si>
+  <si>
+    <t>Onyesha gridi ya taifa</t>
+  </si>
+  <si>
+    <t>ፍርግርግ አሳይ</t>
+  </si>
+  <si>
+    <t>إظهار الشبكة</t>
+  </si>
+  <si>
+    <t>显示网格</t>
+  </si>
+  <si>
+    <t>Zeigen Sie das Raster</t>
+  </si>
+  <si>
+    <t>شبکه را نشان دهید</t>
+  </si>
+  <si>
+    <t>Mostrar la cuadrícula</t>
+  </si>
+  <si>
+    <t>Afficher la grille</t>
+  </si>
+  <si>
+    <t>הצג את הרשת</t>
+  </si>
+  <si>
+    <t>ग्रिड दिखाओ</t>
+  </si>
+  <si>
+    <t>Mostra la griglia</t>
+  </si>
+  <si>
+    <t>그리드 표시</t>
+  </si>
+  <si>
+    <t>Mostrar a grade</t>
+  </si>
+  <si>
+    <t>Показать сетку</t>
   </si>
 </sst>
 </file>
@@ -10815,11 +10959,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P287"/>
+  <dimension ref="A1:P290"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A219" sqref="A219:XFD219"/>
+      <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A216" sqref="A216:XFD216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="60.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20262,3359 +20406,3509 @@
     </row>
     <row r="214" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A214" s="4" t="s">
-        <v>1124</v>
+        <v>3472</v>
       </c>
       <c r="B214" s="4" t="s">
-        <v>76</v>
+        <v>3474</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>1655</v>
+        <v>3491</v>
       </c>
       <c r="D214" s="4" t="s">
-        <v>2069</v>
+        <v>3490</v>
       </c>
       <c r="E214" s="4" t="s">
-        <v>2359</v>
+        <v>3492</v>
       </c>
       <c r="F214" s="4" t="s">
-        <v>330</v>
+        <v>3493</v>
       </c>
       <c r="G214" s="4" t="s">
-        <v>2083</v>
+        <v>3489</v>
       </c>
       <c r="H214" s="4" t="s">
-        <v>170</v>
+        <v>3494</v>
       </c>
       <c r="I214" s="4" t="s">
-        <v>159</v>
+        <v>3495</v>
       </c>
       <c r="J214" s="4" t="s">
-        <v>2097</v>
+        <v>3496</v>
       </c>
       <c r="K214" s="4" t="s">
-        <v>2373</v>
+        <v>3497</v>
       </c>
       <c r="L214" s="4" t="s">
-        <v>206</v>
+        <v>3498</v>
       </c>
       <c r="M214" s="4" t="s">
-        <v>933</v>
+        <v>3499</v>
       </c>
       <c r="N214" s="4" t="s">
-        <v>244</v>
+        <v>3500</v>
       </c>
       <c r="O214" s="4" t="s">
-        <v>287</v>
+        <v>3501</v>
       </c>
       <c r="P214" s="4" t="s">
-        <v>1018</v>
+        <v>3502</v>
       </c>
     </row>
     <row r="215" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A215" s="4" t="s">
-        <v>1125</v>
+        <v>3471</v>
       </c>
       <c r="B215" s="4" t="s">
-        <v>77</v>
+        <v>3473</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>1656</v>
+        <v>3485</v>
       </c>
       <c r="D215" s="4" t="s">
-        <v>2070</v>
+        <v>3486</v>
       </c>
       <c r="E215" s="4" t="s">
-        <v>2360</v>
+        <v>3487</v>
       </c>
       <c r="F215" s="4" t="s">
-        <v>331</v>
+        <v>3476</v>
       </c>
       <c r="G215" s="4" t="s">
-        <v>2084</v>
+        <v>3488</v>
       </c>
       <c r="H215" s="4" t="s">
-        <v>171</v>
+        <v>3477</v>
       </c>
       <c r="I215" s="4" t="s">
-        <v>160</v>
+        <v>3478</v>
       </c>
       <c r="J215" s="4" t="s">
-        <v>2098</v>
+        <v>3479</v>
       </c>
       <c r="K215" s="4" t="s">
-        <v>2374</v>
+        <v>3480</v>
       </c>
       <c r="L215" s="4" t="s">
-        <v>207</v>
+        <v>3475</v>
       </c>
       <c r="M215" s="4" t="s">
-        <v>934</v>
+        <v>3481</v>
       </c>
       <c r="N215" s="4" t="s">
-        <v>245</v>
+        <v>3482</v>
       </c>
       <c r="O215" s="4" t="s">
-        <v>288</v>
+        <v>3483</v>
       </c>
       <c r="P215" s="4" t="s">
-        <v>1019</v>
+        <v>3484</v>
       </c>
     </row>
     <row r="216" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A216" s="4" t="s">
-        <v>1126</v>
+        <v>3503</v>
       </c>
       <c r="B216" s="4" t="s">
-        <v>45</v>
+        <v>3504</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>1591</v>
+        <v>3506</v>
       </c>
       <c r="D216" s="4" t="s">
-        <v>1817</v>
+        <v>3507</v>
       </c>
       <c r="E216" s="4" t="s">
-        <v>2270</v>
+        <v>3508</v>
       </c>
       <c r="F216" s="4" t="s">
-        <v>348</v>
+        <v>3509</v>
       </c>
       <c r="G216" s="4" t="s">
-        <v>1826</v>
+        <v>3510</v>
       </c>
       <c r="H216" s="4" t="s">
-        <v>349</v>
+        <v>3511</v>
       </c>
       <c r="I216" s="4" t="s">
-        <v>350</v>
+        <v>3512</v>
       </c>
       <c r="J216" s="4" t="s">
-        <v>1835</v>
+        <v>3513</v>
       </c>
       <c r="K216" s="4" t="s">
-        <v>2277</v>
+        <v>3514</v>
       </c>
       <c r="L216" s="4" t="s">
-        <v>351</v>
+        <v>3515</v>
       </c>
       <c r="M216" s="4" t="s">
-        <v>893</v>
+        <v>3516</v>
       </c>
       <c r="N216" s="4" t="s">
-        <v>837</v>
+        <v>3517</v>
       </c>
       <c r="O216" s="4" t="s">
-        <v>255</v>
+        <v>3518</v>
       </c>
       <c r="P216" s="4" t="s">
-        <v>984</v>
+        <v>3505</v>
       </c>
     </row>
     <row r="217" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A217" s="4" t="s">
-        <v>1129</v>
+        <v>1124</v>
       </c>
       <c r="B217" s="4" t="s">
-        <v>702</v>
+        <v>76</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>1659</v>
+        <v>1655</v>
       </c>
       <c r="D217" s="4" t="s">
-        <v>2073</v>
+        <v>2069</v>
       </c>
       <c r="E217" s="4" t="s">
-        <v>2363</v>
+        <v>2359</v>
       </c>
       <c r="F217" s="4" t="s">
-        <v>851</v>
+        <v>330</v>
       </c>
       <c r="G217" s="4" t="s">
-        <v>2087</v>
+        <v>2083</v>
       </c>
       <c r="H217" s="4" t="s">
-        <v>846</v>
+        <v>170</v>
       </c>
       <c r="I217" s="4" t="s">
-        <v>847</v>
+        <v>159</v>
       </c>
       <c r="J217" s="4" t="s">
-        <v>2101</v>
+        <v>2097</v>
       </c>
       <c r="K217" s="4" t="s">
-        <v>2377</v>
+        <v>2373</v>
       </c>
       <c r="L217" s="4" t="s">
-        <v>848</v>
+        <v>206</v>
       </c>
       <c r="M217" s="4" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="N217" s="4" t="s">
-        <v>849</v>
+        <v>244</v>
       </c>
       <c r="O217" s="4" t="s">
-        <v>850</v>
+        <v>287</v>
       </c>
       <c r="P217" s="4" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="218" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A218" s="4" t="s">
-        <v>1148</v>
+        <v>1125</v>
       </c>
       <c r="B218" s="4" t="s">
-        <v>1147</v>
+        <v>77</v>
       </c>
       <c r="C218" s="4" t="s">
-        <v>1660</v>
+        <v>1656</v>
       </c>
       <c r="D218" s="4" t="s">
-        <v>2074</v>
+        <v>2070</v>
       </c>
       <c r="E218" s="4" t="s">
-        <v>2364</v>
+        <v>2360</v>
       </c>
       <c r="F218" s="4" t="s">
-        <v>1167</v>
+        <v>331</v>
       </c>
       <c r="G218" s="4" t="s">
-        <v>2088</v>
+        <v>2084</v>
       </c>
       <c r="H218" s="4" t="s">
-        <v>1168</v>
+        <v>171</v>
       </c>
       <c r="I218" s="4" t="s">
-        <v>1169</v>
+        <v>160</v>
       </c>
       <c r="J218" s="4" t="s">
-        <v>2102</v>
+        <v>2098</v>
       </c>
       <c r="K218" s="4" t="s">
-        <v>2378</v>
+        <v>2374</v>
       </c>
       <c r="L218" s="4" t="s">
-        <v>1170</v>
+        <v>207</v>
       </c>
       <c r="M218" s="4" t="s">
-        <v>1171</v>
+        <v>934</v>
       </c>
       <c r="N218" s="4" t="s">
-        <v>1172</v>
+        <v>245</v>
       </c>
       <c r="O218" s="4" t="s">
-        <v>1173</v>
+        <v>288</v>
       </c>
       <c r="P218" s="4" t="s">
-        <v>1174</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="219" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="4" t="s">
-        <v>3441</v>
+        <v>1126</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>3442</v>
+        <v>45</v>
       </c>
       <c r="C219" s="4" t="s">
-        <v>3466</v>
+        <v>1591</v>
       </c>
       <c r="D219" s="4" t="s">
-        <v>3467</v>
+        <v>1817</v>
       </c>
       <c r="E219" s="4" t="s">
-        <v>3468</v>
+        <v>2270</v>
       </c>
       <c r="F219" s="4" t="s">
-        <v>3469</v>
+        <v>348</v>
       </c>
       <c r="G219" s="4" t="s">
-        <v>3470</v>
+        <v>1826</v>
       </c>
       <c r="H219" s="4" t="s">
-        <v>3458</v>
+        <v>349</v>
       </c>
       <c r="I219" s="4" t="s">
-        <v>3457</v>
+        <v>350</v>
       </c>
       <c r="J219" s="4" t="s">
-        <v>3459</v>
+        <v>1835</v>
       </c>
       <c r="K219" s="4" t="s">
-        <v>3460</v>
+        <v>2277</v>
       </c>
       <c r="L219" s="4" t="s">
-        <v>3461</v>
+        <v>351</v>
       </c>
       <c r="M219" s="4" t="s">
-        <v>3462</v>
+        <v>893</v>
       </c>
       <c r="N219" s="4" t="s">
-        <v>3463</v>
+        <v>837</v>
       </c>
       <c r="O219" s="4" t="s">
-        <v>3464</v>
+        <v>255</v>
       </c>
       <c r="P219" s="4" t="s">
-        <v>3465</v>
+        <v>984</v>
+      </c>
+    </row>
+    <row r="220" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="4" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B220" s="4" t="s">
+        <v>702</v>
+      </c>
+      <c r="C220" s="4" t="s">
+        <v>1659</v>
+      </c>
+      <c r="D220" s="4" t="s">
+        <v>2073</v>
+      </c>
+      <c r="E220" s="4" t="s">
+        <v>2363</v>
+      </c>
+      <c r="F220" s="4" t="s">
+        <v>851</v>
+      </c>
+      <c r="G220" s="4" t="s">
+        <v>2087</v>
+      </c>
+      <c r="H220" s="4" t="s">
+        <v>846</v>
+      </c>
+      <c r="I220" s="4" t="s">
+        <v>847</v>
+      </c>
+      <c r="J220" s="4" t="s">
+        <v>2101</v>
+      </c>
+      <c r="K220" s="4" t="s">
+        <v>2377</v>
+      </c>
+      <c r="L220" s="4" t="s">
+        <v>848</v>
+      </c>
+      <c r="M220" s="4" t="s">
+        <v>937</v>
+      </c>
+      <c r="N220" s="4" t="s">
+        <v>849</v>
+      </c>
+      <c r="O220" s="4" t="s">
+        <v>850</v>
+      </c>
+      <c r="P220" s="4" t="s">
+        <v>1022</v>
       </c>
     </row>
     <row r="221" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A221" s="4" t="s">
-        <v>445</v>
+        <v>1148</v>
       </c>
       <c r="B221" s="4" t="s">
-        <v>442</v>
+        <v>1147</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="D221" s="4" t="s">
-        <v>1847</v>
+        <v>2074</v>
       </c>
       <c r="E221" s="4" t="s">
-        <v>2189</v>
+        <v>2364</v>
       </c>
       <c r="F221" s="4" t="s">
-        <v>636</v>
+        <v>1167</v>
       </c>
       <c r="G221" s="4" t="s">
-        <v>1856</v>
+        <v>2088</v>
       </c>
       <c r="H221" s="4" t="s">
-        <v>639</v>
+        <v>1168</v>
       </c>
       <c r="I221" s="4" t="s">
-        <v>658</v>
+        <v>1169</v>
       </c>
       <c r="J221" s="4" t="s">
-        <v>2054</v>
-      </c>
-      <c r="K221" s="5" t="s">
-        <v>2198</v>
+        <v>2102</v>
+      </c>
+      <c r="K221" s="4" t="s">
+        <v>2378</v>
       </c>
       <c r="L221" s="4" t="s">
-        <v>685</v>
+        <v>1170</v>
       </c>
       <c r="M221" s="4" t="s">
-        <v>939</v>
+        <v>1171</v>
       </c>
       <c r="N221" s="4" t="s">
-        <v>643</v>
+        <v>1172</v>
       </c>
       <c r="O221" s="4" t="s">
-        <v>688</v>
+        <v>1173</v>
       </c>
       <c r="P221" s="4" t="s">
-        <v>442</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="222" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A222" s="4" t="s">
-        <v>446</v>
+        <v>3441</v>
       </c>
       <c r="B222" s="4" t="s">
-        <v>0</v>
+        <v>3442</v>
       </c>
       <c r="C222" s="4" t="s">
-        <v>1609</v>
+        <v>3466</v>
       </c>
       <c r="D222" s="4" t="s">
-        <v>1873</v>
+        <v>3467</v>
       </c>
       <c r="E222" s="4" t="s">
-        <v>2208</v>
+        <v>3468</v>
       </c>
       <c r="F222" s="4" t="s">
-        <v>311</v>
+        <v>3469</v>
       </c>
       <c r="G222" s="4" t="s">
-        <v>1889</v>
+        <v>3470</v>
       </c>
       <c r="H222" s="4" t="s">
-        <v>101</v>
+        <v>3458</v>
       </c>
       <c r="I222" s="4" t="s">
-        <v>141</v>
+        <v>3457</v>
       </c>
       <c r="J222" s="4" t="s">
-        <v>1913</v>
+        <v>3459</v>
       </c>
       <c r="K222" s="4" t="s">
-        <v>2225</v>
+        <v>3460</v>
       </c>
       <c r="L222" s="4" t="s">
-        <v>101</v>
+        <v>3461</v>
       </c>
       <c r="M222" s="4" t="s">
-        <v>910</v>
+        <v>3462</v>
       </c>
       <c r="N222" s="4" t="s">
-        <v>101</v>
+        <v>3463</v>
       </c>
       <c r="O222" s="4" t="s">
-        <v>270</v>
+        <v>3464</v>
       </c>
       <c r="P222" s="4" t="s">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="223" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A223" s="4" t="s">
-        <v>447</v>
-      </c>
-      <c r="B223" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C223" s="4" t="s">
-        <v>1607</v>
-      </c>
-      <c r="D223" s="4" t="s">
-        <v>1872</v>
-      </c>
-      <c r="E223" s="4" t="s">
-        <v>2206</v>
-      </c>
-      <c r="F223" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="G223" s="4" t="s">
-        <v>1888</v>
-      </c>
-      <c r="H223" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="I223" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="J223" s="4" t="s">
-        <v>1911</v>
-      </c>
-      <c r="K223" s="4" t="s">
-        <v>2223</v>
-      </c>
-      <c r="L223" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="M223" s="4" t="s">
-        <v>908</v>
-      </c>
-      <c r="N223" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="O223" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="P223" s="4" t="s">
-        <v>997</v>
+        <v>3465</v>
       </c>
     </row>
     <row r="224" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A224" s="4" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B224" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C224" s="4" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="D224" s="4" t="s">
-        <v>2103</v>
+        <v>1847</v>
       </c>
       <c r="E224" s="4" t="s">
-        <v>2209</v>
+        <v>2189</v>
       </c>
       <c r="F224" s="4" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="G224" s="4" t="s">
-        <v>2106</v>
+        <v>1856</v>
       </c>
       <c r="H224" s="4" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I224" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="J224" s="4" t="s">
-        <v>2109</v>
-      </c>
-      <c r="K224" s="4" t="s">
-        <v>2226</v>
+        <v>2054</v>
+      </c>
+      <c r="K224" s="5" t="s">
+        <v>2198</v>
       </c>
       <c r="L224" s="4" t="s">
-        <v>673</v>
+        <v>685</v>
       </c>
       <c r="M224" s="4" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="N224" s="4" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="O224" s="4" t="s">
-        <v>610</v>
+        <v>688</v>
       </c>
       <c r="P224" s="4" t="s">
-        <v>1023</v>
+        <v>442</v>
       </c>
     </row>
     <row r="225" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A225" s="4" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>1608</v>
+        <v>1609</v>
       </c>
       <c r="D225" s="4" t="s">
-        <v>1907</v>
+        <v>1873</v>
       </c>
       <c r="E225" s="4" t="s">
-        <v>2207</v>
+        <v>2208</v>
       </c>
       <c r="F225" s="4" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G225" s="4" t="s">
-        <v>1908</v>
+        <v>1889</v>
       </c>
       <c r="H225" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I225" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J225" s="4" t="s">
-        <v>1912</v>
+        <v>1913</v>
       </c>
       <c r="K225" s="4" t="s">
-        <v>2224</v>
+        <v>2225</v>
       </c>
       <c r="L225" s="4" t="s">
-        <v>191</v>
+        <v>101</v>
       </c>
       <c r="M225" s="4" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="N225" s="4" t="s">
-        <v>226</v>
+        <v>101</v>
       </c>
       <c r="O225" s="4" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="P225" s="4" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
     </row>
     <row r="226" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A226" s="4" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>444</v>
+        <v>50</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>1663</v>
+        <v>1607</v>
       </c>
       <c r="D226" s="4" t="s">
-        <v>2104</v>
+        <v>1872</v>
       </c>
       <c r="E226" s="4" t="s">
-        <v>2379</v>
+        <v>2206</v>
       </c>
       <c r="F226" s="4" t="s">
-        <v>638</v>
+        <v>309</v>
       </c>
       <c r="G226" s="4" t="s">
-        <v>2107</v>
+        <v>1888</v>
       </c>
       <c r="H226" s="4" t="s">
-        <v>641</v>
+        <v>99</v>
       </c>
       <c r="I226" s="4" t="s">
-        <v>660</v>
+        <v>139</v>
       </c>
       <c r="J226" s="4" t="s">
-        <v>2110</v>
+        <v>1911</v>
       </c>
       <c r="K226" s="4" t="s">
-        <v>2382</v>
+        <v>2223</v>
       </c>
       <c r="L226" s="4" t="s">
-        <v>674</v>
+        <v>190</v>
       </c>
       <c r="M226" s="4" t="s">
-        <v>941</v>
+        <v>908</v>
       </c>
       <c r="N226" s="4" t="s">
-        <v>645</v>
+        <v>225</v>
       </c>
       <c r="O226" s="4" t="s">
-        <v>689</v>
+        <v>268</v>
       </c>
       <c r="P226" s="4" t="s">
-        <v>1024</v>
+        <v>997</v>
       </c>
     </row>
     <row r="227" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A227" s="4" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>53</v>
+        <v>443</v>
       </c>
       <c r="C227" s="4" t="s">
-        <v>1611</v>
+        <v>1662</v>
       </c>
       <c r="D227" s="4" t="s">
-        <v>1875</v>
+        <v>2103</v>
       </c>
       <c r="E227" s="4" t="s">
-        <v>2210</v>
+        <v>2209</v>
       </c>
       <c r="F227" s="4" t="s">
-        <v>313</v>
+        <v>637</v>
       </c>
       <c r="G227" s="4" t="s">
-        <v>1887</v>
+        <v>2106</v>
       </c>
       <c r="H227" s="4" t="s">
-        <v>102</v>
+        <v>640</v>
       </c>
       <c r="I227" s="4" t="s">
-        <v>143</v>
+        <v>659</v>
       </c>
       <c r="J227" s="4" t="s">
-        <v>1915</v>
+        <v>2109</v>
       </c>
       <c r="K227" s="4" t="s">
-        <v>2227</v>
+        <v>2226</v>
       </c>
       <c r="L227" s="4" t="s">
-        <v>192</v>
+        <v>673</v>
       </c>
       <c r="M227" s="4" t="s">
-        <v>911</v>
+        <v>940</v>
       </c>
       <c r="N227" s="4" t="s">
-        <v>227</v>
+        <v>644</v>
       </c>
       <c r="O227" s="4" t="s">
-        <v>271</v>
+        <v>610</v>
       </c>
       <c r="P227" s="4" t="s">
-        <v>1000</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="228" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A228" s="4" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C228" s="4" t="s">
-        <v>1612</v>
+        <v>1608</v>
       </c>
       <c r="D228" s="4" t="s">
-        <v>1876</v>
+        <v>1907</v>
       </c>
       <c r="E228" s="4" t="s">
-        <v>2211</v>
+        <v>2207</v>
       </c>
       <c r="F228" s="4" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="G228" s="4" t="s">
-        <v>1891</v>
+        <v>1908</v>
       </c>
       <c r="H228" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I228" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="J228" s="4" t="s">
-        <v>1916</v>
+        <v>1912</v>
       </c>
       <c r="K228" s="4" t="s">
-        <v>2228</v>
+        <v>2224</v>
       </c>
       <c r="L228" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="M228" s="4" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="N228" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="O228" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="P228" s="4" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
     </row>
     <row r="229" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A229" s="4" t="s">
-        <v>703</v>
+        <v>450</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>55</v>
+        <v>444</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>1613</v>
+        <v>1663</v>
       </c>
       <c r="D229" s="4" t="s">
-        <v>1877</v>
+        <v>2104</v>
       </c>
       <c r="E229" s="4" t="s">
-        <v>2212</v>
+        <v>2379</v>
       </c>
       <c r="F229" s="4" t="s">
-        <v>315</v>
+        <v>638</v>
       </c>
       <c r="G229" s="4" t="s">
-        <v>1892</v>
+        <v>2107</v>
       </c>
       <c r="H229" s="4" t="s">
-        <v>104</v>
+        <v>641</v>
       </c>
       <c r="I229" s="4" t="s">
-        <v>145</v>
+        <v>660</v>
       </c>
       <c r="J229" s="4" t="s">
-        <v>1917</v>
+        <v>2110</v>
       </c>
       <c r="K229" s="4" t="s">
-        <v>2229</v>
+        <v>2382</v>
       </c>
       <c r="L229" s="4" t="s">
-        <v>194</v>
+        <v>674</v>
       </c>
       <c r="M229" s="4" t="s">
-        <v>913</v>
+        <v>941</v>
       </c>
       <c r="N229" s="4" t="s">
-        <v>229</v>
+        <v>645</v>
       </c>
       <c r="O229" s="4" t="s">
-        <v>273</v>
+        <v>689</v>
       </c>
       <c r="P229" s="4" t="s">
-        <v>1002</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="230" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A230" s="4" t="s">
-        <v>2531</v>
+        <v>451</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>2533</v>
+        <v>53</v>
       </c>
       <c r="C230" s="4" t="s">
-        <v>2538</v>
+        <v>1611</v>
       </c>
       <c r="D230" s="4" t="s">
-        <v>2534</v>
+        <v>1875</v>
       </c>
       <c r="E230" s="4" t="s">
-        <v>2539</v>
+        <v>2210</v>
       </c>
       <c r="F230" s="4" t="s">
-        <v>2540</v>
+        <v>313</v>
       </c>
       <c r="G230" s="4" t="s">
-        <v>2537</v>
+        <v>1887</v>
       </c>
       <c r="H230" s="4" t="s">
-        <v>2535</v>
+        <v>102</v>
       </c>
       <c r="I230" s="4" t="s">
-        <v>2536</v>
+        <v>143</v>
       </c>
       <c r="J230" s="4" t="s">
-        <v>2541</v>
+        <v>1915</v>
       </c>
       <c r="K230" s="4" t="s">
-        <v>2542</v>
+        <v>2227</v>
       </c>
       <c r="L230" s="4" t="s">
-        <v>2543</v>
+        <v>192</v>
       </c>
       <c r="M230" s="4" t="s">
-        <v>2544</v>
+        <v>911</v>
       </c>
       <c r="N230" s="4" t="s">
-        <v>2545</v>
+        <v>227</v>
       </c>
       <c r="O230" s="4" t="s">
-        <v>2546</v>
+        <v>271</v>
       </c>
       <c r="P230" s="4" t="s">
-        <v>2547</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="231" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A231" s="4" t="s">
-        <v>2551</v>
+        <v>452</v>
       </c>
       <c r="B231" s="4" t="s">
-        <v>2549</v>
+        <v>54</v>
       </c>
       <c r="C231" s="4" t="s">
-        <v>2554</v>
+        <v>1612</v>
       </c>
       <c r="D231" s="4" t="s">
-        <v>2555</v>
+        <v>1876</v>
       </c>
       <c r="E231" s="4" t="s">
-        <v>2556</v>
+        <v>2211</v>
       </c>
       <c r="F231" s="4" t="s">
-        <v>2557</v>
+        <v>314</v>
       </c>
       <c r="G231" s="4" t="s">
-        <v>2558</v>
+        <v>1891</v>
       </c>
       <c r="H231" s="4" t="s">
-        <v>2559</v>
+        <v>103</v>
       </c>
       <c r="I231" s="4" t="s">
-        <v>2560</v>
+        <v>144</v>
       </c>
       <c r="J231" s="4" t="s">
-        <v>2561</v>
+        <v>1916</v>
       </c>
       <c r="K231" s="4" t="s">
-        <v>2562</v>
+        <v>2228</v>
       </c>
       <c r="L231" s="4" t="s">
-        <v>2563</v>
+        <v>193</v>
       </c>
       <c r="M231" s="4" t="s">
-        <v>2564</v>
+        <v>912</v>
       </c>
       <c r="N231" s="4" t="s">
-        <v>2565</v>
+        <v>228</v>
       </c>
       <c r="O231" s="4" t="s">
-        <v>2553</v>
+        <v>272</v>
       </c>
       <c r="P231" s="4" t="s">
-        <v>2552</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="232" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A232" s="4" t="s">
-        <v>1310</v>
+        <v>703</v>
       </c>
       <c r="B232" s="4" t="s">
-        <v>1157</v>
+        <v>55</v>
       </c>
       <c r="C232" s="4" t="s">
-        <v>1664</v>
+        <v>1613</v>
       </c>
       <c r="D232" s="4" t="s">
-        <v>2015</v>
+        <v>1877</v>
       </c>
       <c r="E232" s="4" t="s">
-        <v>2380</v>
+        <v>2212</v>
       </c>
       <c r="F232" s="4" t="s">
-        <v>1286</v>
+        <v>315</v>
       </c>
       <c r="G232" s="4" t="s">
-        <v>2030</v>
+        <v>1892</v>
       </c>
       <c r="H232" s="4" t="s">
-        <v>1287</v>
+        <v>104</v>
       </c>
       <c r="I232" s="4" t="s">
-        <v>1288</v>
+        <v>145</v>
       </c>
       <c r="J232" s="4" t="s">
-        <v>2046</v>
+        <v>1917</v>
       </c>
       <c r="K232" s="4" t="s">
-        <v>2383</v>
+        <v>2229</v>
       </c>
       <c r="L232" s="4" t="s">
-        <v>1289</v>
+        <v>194</v>
       </c>
       <c r="M232" s="4" t="s">
-        <v>1290</v>
+        <v>913</v>
       </c>
       <c r="N232" s="4" t="s">
-        <v>1291</v>
+        <v>229</v>
       </c>
       <c r="O232" s="4" t="s">
-        <v>1292</v>
+        <v>273</v>
       </c>
       <c r="P232" s="4" t="s">
-        <v>1293</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="233" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A233" s="4" t="s">
-        <v>1336</v>
+        <v>2531</v>
       </c>
       <c r="B233" s="4" t="s">
-        <v>1335</v>
+        <v>2533</v>
       </c>
       <c r="C233" s="4" t="s">
-        <v>1665</v>
+        <v>2538</v>
       </c>
       <c r="D233" s="4" t="s">
-        <v>2105</v>
+        <v>2534</v>
       </c>
       <c r="E233" s="4" t="s">
-        <v>2381</v>
+        <v>2539</v>
       </c>
       <c r="F233" s="4" t="s">
-        <v>1378</v>
+        <v>2540</v>
       </c>
       <c r="G233" s="4" t="s">
-        <v>2108</v>
+        <v>2537</v>
       </c>
       <c r="H233" s="4" t="s">
-        <v>1403</v>
+        <v>2535</v>
       </c>
       <c r="I233" s="4" t="s">
-        <v>1404</v>
+        <v>2536</v>
       </c>
       <c r="J233" s="4" t="s">
-        <v>2111</v>
+        <v>2541</v>
       </c>
       <c r="K233" s="4" t="s">
-        <v>2384</v>
+        <v>2542</v>
       </c>
       <c r="L233" s="4" t="s">
-        <v>1405</v>
+        <v>2543</v>
       </c>
       <c r="M233" s="4" t="s">
-        <v>1406</v>
+        <v>2544</v>
       </c>
       <c r="N233" s="4" t="s">
-        <v>1407</v>
+        <v>2545</v>
       </c>
       <c r="O233" s="4" t="s">
-        <v>1408</v>
+        <v>2546</v>
       </c>
       <c r="P233" s="4" t="s">
-        <v>1409</v>
+        <v>2547</v>
       </c>
     </row>
     <row r="234" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A234" s="4" t="s">
-        <v>1149</v>
+        <v>2551</v>
       </c>
       <c r="B234" s="4" t="s">
-        <v>3416</v>
+        <v>2549</v>
       </c>
       <c r="C234" s="4" t="s">
-        <v>1660</v>
+        <v>2554</v>
       </c>
       <c r="D234" s="4" t="s">
-        <v>3422</v>
+        <v>2555</v>
       </c>
       <c r="E234" s="4" t="s">
-        <v>2364</v>
+        <v>2556</v>
       </c>
       <c r="F234" s="4" t="s">
-        <v>3420</v>
+        <v>2557</v>
       </c>
       <c r="G234" s="4" t="s">
-        <v>3422</v>
+        <v>2558</v>
       </c>
       <c r="H234" s="4" t="s">
-        <v>3414</v>
+        <v>2559</v>
       </c>
       <c r="I234" s="4" t="s">
-        <v>3415</v>
+        <v>2560</v>
       </c>
       <c r="J234" s="4" t="s">
-        <v>3421</v>
+        <v>2561</v>
       </c>
       <c r="K234" s="4" t="s">
-        <v>2378</v>
+        <v>2562</v>
       </c>
       <c r="L234" s="4" t="s">
-        <v>3416</v>
+        <v>2563</v>
       </c>
       <c r="M234" s="4" t="s">
-        <v>3419</v>
+        <v>2564</v>
       </c>
       <c r="N234" s="4" t="s">
-        <v>3416</v>
+        <v>2565</v>
       </c>
       <c r="O234" s="4" t="s">
-        <v>3418</v>
+        <v>2553</v>
       </c>
       <c r="P234" s="4" t="s">
-        <v>3417</v>
-      </c>
-    </row>
-    <row r="235" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>2552</v>
+      </c>
+    </row>
+    <row r="235" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="4" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B235" s="4" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C235" s="4" t="s">
+        <v>1664</v>
+      </c>
+      <c r="D235" s="4" t="s">
+        <v>2015</v>
+      </c>
+      <c r="E235" s="4" t="s">
+        <v>2380</v>
+      </c>
+      <c r="F235" s="4" t="s">
+        <v>1286</v>
+      </c>
+      <c r="G235" s="4" t="s">
+        <v>2030</v>
+      </c>
+      <c r="H235" s="4" t="s">
+        <v>1287</v>
+      </c>
+      <c r="I235" s="4" t="s">
+        <v>1288</v>
+      </c>
+      <c r="J235" s="4" t="s">
+        <v>2046</v>
+      </c>
+      <c r="K235" s="4" t="s">
+        <v>2383</v>
+      </c>
+      <c r="L235" s="4" t="s">
+        <v>1289</v>
+      </c>
+      <c r="M235" s="4" t="s">
+        <v>1290</v>
+      </c>
+      <c r="N235" s="4" t="s">
+        <v>1291</v>
+      </c>
+      <c r="O235" s="4" t="s">
+        <v>1292</v>
+      </c>
+      <c r="P235" s="4" t="s">
+        <v>1293</v>
+      </c>
+    </row>
     <row r="236" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A236" s="4" t="s">
-        <v>699</v>
+        <v>1336</v>
       </c>
       <c r="B236" s="4" t="s">
-        <v>442</v>
+        <v>1335</v>
       </c>
       <c r="C236" s="4" t="s">
-        <v>1661</v>
+        <v>1665</v>
       </c>
       <c r="D236" s="4" t="s">
-        <v>1847</v>
+        <v>2105</v>
       </c>
       <c r="E236" s="4" t="s">
-        <v>2189</v>
+        <v>2381</v>
       </c>
       <c r="F236" s="4" t="s">
-        <v>636</v>
+        <v>1378</v>
       </c>
       <c r="G236" s="4" t="s">
-        <v>1856</v>
+        <v>2108</v>
       </c>
       <c r="H236" s="4" t="s">
-        <v>639</v>
+        <v>1403</v>
       </c>
       <c r="I236" s="4" t="s">
-        <v>658</v>
+        <v>1404</v>
       </c>
       <c r="J236" s="4" t="s">
-        <v>2054</v>
-      </c>
-      <c r="K236" s="5" t="s">
-        <v>2198</v>
+        <v>2111</v>
+      </c>
+      <c r="K236" s="4" t="s">
+        <v>2384</v>
       </c>
       <c r="L236" s="4" t="s">
-        <v>685</v>
+        <v>1405</v>
       </c>
       <c r="M236" s="4" t="s">
-        <v>939</v>
+        <v>1406</v>
       </c>
       <c r="N236" s="4" t="s">
-        <v>643</v>
+        <v>1407</v>
       </c>
       <c r="O236" s="4" t="s">
-        <v>688</v>
+        <v>1408</v>
       </c>
       <c r="P236" s="4" t="s">
-        <v>442</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="237" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A237" s="4" t="s">
-        <v>3439</v>
+        <v>1149</v>
       </c>
       <c r="B237" s="4" t="s">
-        <v>1138</v>
+        <v>3416</v>
       </c>
       <c r="C237" s="4" t="s">
-        <v>1708</v>
+        <v>1660</v>
       </c>
       <c r="D237" s="4" t="s">
-        <v>2022</v>
+        <v>3422</v>
       </c>
       <c r="E237" s="4" t="s">
-        <v>2344</v>
+        <v>2364</v>
       </c>
       <c r="F237" s="4" t="s">
-        <v>1199</v>
+        <v>3420</v>
       </c>
       <c r="G237" s="4" t="s">
-        <v>2038</v>
+        <v>3422</v>
       </c>
       <c r="H237" s="4" t="s">
-        <v>1200</v>
+        <v>3414</v>
       </c>
       <c r="I237" s="4" t="s">
-        <v>1191</v>
+        <v>3415</v>
       </c>
       <c r="J237" s="4" t="s">
-        <v>2055</v>
+        <v>3421</v>
       </c>
       <c r="K237" s="4" t="s">
-        <v>2345</v>
+        <v>2378</v>
       </c>
       <c r="L237" s="4" t="s">
-        <v>1195</v>
+        <v>3416</v>
       </c>
       <c r="M237" s="4" t="s">
-        <v>1192</v>
+        <v>3419</v>
       </c>
       <c r="N237" s="4" t="s">
-        <v>1200</v>
+        <v>3416</v>
       </c>
       <c r="O237" s="4" t="s">
-        <v>1203</v>
+        <v>3418</v>
       </c>
       <c r="P237" s="4" t="s">
-        <v>1204</v>
-      </c>
-    </row>
-    <row r="238" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="4" t="s">
-        <v>3440</v>
-      </c>
-      <c r="B238" s="4" t="s">
-        <v>3444</v>
-      </c>
-      <c r="C238" s="4" t="s">
-        <v>3451</v>
-      </c>
-      <c r="D238" s="4" t="s">
-        <v>3452</v>
-      </c>
-      <c r="E238" s="4" t="s">
-        <v>3453</v>
-      </c>
-      <c r="F238" s="4" t="s">
-        <v>3450</v>
-      </c>
-      <c r="G238" s="4" t="s">
-        <v>3452</v>
-      </c>
-      <c r="H238" s="4" t="s">
-        <v>3449</v>
-      </c>
-      <c r="I238" s="4" t="s">
-        <v>3448</v>
-      </c>
-      <c r="J238" s="4" t="s">
-        <v>3454</v>
-      </c>
-      <c r="K238" s="4" t="s">
-        <v>3455</v>
-      </c>
-      <c r="L238" s="4" t="s">
-        <v>3446</v>
-      </c>
-      <c r="M238" s="4" t="s">
-        <v>3456</v>
-      </c>
-      <c r="N238" s="4" t="s">
-        <v>3447</v>
-      </c>
-      <c r="O238" s="4" t="s">
-        <v>3445</v>
-      </c>
-      <c r="P238" s="4" t="s">
-        <v>3443</v>
-      </c>
-    </row>
+        <v>3417</v>
+      </c>
+    </row>
+    <row r="238" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="239" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K239" s="5"/>
+      <c r="A239" s="4" t="s">
+        <v>699</v>
+      </c>
+      <c r="B239" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="C239" s="4" t="s">
+        <v>1661</v>
+      </c>
+      <c r="D239" s="4" t="s">
+        <v>1847</v>
+      </c>
+      <c r="E239" s="4" t="s">
+        <v>2189</v>
+      </c>
+      <c r="F239" s="4" t="s">
+        <v>636</v>
+      </c>
+      <c r="G239" s="4" t="s">
+        <v>1856</v>
+      </c>
+      <c r="H239" s="4" t="s">
+        <v>639</v>
+      </c>
+      <c r="I239" s="4" t="s">
+        <v>658</v>
+      </c>
+      <c r="J239" s="4" t="s">
+        <v>2054</v>
+      </c>
+      <c r="K239" s="5" t="s">
+        <v>2198</v>
+      </c>
+      <c r="L239" s="4" t="s">
+        <v>685</v>
+      </c>
+      <c r="M239" s="4" t="s">
+        <v>939</v>
+      </c>
+      <c r="N239" s="4" t="s">
+        <v>643</v>
+      </c>
+      <c r="O239" s="4" t="s">
+        <v>688</v>
+      </c>
+      <c r="P239" s="4" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="240" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A240" s="4" t="s">
-        <v>465</v>
+        <v>3439</v>
       </c>
       <c r="B240" s="4" t="s">
-        <v>51</v>
+        <v>1138</v>
       </c>
       <c r="C240" s="4" t="s">
-        <v>1608</v>
+        <v>1708</v>
       </c>
       <c r="D240" s="4" t="s">
-        <v>1907</v>
+        <v>2022</v>
       </c>
       <c r="E240" s="4" t="s">
-        <v>2207</v>
+        <v>2344</v>
       </c>
       <c r="F240" s="4" t="s">
-        <v>310</v>
+        <v>1199</v>
       </c>
       <c r="G240" s="4" t="s">
-        <v>1908</v>
+        <v>2038</v>
       </c>
       <c r="H240" s="4" t="s">
-        <v>100</v>
+        <v>1200</v>
       </c>
       <c r="I240" s="4" t="s">
-        <v>140</v>
+        <v>1191</v>
       </c>
       <c r="J240" s="4" t="s">
-        <v>1912</v>
+        <v>2055</v>
       </c>
       <c r="K240" s="4" t="s">
-        <v>2224</v>
+        <v>2345</v>
       </c>
       <c r="L240" s="4" t="s">
-        <v>191</v>
+        <v>1195</v>
       </c>
       <c r="M240" s="4" t="s">
-        <v>909</v>
+        <v>1192</v>
       </c>
       <c r="N240" s="4" t="s">
-        <v>226</v>
+        <v>1200</v>
       </c>
       <c r="O240" s="4" t="s">
-        <v>269</v>
+        <v>1203</v>
       </c>
       <c r="P240" s="4" t="s">
-        <v>1035</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="241" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A241" s="4" t="s">
-        <v>466</v>
+        <v>3440</v>
       </c>
       <c r="B241" s="4" t="s">
-        <v>54</v>
+        <v>3444</v>
       </c>
       <c r="C241" s="4" t="s">
-        <v>1612</v>
+        <v>3451</v>
       </c>
       <c r="D241" s="4" t="s">
-        <v>1876</v>
+        <v>3452</v>
       </c>
       <c r="E241" s="4" t="s">
-        <v>2211</v>
+        <v>3453</v>
       </c>
       <c r="F241" s="4" t="s">
-        <v>314</v>
+        <v>3450</v>
       </c>
       <c r="G241" s="4" t="s">
-        <v>1891</v>
+        <v>3452</v>
       </c>
       <c r="H241" s="4" t="s">
-        <v>103</v>
+        <v>3449</v>
       </c>
       <c r="I241" s="4" t="s">
-        <v>144</v>
+        <v>3448</v>
       </c>
       <c r="J241" s="4" t="s">
-        <v>1916</v>
+        <v>3454</v>
       </c>
       <c r="K241" s="4" t="s">
-        <v>2228</v>
+        <v>3455</v>
       </c>
       <c r="L241" s="4" t="s">
-        <v>193</v>
+        <v>3446</v>
       </c>
       <c r="M241" s="4" t="s">
-        <v>912</v>
+        <v>3456</v>
       </c>
       <c r="N241" s="4" t="s">
-        <v>228</v>
+        <v>3447</v>
       </c>
       <c r="O241" s="4" t="s">
-        <v>272</v>
+        <v>3445</v>
       </c>
       <c r="P241" s="4" t="s">
-        <v>1001</v>
+        <v>3443</v>
       </c>
     </row>
     <row r="242" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A242" s="4" t="s">
-        <v>467</v>
-      </c>
-      <c r="B242" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C242" s="4" t="s">
-        <v>1611</v>
-      </c>
-      <c r="D242" s="4" t="s">
-        <v>1875</v>
-      </c>
-      <c r="E242" s="4" t="s">
-        <v>2210</v>
-      </c>
-      <c r="F242" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="G242" s="4" t="s">
-        <v>1887</v>
-      </c>
-      <c r="H242" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="I242" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="J242" s="4" t="s">
-        <v>1915</v>
-      </c>
-      <c r="K242" s="4" t="s">
-        <v>2227</v>
-      </c>
-      <c r="L242" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="M242" s="4" t="s">
-        <v>911</v>
-      </c>
-      <c r="N242" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="O242" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="P242" s="4" t="s">
-        <v>1000</v>
-      </c>
+      <c r="K242" s="5"/>
     </row>
     <row r="243" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A243" s="4" t="s">
-        <v>482</v>
+        <v>465</v>
       </c>
       <c r="B243" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C243" s="4" t="s">
-        <v>1613</v>
+        <v>1608</v>
       </c>
       <c r="D243" s="4" t="s">
-        <v>1877</v>
+        <v>1907</v>
       </c>
       <c r="E243" s="4" t="s">
-        <v>2212</v>
+        <v>2207</v>
       </c>
       <c r="F243" s="4" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="G243" s="4" t="s">
-        <v>1892</v>
+        <v>1908</v>
       </c>
       <c r="H243" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I243" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="J243" s="4" t="s">
-        <v>1917</v>
+        <v>1912</v>
       </c>
       <c r="K243" s="4" t="s">
-        <v>2229</v>
+        <v>2224</v>
       </c>
       <c r="L243" s="4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="M243" s="4" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="N243" s="4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="O243" s="4" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="P243" s="4" t="s">
-        <v>1002</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="244" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A244" s="4" t="s">
-        <v>2532</v>
+        <v>466</v>
       </c>
       <c r="B244" s="4" t="s">
-        <v>2533</v>
+        <v>54</v>
       </c>
       <c r="C244" s="4" t="s">
-        <v>2538</v>
+        <v>1612</v>
       </c>
       <c r="D244" s="4" t="s">
-        <v>2534</v>
+        <v>1876</v>
       </c>
       <c r="E244" s="4" t="s">
-        <v>2539</v>
+        <v>2211</v>
       </c>
       <c r="F244" s="4" t="s">
-        <v>2540</v>
+        <v>314</v>
       </c>
       <c r="G244" s="4" t="s">
-        <v>2537</v>
+        <v>1891</v>
       </c>
       <c r="H244" s="4" t="s">
-        <v>2535</v>
+        <v>103</v>
       </c>
       <c r="I244" s="4" t="s">
-        <v>2536</v>
+        <v>144</v>
       </c>
       <c r="J244" s="4" t="s">
-        <v>2541</v>
+        <v>1916</v>
       </c>
       <c r="K244" s="4" t="s">
-        <v>2542</v>
+        <v>2228</v>
       </c>
       <c r="L244" s="4" t="s">
-        <v>2543</v>
+        <v>193</v>
       </c>
       <c r="M244" s="4" t="s">
-        <v>2544</v>
+        <v>912</v>
       </c>
       <c r="N244" s="4" t="s">
-        <v>2545</v>
+        <v>228</v>
       </c>
       <c r="O244" s="4" t="s">
-        <v>2546</v>
+        <v>272</v>
       </c>
       <c r="P244" s="4" t="s">
-        <v>2547</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="245" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A245" s="4" t="s">
-        <v>2550</v>
+        <v>467</v>
       </c>
       <c r="B245" s="4" t="s">
-        <v>2549</v>
+        <v>53</v>
       </c>
       <c r="C245" s="4" t="s">
-        <v>2554</v>
+        <v>1611</v>
       </c>
       <c r="D245" s="4" t="s">
-        <v>2555</v>
+        <v>1875</v>
       </c>
       <c r="E245" s="4" t="s">
-        <v>2556</v>
+        <v>2210</v>
       </c>
       <c r="F245" s="4" t="s">
-        <v>2557</v>
+        <v>313</v>
       </c>
       <c r="G245" s="4" t="s">
-        <v>2558</v>
+        <v>1887</v>
       </c>
       <c r="H245" s="4" t="s">
-        <v>2559</v>
+        <v>102</v>
       </c>
       <c r="I245" s="4" t="s">
-        <v>2560</v>
+        <v>143</v>
       </c>
       <c r="J245" s="4" t="s">
-        <v>2561</v>
+        <v>1915</v>
       </c>
       <c r="K245" s="4" t="s">
-        <v>2562</v>
+        <v>2227</v>
       </c>
       <c r="L245" s="4" t="s">
-        <v>2563</v>
+        <v>192</v>
       </c>
       <c r="M245" s="4" t="s">
-        <v>2564</v>
+        <v>911</v>
       </c>
       <c r="N245" s="4" t="s">
-        <v>2565</v>
+        <v>227</v>
       </c>
       <c r="O245" s="4" t="s">
-        <v>2553</v>
+        <v>271</v>
       </c>
       <c r="P245" s="4" t="s">
-        <v>2552</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="246" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A246" s="4" t="s">
-        <v>1139</v>
+        <v>482</v>
       </c>
       <c r="B246" s="4" t="s">
-        <v>1140</v>
+        <v>55</v>
       </c>
       <c r="C246" s="4" t="s">
-        <v>1666</v>
+        <v>1613</v>
       </c>
       <c r="D246" s="4" t="s">
-        <v>1850</v>
+        <v>1877</v>
       </c>
       <c r="E246" s="4" t="s">
-        <v>2192</v>
+        <v>2212</v>
       </c>
       <c r="F246" s="4" t="s">
-        <v>304</v>
+        <v>315</v>
       </c>
       <c r="G246" s="4" t="s">
-        <v>1859</v>
+        <v>1892</v>
       </c>
       <c r="H246" s="4" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="I246" s="4" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="J246" s="4" t="s">
-        <v>1843</v>
+        <v>1917</v>
       </c>
       <c r="K246" s="4" t="s">
-        <v>2385</v>
+        <v>2229</v>
       </c>
       <c r="L246" s="4" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="M246" s="4" t="s">
-        <v>903</v>
+        <v>913</v>
       </c>
       <c r="N246" s="4" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="O246" s="4" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="P246" s="4" t="s">
-        <v>992</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="247" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A247" s="4" t="s">
-        <v>468</v>
+        <v>2532</v>
       </c>
       <c r="B247" s="4" t="s">
-        <v>50</v>
+        <v>2533</v>
       </c>
       <c r="C247" s="4" t="s">
-        <v>1607</v>
+        <v>2538</v>
       </c>
       <c r="D247" s="4" t="s">
-        <v>1872</v>
+        <v>2534</v>
       </c>
       <c r="E247" s="4" t="s">
-        <v>2206</v>
+        <v>2539</v>
       </c>
       <c r="F247" s="4" t="s">
-        <v>309</v>
+        <v>2540</v>
       </c>
       <c r="G247" s="4" t="s">
-        <v>1888</v>
+        <v>2537</v>
       </c>
       <c r="H247" s="4" t="s">
-        <v>99</v>
+        <v>2535</v>
       </c>
       <c r="I247" s="4" t="s">
-        <v>139</v>
+        <v>2536</v>
       </c>
       <c r="J247" s="4" t="s">
-        <v>1911</v>
+        <v>2541</v>
       </c>
       <c r="K247" s="4" t="s">
-        <v>2223</v>
+        <v>2542</v>
       </c>
       <c r="L247" s="4" t="s">
-        <v>190</v>
+        <v>2543</v>
       </c>
       <c r="M247" s="4" t="s">
-        <v>908</v>
+        <v>2544</v>
       </c>
       <c r="N247" s="4" t="s">
-        <v>225</v>
+        <v>2545</v>
       </c>
       <c r="O247" s="4" t="s">
-        <v>268</v>
+        <v>2546</v>
       </c>
       <c r="P247" s="4" t="s">
-        <v>997</v>
+        <v>2547</v>
       </c>
     </row>
     <row r="248" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A248" s="4" t="s">
-        <v>469</v>
+        <v>2550</v>
       </c>
       <c r="B248" s="4" t="s">
-        <v>443</v>
+        <v>2549</v>
       </c>
       <c r="C248" s="4" t="s">
-        <v>1662</v>
+        <v>2554</v>
       </c>
       <c r="D248" s="4" t="s">
-        <v>2103</v>
+        <v>2555</v>
       </c>
       <c r="E248" s="4" t="s">
-        <v>2209</v>
+        <v>2556</v>
       </c>
       <c r="F248" s="4" t="s">
-        <v>637</v>
+        <v>2557</v>
       </c>
       <c r="G248" s="4" t="s">
-        <v>2106</v>
+        <v>2558</v>
       </c>
       <c r="H248" s="4" t="s">
-        <v>642</v>
+        <v>2559</v>
       </c>
       <c r="I248" s="4" t="s">
-        <v>659</v>
+        <v>2560</v>
       </c>
       <c r="J248" s="4" t="s">
-        <v>2109</v>
+        <v>2561</v>
       </c>
       <c r="K248" s="4" t="s">
-        <v>2226</v>
+        <v>2562</v>
       </c>
       <c r="L248" s="4" t="s">
-        <v>673</v>
+        <v>2563</v>
       </c>
       <c r="M248" s="4" t="s">
-        <v>942</v>
+        <v>2564</v>
       </c>
       <c r="N248" s="4" t="s">
-        <v>644</v>
+        <v>2565</v>
       </c>
       <c r="O248" s="4" t="s">
-        <v>610</v>
+        <v>2553</v>
       </c>
       <c r="P248" s="4" t="s">
-        <v>1034</v>
+        <v>2552</v>
       </c>
     </row>
     <row r="249" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A249" s="4" t="s">
-        <v>470</v>
+        <v>1139</v>
       </c>
       <c r="B249" s="4" t="s">
-        <v>453</v>
+        <v>1140</v>
       </c>
       <c r="C249" s="4" t="s">
-        <v>1686</v>
+        <v>1666</v>
       </c>
       <c r="D249" s="4" t="s">
-        <v>2148</v>
+        <v>1850</v>
       </c>
       <c r="E249" s="4" t="s">
-        <v>2468</v>
+        <v>2192</v>
       </c>
       <c r="F249" s="4" t="s">
-        <v>734</v>
+        <v>304</v>
       </c>
       <c r="G249" s="4" t="s">
-        <v>2160</v>
+        <v>1859</v>
       </c>
       <c r="H249" s="4" t="s">
-        <v>758</v>
+        <v>94</v>
       </c>
       <c r="I249" s="4" t="s">
-        <v>672</v>
+        <v>134</v>
       </c>
       <c r="J249" s="4" t="s">
-        <v>2172</v>
+        <v>1843</v>
       </c>
       <c r="K249" s="4" t="s">
-        <v>2480</v>
+        <v>2385</v>
       </c>
       <c r="L249" s="4" t="s">
-        <v>675</v>
+        <v>185</v>
       </c>
       <c r="M249" s="4" t="s">
-        <v>943</v>
+        <v>903</v>
       </c>
       <c r="N249" s="4" t="s">
-        <v>646</v>
+        <v>221</v>
       </c>
       <c r="O249" s="4" t="s">
-        <v>830</v>
+        <v>263</v>
       </c>
       <c r="P249" s="4" t="s">
-        <v>1060</v>
+        <v>992</v>
       </c>
     </row>
     <row r="250" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A250" s="4" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B250" s="4" t="s">
-        <v>454</v>
+        <v>50</v>
       </c>
       <c r="C250" s="4" t="s">
-        <v>1687</v>
+        <v>1607</v>
       </c>
       <c r="D250" s="4" t="s">
-        <v>2149</v>
+        <v>1872</v>
       </c>
       <c r="E250" s="4" t="s">
-        <v>2469</v>
+        <v>2206</v>
       </c>
       <c r="F250" s="4" t="s">
-        <v>740</v>
+        <v>309</v>
       </c>
       <c r="G250" s="4" t="s">
-        <v>2161</v>
+        <v>1888</v>
       </c>
       <c r="H250" s="4" t="s">
-        <v>759</v>
+        <v>99</v>
       </c>
       <c r="I250" s="4" t="s">
-        <v>671</v>
+        <v>139</v>
       </c>
       <c r="J250" s="4" t="s">
-        <v>2173</v>
+        <v>1911</v>
       </c>
       <c r="K250" s="4" t="s">
-        <v>2481</v>
+        <v>2223</v>
       </c>
       <c r="L250" s="4" t="s">
-        <v>686</v>
+        <v>190</v>
       </c>
       <c r="M250" s="4" t="s">
-        <v>944</v>
+        <v>908</v>
       </c>
       <c r="N250" s="4" t="s">
-        <v>650</v>
+        <v>225</v>
       </c>
       <c r="O250" s="4" t="s">
-        <v>831</v>
+        <v>268</v>
       </c>
       <c r="P250" s="4" t="s">
-        <v>1061</v>
+        <v>997</v>
       </c>
     </row>
     <row r="251" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A251" s="4" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B251" s="4" t="s">
-        <v>455</v>
+        <v>443</v>
       </c>
       <c r="C251" s="4" t="s">
-        <v>1688</v>
+        <v>1662</v>
       </c>
       <c r="D251" s="4" t="s">
-        <v>2150</v>
+        <v>2103</v>
       </c>
       <c r="E251" s="4" t="s">
-        <v>2470</v>
+        <v>2209</v>
       </c>
       <c r="F251" s="4" t="s">
-        <v>741</v>
+        <v>637</v>
       </c>
       <c r="G251" s="4" t="s">
-        <v>2162</v>
+        <v>2106</v>
       </c>
       <c r="H251" s="4" t="s">
-        <v>760</v>
+        <v>642</v>
       </c>
       <c r="I251" s="4" t="s">
-        <v>670</v>
+        <v>659</v>
       </c>
       <c r="J251" s="4" t="s">
-        <v>2174</v>
+        <v>2109</v>
       </c>
       <c r="K251" s="4" t="s">
-        <v>2482</v>
+        <v>2226</v>
       </c>
       <c r="L251" s="4" t="s">
-        <v>687</v>
+        <v>673</v>
       </c>
       <c r="M251" s="4" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="N251" s="4" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="O251" s="4" t="s">
-        <v>832</v>
+        <v>610</v>
       </c>
       <c r="P251" s="4" t="s">
-        <v>1062</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="252" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A252" s="4" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B252" s="4" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C252" s="4" t="s">
-        <v>1689</v>
+        <v>1686</v>
       </c>
       <c r="D252" s="4" t="s">
-        <v>2151</v>
+        <v>2148</v>
       </c>
       <c r="E252" s="4" t="s">
-        <v>2471</v>
+        <v>2468</v>
       </c>
       <c r="F252" s="4" t="s">
-        <v>742</v>
+        <v>734</v>
       </c>
       <c r="G252" s="4" t="s">
-        <v>2163</v>
+        <v>2160</v>
       </c>
       <c r="H252" s="4" t="s">
-        <v>769</v>
+        <v>758</v>
       </c>
       <c r="I252" s="4" t="s">
-        <v>661</v>
+        <v>672</v>
       </c>
       <c r="J252" s="4" t="s">
-        <v>2175</v>
+        <v>2172</v>
       </c>
       <c r="K252" s="4" t="s">
-        <v>2483</v>
+        <v>2480</v>
       </c>
       <c r="L252" s="4" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="M252" s="4" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="N252" s="4" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="O252" s="4" t="s">
-        <v>690</v>
+        <v>830</v>
       </c>
       <c r="P252" s="4" t="s">
-        <v>1051</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="253" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A253" s="4" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="B253" s="4" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C253" s="4" t="s">
-        <v>1690</v>
+        <v>1687</v>
       </c>
       <c r="D253" s="4" t="s">
-        <v>2152</v>
+        <v>2149</v>
       </c>
       <c r="E253" s="4" t="s">
-        <v>2472</v>
+        <v>2469</v>
       </c>
       <c r="F253" s="4" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="G253" s="4" t="s">
-        <v>2164</v>
+        <v>2161</v>
       </c>
       <c r="H253" s="4" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="I253" s="4" t="s">
-        <v>662</v>
+        <v>671</v>
       </c>
       <c r="J253" s="4" t="s">
-        <v>2176</v>
+        <v>2173</v>
       </c>
       <c r="K253" s="4" t="s">
-        <v>2484</v>
+        <v>2481</v>
       </c>
       <c r="L253" s="4" t="s">
-        <v>677</v>
+        <v>686</v>
       </c>
       <c r="M253" s="4" t="s">
-        <v>1071</v>
+        <v>944</v>
       </c>
       <c r="N253" s="4" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="O253" s="4" t="s">
-        <v>691</v>
+        <v>831</v>
       </c>
       <c r="P253" s="4" t="s">
-        <v>1052</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="254" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A254" s="4" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B254" s="4" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C254" s="4" t="s">
-        <v>1691</v>
+        <v>1688</v>
       </c>
       <c r="D254" s="4" t="s">
-        <v>2153</v>
+        <v>2150</v>
       </c>
       <c r="E254" s="4" t="s">
-        <v>2473</v>
+        <v>2470</v>
       </c>
       <c r="F254" s="4" t="s">
-        <v>735</v>
+        <v>741</v>
       </c>
       <c r="G254" s="4" t="s">
-        <v>2165</v>
+        <v>2162</v>
       </c>
       <c r="H254" s="4" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="I254" s="4" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="J254" s="4" t="s">
-        <v>2177</v>
+        <v>2174</v>
       </c>
       <c r="K254" s="4" t="s">
-        <v>2485</v>
+        <v>2482</v>
       </c>
       <c r="L254" s="4" t="s">
-        <v>678</v>
+        <v>687</v>
       </c>
       <c r="M254" s="4" t="s">
-        <v>1072</v>
+        <v>945</v>
       </c>
       <c r="N254" s="4" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="O254" s="4" t="s">
-        <v>692</v>
+        <v>832</v>
       </c>
       <c r="P254" s="4" t="s">
-        <v>1053</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="255" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A255" s="4" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B255" s="4" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C255" s="4" t="s">
-        <v>1692</v>
+        <v>1689</v>
       </c>
       <c r="D255" s="4" t="s">
-        <v>2154</v>
+        <v>2151</v>
       </c>
       <c r="E255" s="4" t="s">
-        <v>2474</v>
+        <v>2471</v>
       </c>
       <c r="F255" s="4" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="G255" s="4" t="s">
-        <v>2166</v>
+        <v>2163</v>
       </c>
       <c r="H255" s="4" t="s">
-        <v>763</v>
+        <v>769</v>
       </c>
       <c r="I255" s="4" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="J255" s="4" t="s">
-        <v>2178</v>
+        <v>2175</v>
       </c>
       <c r="K255" s="4" t="s">
-        <v>2486</v>
+        <v>2483</v>
       </c>
       <c r="L255" s="4" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="M255" s="4" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="N255" s="4" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="O255" s="4" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="P255" s="4" t="s">
-        <v>1057</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="256" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A256" s="4" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B256" s="4" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C256" s="4" t="s">
-        <v>1693</v>
+        <v>1690</v>
       </c>
       <c r="D256" s="4" t="s">
-        <v>2155</v>
+        <v>2152</v>
       </c>
       <c r="E256" s="4" t="s">
-        <v>2475</v>
+        <v>2472</v>
       </c>
       <c r="F256" s="4" t="s">
-        <v>736</v>
+        <v>743</v>
       </c>
       <c r="G256" s="4" t="s">
-        <v>2167</v>
+        <v>2164</v>
       </c>
       <c r="H256" s="4" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="I256" s="4" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="J256" s="4" t="s">
-        <v>2179</v>
+        <v>2176</v>
       </c>
       <c r="K256" s="4" t="s">
-        <v>2487</v>
+        <v>2484</v>
       </c>
       <c r="L256" s="4" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="M256" s="4" t="s">
-        <v>948</v>
+        <v>1071</v>
       </c>
       <c r="N256" s="4" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="O256" s="4" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="P256" s="4" t="s">
-        <v>1058</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="257" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A257" s="4" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B257" s="4" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C257" s="4" t="s">
-        <v>1694</v>
+        <v>1691</v>
       </c>
       <c r="D257" s="4" t="s">
-        <v>2156</v>
+        <v>2153</v>
       </c>
       <c r="E257" s="4" t="s">
-        <v>2476</v>
+        <v>2473</v>
       </c>
       <c r="F257" s="4" t="s">
-        <v>745</v>
+        <v>735</v>
       </c>
       <c r="G257" s="4" t="s">
-        <v>2168</v>
+        <v>2165</v>
       </c>
       <c r="H257" s="4" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="I257" s="4" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="J257" s="4" t="s">
-        <v>2180</v>
+        <v>2177</v>
       </c>
       <c r="K257" s="4" t="s">
-        <v>2488</v>
+        <v>2485</v>
       </c>
       <c r="L257" s="4" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="M257" s="4" t="s">
-        <v>949</v>
+        <v>1072</v>
       </c>
       <c r="N257" s="4" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="O257" s="4" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="P257" s="4" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="258" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A258" s="4" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B258" s="4" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C258" s="4" t="s">
-        <v>1695</v>
+        <v>1692</v>
       </c>
       <c r="D258" s="4" t="s">
-        <v>2157</v>
+        <v>2154</v>
       </c>
       <c r="E258" s="4" t="s">
-        <v>2477</v>
+        <v>2474</v>
       </c>
       <c r="F258" s="4" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="G258" s="4" t="s">
-        <v>2169</v>
+        <v>2166</v>
       </c>
       <c r="H258" s="4" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="I258" s="4" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="J258" s="4" t="s">
-        <v>2181</v>
+        <v>2178</v>
       </c>
       <c r="K258" s="4" t="s">
-        <v>2489</v>
+        <v>2486</v>
       </c>
       <c r="L258" s="4" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="M258" s="4" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="N258" s="4" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="O258" s="4" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="P258" s="4" t="s">
-        <v>1055</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="259" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A259" s="4" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B259" s="4" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="C259" s="4" t="s">
-        <v>1696</v>
+        <v>1693</v>
       </c>
       <c r="D259" s="4" t="s">
-        <v>2158</v>
+        <v>2155</v>
       </c>
       <c r="E259" s="4" t="s">
-        <v>2478</v>
+        <v>2475</v>
       </c>
       <c r="F259" s="4" t="s">
-        <v>747</v>
+        <v>736</v>
       </c>
       <c r="G259" s="4" t="s">
-        <v>2170</v>
+        <v>2167</v>
       </c>
       <c r="H259" s="4" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="I259" s="4" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="J259" s="4" t="s">
-        <v>2182</v>
+        <v>2179</v>
       </c>
       <c r="K259" s="4" t="s">
-        <v>2490</v>
+        <v>2487</v>
       </c>
       <c r="L259" s="4" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="M259" s="4" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="N259" s="4" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="O259" s="4" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="P259" s="4" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="260" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A260" s="4" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B260" s="4" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="C260" s="4" t="s">
-        <v>1697</v>
+        <v>1694</v>
       </c>
       <c r="D260" s="4" t="s">
-        <v>2159</v>
+        <v>2156</v>
       </c>
       <c r="E260" s="4" t="s">
-        <v>2479</v>
+        <v>2476</v>
       </c>
       <c r="F260" s="4" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="G260" s="4" t="s">
-        <v>2171</v>
+        <v>2168</v>
       </c>
       <c r="H260" s="4" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="I260" s="4" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="J260" s="4" t="s">
-        <v>2183</v>
+        <v>2180</v>
       </c>
       <c r="K260" s="4" t="s">
-        <v>2491</v>
+        <v>2488</v>
       </c>
       <c r="L260" s="4" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="M260" s="4" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="N260" s="4" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="O260" s="4" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="P260" s="4" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="261" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A261" s="4" t="s">
-        <v>710</v>
+        <v>479</v>
       </c>
       <c r="B261" s="4" t="s">
-        <v>722</v>
+        <v>462</v>
       </c>
       <c r="C261" s="4" t="s">
-        <v>1674</v>
+        <v>1695</v>
       </c>
       <c r="D261" s="4" t="s">
-        <v>2112</v>
+        <v>2157</v>
       </c>
       <c r="E261" s="4" t="s">
-        <v>2456</v>
+        <v>2477</v>
       </c>
       <c r="F261" s="4" t="s">
-        <v>737</v>
+        <v>746</v>
       </c>
       <c r="G261" s="4" t="s">
-        <v>2113</v>
+        <v>2169</v>
       </c>
       <c r="H261" s="4" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="I261" s="4" t="s">
-        <v>782</v>
+        <v>667</v>
       </c>
       <c r="J261" s="4" t="s">
-        <v>2114</v>
+        <v>2181</v>
       </c>
       <c r="K261" s="4" t="s">
-        <v>2492</v>
+        <v>2489</v>
       </c>
       <c r="L261" s="4" t="s">
-        <v>794</v>
+        <v>682</v>
       </c>
       <c r="M261" s="4" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="N261" s="4" t="s">
-        <v>806</v>
+        <v>655</v>
       </c>
       <c r="O261" s="4" t="s">
-        <v>818</v>
+        <v>696</v>
       </c>
       <c r="P261" s="4" t="s">
-        <v>1039</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="262" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A262" s="4" t="s">
-        <v>711</v>
+        <v>480</v>
       </c>
       <c r="B262" s="4" t="s">
-        <v>723</v>
+        <v>463</v>
       </c>
       <c r="C262" s="4" t="s">
-        <v>1675</v>
+        <v>1696</v>
       </c>
       <c r="D262" s="4" t="s">
-        <v>2115</v>
+        <v>2158</v>
       </c>
       <c r="E262" s="4" t="s">
-        <v>2457</v>
+        <v>2478</v>
       </c>
       <c r="F262" s="4" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="G262" s="4" t="s">
-        <v>2126</v>
+        <v>2170</v>
       </c>
       <c r="H262" s="4" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="I262" s="4" t="s">
-        <v>783</v>
+        <v>668</v>
       </c>
       <c r="J262" s="4" t="s">
-        <v>2137</v>
+        <v>2182</v>
       </c>
       <c r="K262" s="4" t="s">
-        <v>2493</v>
+        <v>2490</v>
       </c>
       <c r="L262" s="4" t="s">
-        <v>795</v>
+        <v>683</v>
       </c>
       <c r="M262" s="4" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
       <c r="N262" s="4" t="s">
-        <v>807</v>
+        <v>656</v>
       </c>
       <c r="O262" s="4" t="s">
-        <v>819</v>
+        <v>697</v>
       </c>
       <c r="P262" s="4" t="s">
-        <v>1040</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="263" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A263" s="4" t="s">
-        <v>712</v>
+        <v>481</v>
       </c>
       <c r="B263" s="4" t="s">
-        <v>724</v>
+        <v>464</v>
       </c>
       <c r="C263" s="4" t="s">
-        <v>1676</v>
+        <v>1697</v>
       </c>
       <c r="D263" s="4" t="s">
-        <v>2116</v>
+        <v>2159</v>
       </c>
       <c r="E263" s="4" t="s">
-        <v>2458</v>
+        <v>2479</v>
       </c>
       <c r="F263" s="4" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="G263" s="4" t="s">
-        <v>2127</v>
+        <v>2171</v>
       </c>
       <c r="H263" s="4" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="I263" s="4" t="s">
-        <v>784</v>
+        <v>669</v>
       </c>
       <c r="J263" s="4" t="s">
-        <v>2138</v>
+        <v>2183</v>
       </c>
       <c r="K263" s="4" t="s">
-        <v>2494</v>
+        <v>2491</v>
       </c>
       <c r="L263" s="4" t="s">
-        <v>796</v>
+        <v>684</v>
       </c>
       <c r="M263" s="4" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="N263" s="4" t="s">
-        <v>808</v>
+        <v>657</v>
       </c>
       <c r="O263" s="4" t="s">
-        <v>820</v>
+        <v>698</v>
       </c>
       <c r="P263" s="4" t="s">
-        <v>1041</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="264" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A264" s="4" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="B264" s="4" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="C264" s="4" t="s">
-        <v>1677</v>
+        <v>1674</v>
       </c>
       <c r="D264" s="4" t="s">
-        <v>2117</v>
+        <v>2112</v>
       </c>
       <c r="E264" s="4" t="s">
-        <v>2459</v>
+        <v>2456</v>
       </c>
       <c r="F264" s="4" t="s">
-        <v>751</v>
+        <v>737</v>
       </c>
       <c r="G264" s="4" t="s">
-        <v>2128</v>
+        <v>2113</v>
       </c>
       <c r="H264" s="4" t="s">
-        <v>781</v>
+        <v>770</v>
       </c>
       <c r="I264" s="4" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="J264" s="4" t="s">
-        <v>2139</v>
+        <v>2114</v>
       </c>
       <c r="K264" s="4" t="s">
-        <v>2495</v>
+        <v>2492</v>
       </c>
       <c r="L264" s="4" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="M264" s="4" t="s">
-        <v>1074</v>
+        <v>953</v>
       </c>
       <c r="N264" s="4" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="O264" s="4" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="P264" s="4" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="265" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A265" s="4" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="B265" s="4" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="C265" s="4" t="s">
-        <v>1678</v>
+        <v>1675</v>
       </c>
       <c r="D265" s="4" t="s">
-        <v>2118</v>
+        <v>2115</v>
       </c>
       <c r="E265" s="4" t="s">
-        <v>2460</v>
+        <v>2457</v>
       </c>
       <c r="F265" s="4" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="G265" s="4" t="s">
-        <v>2129</v>
+        <v>2126</v>
       </c>
       <c r="H265" s="4" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="I265" s="4" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="J265" s="4" t="s">
-        <v>2140</v>
+        <v>2137</v>
       </c>
       <c r="K265" s="4" t="s">
-        <v>2496</v>
+        <v>2493</v>
       </c>
       <c r="L265" s="4" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="M265" s="4" t="s">
-        <v>1073</v>
+        <v>954</v>
       </c>
       <c r="N265" s="4" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="O265" s="4" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="P265" s="4" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="266" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A266" s="4" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="B266" s="4" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="C266" s="4" t="s">
-        <v>1679</v>
+        <v>1676</v>
       </c>
       <c r="D266" s="4" t="s">
-        <v>2119</v>
+        <v>2116</v>
       </c>
       <c r="E266" s="4" t="s">
-        <v>2461</v>
+        <v>2458</v>
       </c>
       <c r="F266" s="4" t="s">
-        <v>738</v>
+        <v>750</v>
       </c>
       <c r="G266" s="4" t="s">
-        <v>2130</v>
+        <v>2127</v>
       </c>
       <c r="H266" s="4" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="I266" s="4" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="J266" s="4" t="s">
-        <v>2141</v>
+        <v>2138</v>
       </c>
       <c r="K266" s="4" t="s">
-        <v>2497</v>
+        <v>2494</v>
       </c>
       <c r="L266" s="4" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="M266" s="4" t="s">
-        <v>1075</v>
+        <v>955</v>
       </c>
       <c r="N266" s="4" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="O266" s="4" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="P266" s="4" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="267" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A267" s="4" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="B267" s="4" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="C267" s="4" t="s">
-        <v>1680</v>
+        <v>1677</v>
       </c>
       <c r="D267" s="4" t="s">
-        <v>2120</v>
+        <v>2117</v>
       </c>
       <c r="E267" s="4" t="s">
-        <v>2462</v>
+        <v>2459</v>
       </c>
       <c r="F267" s="4" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="G267" s="4" t="s">
-        <v>2131</v>
+        <v>2128</v>
       </c>
       <c r="H267" s="4" t="s">
-        <v>775</v>
+        <v>781</v>
       </c>
       <c r="I267" s="4" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="J267" s="4" t="s">
-        <v>2142</v>
+        <v>2139</v>
       </c>
       <c r="K267" s="4" t="s">
-        <v>2498</v>
+        <v>2495</v>
       </c>
       <c r="L267" s="4" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="M267" s="4" t="s">
-        <v>956</v>
+        <v>1074</v>
       </c>
       <c r="N267" s="4" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="O267" s="4" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="P267" s="4" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="268" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A268" s="4" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="B268" s="4" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="C268" s="4" t="s">
-        <v>1681</v>
+        <v>1678</v>
       </c>
       <c r="D268" s="4" t="s">
-        <v>2121</v>
+        <v>2118</v>
       </c>
       <c r="E268" s="4" t="s">
-        <v>2463</v>
+        <v>2460</v>
       </c>
       <c r="F268" s="4" t="s">
-        <v>739</v>
+        <v>752</v>
       </c>
       <c r="G268" s="4" t="s">
-        <v>2132</v>
+        <v>2129</v>
       </c>
       <c r="H268" s="4" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="I268" s="4" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="J268" s="4" t="s">
-        <v>2143</v>
+        <v>2140</v>
       </c>
       <c r="K268" s="4" t="s">
-        <v>2499</v>
+        <v>2496</v>
       </c>
       <c r="L268" s="4" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="M268" s="4" t="s">
-        <v>957</v>
+        <v>1073</v>
       </c>
       <c r="N268" s="4" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="O268" s="4" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="P268" s="4" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="269" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A269" s="4" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="B269" s="4" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="C269" s="4" t="s">
-        <v>1682</v>
+        <v>1679</v>
       </c>
       <c r="D269" s="4" t="s">
-        <v>2122</v>
+        <v>2119</v>
       </c>
       <c r="E269" s="4" t="s">
-        <v>2464</v>
+        <v>2461</v>
       </c>
       <c r="F269" s="4" t="s">
-        <v>754</v>
+        <v>738</v>
       </c>
       <c r="G269" s="4" t="s">
-        <v>2133</v>
+        <v>2130</v>
       </c>
       <c r="H269" s="4" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="I269" s="4" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="J269" s="4" t="s">
-        <v>2144</v>
+        <v>2141</v>
       </c>
       <c r="K269" s="4" t="s">
-        <v>2500</v>
+        <v>2497</v>
       </c>
       <c r="L269" s="4" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="M269" s="4" t="s">
-        <v>958</v>
+        <v>1075</v>
       </c>
       <c r="N269" s="4" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="O269" s="4" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="P269" s="4" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="270" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A270" s="4" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="B270" s="4" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="C270" s="4" t="s">
-        <v>1683</v>
+        <v>1680</v>
       </c>
       <c r="D270" s="4" t="s">
-        <v>2123</v>
+        <v>2120</v>
       </c>
       <c r="E270" s="4" t="s">
-        <v>2465</v>
+        <v>2462</v>
       </c>
       <c r="F270" s="4" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="G270" s="4" t="s">
-        <v>2134</v>
+        <v>2131</v>
       </c>
       <c r="H270" s="4" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="I270" s="4" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="J270" s="4" t="s">
-        <v>2145</v>
+        <v>2142</v>
       </c>
       <c r="K270" s="4" t="s">
-        <v>2501</v>
+        <v>2498</v>
       </c>
       <c r="L270" s="4" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="M270" s="4" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
       <c r="N270" s="4" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="O270" s="4" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="P270" s="4" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="271" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A271" s="4" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="B271" s="4" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="C271" s="4" t="s">
-        <v>1684</v>
+        <v>1681</v>
       </c>
       <c r="D271" s="4" t="s">
-        <v>2124</v>
+        <v>2121</v>
       </c>
       <c r="E271" s="4" t="s">
-        <v>2466</v>
+        <v>2463</v>
       </c>
       <c r="F271" s="4" t="s">
-        <v>756</v>
+        <v>739</v>
       </c>
       <c r="G271" s="4" t="s">
-        <v>2135</v>
+        <v>2132</v>
       </c>
       <c r="H271" s="4" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="I271" s="4" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="J271" s="4" t="s">
-        <v>2146</v>
+        <v>2143</v>
       </c>
       <c r="K271" s="4" t="s">
-        <v>2502</v>
+        <v>2499</v>
       </c>
       <c r="L271" s="4" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="M271" s="4" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="N271" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="O271" s="4" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="P271" s="4" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="272" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A272" s="4" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="B272" s="4" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="C272" s="4" t="s">
-        <v>1685</v>
+        <v>1682</v>
       </c>
       <c r="D272" s="4" t="s">
-        <v>2125</v>
+        <v>2122</v>
       </c>
       <c r="E272" s="4" t="s">
-        <v>2467</v>
+        <v>2464</v>
       </c>
       <c r="F272" s="4" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="G272" s="4" t="s">
-        <v>2136</v>
+        <v>2133</v>
       </c>
       <c r="H272" s="4" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="I272" s="4" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="J272" s="4" t="s">
-        <v>2147</v>
+        <v>2144</v>
       </c>
       <c r="K272" s="4" t="s">
-        <v>2503</v>
+        <v>2500</v>
       </c>
       <c r="L272" s="4" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="M272" s="4" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="N272" s="4" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="O272" s="4" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="P272" s="4" t="s">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="273" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="273" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A273" s="4" t="s">
+        <v>719</v>
+      </c>
+      <c r="B273" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="C273" s="4" t="s">
+        <v>1683</v>
+      </c>
+      <c r="D273" s="4" t="s">
+        <v>2123</v>
+      </c>
+      <c r="E273" s="4" t="s">
+        <v>2465</v>
+      </c>
+      <c r="F273" s="4" t="s">
+        <v>755</v>
+      </c>
+      <c r="G273" s="4" t="s">
+        <v>2134</v>
+      </c>
+      <c r="H273" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="I273" s="4" t="s">
+        <v>791</v>
+      </c>
+      <c r="J273" s="4" t="s">
+        <v>2145</v>
+      </c>
+      <c r="K273" s="4" t="s">
+        <v>2501</v>
+      </c>
+      <c r="L273" s="4" t="s">
+        <v>803</v>
+      </c>
+      <c r="M273" s="4" t="s">
+        <v>959</v>
+      </c>
+      <c r="N273" s="4" t="s">
+        <v>815</v>
+      </c>
+      <c r="O273" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="P273" s="4" t="s">
+        <v>1048</v>
+      </c>
+    </row>
     <row r="274" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A274" s="4" t="s">
-        <v>1098</v>
+        <v>720</v>
       </c>
       <c r="B274" s="4" t="s">
-        <v>1102</v>
+        <v>732</v>
       </c>
       <c r="C274" s="4" t="s">
-        <v>1667</v>
+        <v>1684</v>
       </c>
       <c r="D274" s="4" t="s">
-        <v>1945</v>
+        <v>2124</v>
       </c>
       <c r="E274" s="4" t="s">
-        <v>2386</v>
+        <v>2466</v>
       </c>
       <c r="F274" s="4" t="s">
-        <v>1223</v>
+        <v>756</v>
       </c>
       <c r="G274" s="4" t="s">
-        <v>1949</v>
+        <v>2135</v>
       </c>
       <c r="H274" s="4" t="s">
-        <v>1222</v>
+        <v>779</v>
       </c>
       <c r="I274" s="4" t="s">
-        <v>1102</v>
+        <v>792</v>
       </c>
       <c r="J274" s="4" t="s">
-        <v>1953</v>
+        <v>2146</v>
       </c>
       <c r="K274" s="4" t="s">
-        <v>2390</v>
+        <v>2502</v>
       </c>
       <c r="L274" s="4" t="s">
-        <v>1240</v>
+        <v>804</v>
       </c>
       <c r="M274" s="4" t="s">
-        <v>1239</v>
+        <v>960</v>
       </c>
       <c r="N274" s="4" t="s">
-        <v>1222</v>
+        <v>816</v>
       </c>
       <c r="O274" s="4" t="s">
-        <v>1241</v>
+        <v>828</v>
       </c>
       <c r="P274" s="4" t="s">
-        <v>1242</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="275" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A275" s="4" t="s">
-        <v>1099</v>
+        <v>721</v>
       </c>
       <c r="B275" s="4" t="s">
-        <v>1103</v>
+        <v>733</v>
       </c>
       <c r="C275" s="4" t="s">
-        <v>1668</v>
+        <v>1685</v>
       </c>
       <c r="D275" s="4" t="s">
-        <v>1946</v>
+        <v>2125</v>
       </c>
       <c r="E275" s="4" t="s">
-        <v>2387</v>
+        <v>2467</v>
       </c>
       <c r="F275" s="4" t="s">
-        <v>1225</v>
+        <v>757</v>
       </c>
       <c r="G275" s="4" t="s">
-        <v>1950</v>
+        <v>2136</v>
       </c>
       <c r="H275" s="4" t="s">
-        <v>1226</v>
+        <v>780</v>
       </c>
       <c r="I275" s="4" t="s">
-        <v>1224</v>
+        <v>793</v>
       </c>
       <c r="J275" s="4" t="s">
-        <v>1954</v>
+        <v>2147</v>
       </c>
       <c r="K275" s="4" t="s">
-        <v>2391</v>
+        <v>2503</v>
       </c>
       <c r="L275" s="4" t="s">
-        <v>1236</v>
+        <v>805</v>
       </c>
       <c r="M275" s="4" t="s">
-        <v>1237</v>
+        <v>961</v>
       </c>
       <c r="N275" s="4" t="s">
-        <v>1238</v>
+        <v>817</v>
       </c>
       <c r="O275" s="4" t="s">
-        <v>1248</v>
+        <v>829</v>
       </c>
       <c r="P275" s="4" t="s">
-        <v>1247</v>
-      </c>
-    </row>
-    <row r="276" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A276" s="4" t="s">
-        <v>1100</v>
-      </c>
-      <c r="B276" s="4" t="s">
-        <v>1104</v>
-      </c>
-      <c r="C276" s="4" t="s">
-        <v>1669</v>
-      </c>
-      <c r="D276" s="4" t="s">
-        <v>1947</v>
-      </c>
-      <c r="E276" s="4" t="s">
-        <v>2388</v>
-      </c>
-      <c r="F276" s="4" t="s">
-        <v>1228</v>
-      </c>
-      <c r="G276" s="4" t="s">
-        <v>1951</v>
-      </c>
-      <c r="H276" s="4" t="s">
-        <v>1227</v>
-      </c>
-      <c r="I276" s="4" t="s">
-        <v>1229</v>
-      </c>
-      <c r="J276" s="4" t="s">
-        <v>1955</v>
-      </c>
-      <c r="K276" s="4" t="s">
-        <v>2392</v>
-      </c>
-      <c r="L276" s="4" t="s">
-        <v>1234</v>
-      </c>
-      <c r="M276" s="4" t="s">
-        <v>1235</v>
-      </c>
-      <c r="N276" s="4" t="s">
-        <v>1227</v>
-      </c>
-      <c r="O276" s="4" t="s">
-        <v>1245</v>
-      </c>
-      <c r="P276" s="4" t="s">
-        <v>1246</v>
-      </c>
-    </row>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="276" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="277" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A277" s="4" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="B277" s="4" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
       <c r="C277" s="4" t="s">
-        <v>1670</v>
+        <v>1667</v>
       </c>
       <c r="D277" s="4" t="s">
-        <v>1948</v>
+        <v>1945</v>
       </c>
       <c r="E277" s="4" t="s">
-        <v>2389</v>
+        <v>2386</v>
       </c>
       <c r="F277" s="4" t="s">
-        <v>1232</v>
+        <v>1223</v>
       </c>
       <c r="G277" s="4" t="s">
-        <v>1952</v>
+        <v>1949</v>
       </c>
       <c r="H277" s="4" t="s">
-        <v>1231</v>
+        <v>1222</v>
       </c>
       <c r="I277" s="4" t="s">
-        <v>1230</v>
+        <v>1102</v>
       </c>
       <c r="J277" s="4" t="s">
-        <v>1956</v>
+        <v>1953</v>
       </c>
       <c r="K277" s="4" t="s">
-        <v>2393</v>
+        <v>2390</v>
       </c>
       <c r="L277" s="4" t="s">
-        <v>1231</v>
+        <v>1240</v>
       </c>
       <c r="M277" s="4" t="s">
-        <v>1233</v>
+        <v>1239</v>
       </c>
       <c r="N277" s="4" t="s">
-        <v>1231</v>
+        <v>1222</v>
       </c>
       <c r="O277" s="4" t="s">
-        <v>1244</v>
+        <v>1241</v>
       </c>
       <c r="P277" s="4" t="s">
-        <v>1243</v>
-      </c>
-    </row>
-    <row r="278" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="278" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A278" s="4" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B278" s="4" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C278" s="4" t="s">
+        <v>1668</v>
+      </c>
+      <c r="D278" s="4" t="s">
+        <v>1946</v>
+      </c>
+      <c r="E278" s="4" t="s">
+        <v>2387</v>
+      </c>
+      <c r="F278" s="4" t="s">
+        <v>1225</v>
+      </c>
+      <c r="G278" s="4" t="s">
+        <v>1950</v>
+      </c>
+      <c r="H278" s="4" t="s">
+        <v>1226</v>
+      </c>
+      <c r="I278" s="4" t="s">
+        <v>1224</v>
+      </c>
+      <c r="J278" s="4" t="s">
+        <v>1954</v>
+      </c>
+      <c r="K278" s="4" t="s">
+        <v>2391</v>
+      </c>
+      <c r="L278" s="4" t="s">
+        <v>1236</v>
+      </c>
+      <c r="M278" s="4" t="s">
+        <v>1237</v>
+      </c>
+      <c r="N278" s="4" t="s">
+        <v>1238</v>
+      </c>
+      <c r="O278" s="4" t="s">
+        <v>1248</v>
+      </c>
+      <c r="P278" s="4" t="s">
+        <v>1247</v>
+      </c>
+    </row>
     <row r="279" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A279" s="4" t="s">
-        <v>2615</v>
+        <v>1100</v>
       </c>
       <c r="B279" s="4" t="s">
-        <v>2616</v>
+        <v>1104</v>
       </c>
       <c r="C279" s="4" t="s">
-        <v>2623</v>
+        <v>1669</v>
       </c>
       <c r="D279" s="4" t="s">
-        <v>2622</v>
+        <v>1947</v>
       </c>
       <c r="E279" s="4" t="s">
-        <v>2621</v>
+        <v>2388</v>
       </c>
       <c r="F279" s="4" t="s">
-        <v>2620</v>
+        <v>1228</v>
       </c>
       <c r="G279" s="4" t="s">
-        <v>2619</v>
+        <v>1951</v>
       </c>
       <c r="H279" s="4" t="s">
-        <v>2618</v>
+        <v>1227</v>
       </c>
       <c r="I279" s="4" t="s">
-        <v>2617</v>
+        <v>1229</v>
       </c>
       <c r="J279" s="4" t="s">
-        <v>2624</v>
+        <v>1955</v>
       </c>
       <c r="K279" s="4" t="s">
-        <v>2625</v>
+        <v>2392</v>
       </c>
       <c r="L279" s="4" t="s">
-        <v>2626</v>
+        <v>1234</v>
       </c>
       <c r="M279" s="4" t="s">
-        <v>2627</v>
+        <v>1235</v>
       </c>
       <c r="N279" s="4" t="s">
-        <v>2628</v>
+        <v>1227</v>
       </c>
       <c r="O279" s="4" t="s">
-        <v>2629</v>
+        <v>1245</v>
       </c>
       <c r="P279" s="4" t="s">
-        <v>2630</v>
-      </c>
-    </row>
-    <row r="280" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="281" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A281" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B281" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C281" s="4" t="s">
-        <v>1595</v>
-      </c>
-      <c r="D281" s="4" t="s">
-        <v>1821</v>
-      </c>
-      <c r="E281" s="4" t="s">
-        <v>2394</v>
-      </c>
-      <c r="F281" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="G281" s="4" t="s">
-        <v>1830</v>
-      </c>
-      <c r="H281" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="I281" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="J281" s="4" t="s">
-        <v>1937</v>
-      </c>
-      <c r="K281" s="4" t="s">
-        <v>2396</v>
-      </c>
-      <c r="L281" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="M281" s="4" t="s">
-        <v>897</v>
-      </c>
-      <c r="N281" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="O281" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="P281" s="4" t="s">
-        <v>988</v>
-      </c>
-    </row>
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="280" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A280" s="4" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B280" s="4" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C280" s="4" t="s">
+        <v>1670</v>
+      </c>
+      <c r="D280" s="4" t="s">
+        <v>1948</v>
+      </c>
+      <c r="E280" s="4" t="s">
+        <v>2389</v>
+      </c>
+      <c r="F280" s="4" t="s">
+        <v>1232</v>
+      </c>
+      <c r="G280" s="4" t="s">
+        <v>1952</v>
+      </c>
+      <c r="H280" s="4" t="s">
+        <v>1231</v>
+      </c>
+      <c r="I280" s="4" t="s">
+        <v>1230</v>
+      </c>
+      <c r="J280" s="4" t="s">
+        <v>1956</v>
+      </c>
+      <c r="K280" s="4" t="s">
+        <v>2393</v>
+      </c>
+      <c r="L280" s="4" t="s">
+        <v>1231</v>
+      </c>
+      <c r="M280" s="4" t="s">
+        <v>1233</v>
+      </c>
+      <c r="N280" s="4" t="s">
+        <v>1231</v>
+      </c>
+      <c r="O280" s="4" t="s">
+        <v>1244</v>
+      </c>
+      <c r="P280" s="4" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="281" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="282" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A282" s="4" t="s">
-        <v>38</v>
+        <v>2615</v>
       </c>
       <c r="B282" s="4" t="s">
-        <v>81</v>
+        <v>2616</v>
       </c>
       <c r="C282" s="4" t="s">
-        <v>1672</v>
+        <v>2623</v>
       </c>
       <c r="D282" s="4" t="s">
-        <v>1935</v>
+        <v>2622</v>
       </c>
       <c r="E282" s="4" t="s">
-        <v>2395</v>
+        <v>2621</v>
       </c>
       <c r="F282" s="4" t="s">
-        <v>81</v>
+        <v>2620</v>
       </c>
       <c r="G282" s="4" t="s">
-        <v>1936</v>
+        <v>2619</v>
       </c>
       <c r="H282" s="4" t="s">
-        <v>118</v>
+        <v>2618</v>
       </c>
       <c r="I282" s="4" t="s">
-        <v>81</v>
+        <v>2617</v>
       </c>
       <c r="J282" s="4" t="s">
-        <v>1938</v>
+        <v>2624</v>
       </c>
       <c r="K282" s="4" t="s">
-        <v>2397</v>
+        <v>2625</v>
       </c>
       <c r="L282" s="4" t="s">
-        <v>209</v>
+        <v>2626</v>
       </c>
       <c r="M282" s="4" t="s">
-        <v>962</v>
+        <v>2627</v>
       </c>
       <c r="N282" s="4" t="s">
-        <v>246</v>
+        <v>2628</v>
       </c>
       <c r="O282" s="4" t="s">
-        <v>290</v>
+        <v>2629</v>
       </c>
       <c r="P282" s="4" t="s">
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="283" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A283" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B283" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C283" s="4" t="s">
-        <v>1673</v>
-      </c>
-      <c r="D283" s="4" t="s">
-        <v>1940</v>
-      </c>
-      <c r="E283" s="4" t="s">
-        <v>2399</v>
-      </c>
-      <c r="F283" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="G283" s="4" t="s">
-        <v>1941</v>
-      </c>
-      <c r="H283" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="I283" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="J283" s="4" t="s">
-        <v>1939</v>
-      </c>
-      <c r="K283" s="4" t="s">
-        <v>2398</v>
-      </c>
-      <c r="L283" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="M283" s="4" t="s">
-        <v>963</v>
-      </c>
-      <c r="N283" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="O283" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="P283" s="4" t="s">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="284" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>2630</v>
+      </c>
+    </row>
+    <row r="283" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="284" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A284" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B284" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C284" s="4" t="s">
+        <v>1595</v>
+      </c>
+      <c r="D284" s="4" t="s">
+        <v>1821</v>
+      </c>
+      <c r="E284" s="4" t="s">
+        <v>2394</v>
+      </c>
+      <c r="F284" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="G284" s="4" t="s">
+        <v>1830</v>
+      </c>
+      <c r="H284" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="I284" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="J284" s="4" t="s">
+        <v>1937</v>
+      </c>
+      <c r="K284" s="4" t="s">
+        <v>2396</v>
+      </c>
+      <c r="L284" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="M284" s="4" t="s">
+        <v>897</v>
+      </c>
+      <c r="N284" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O284" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="P284" s="4" t="s">
+        <v>988</v>
+      </c>
+    </row>
     <row r="285" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A285" s="4" t="s">
-        <v>2583</v>
+        <v>38</v>
       </c>
       <c r="B285" s="4" t="s">
-        <v>2585</v>
+        <v>81</v>
       </c>
       <c r="C285" s="4" t="s">
-        <v>2587</v>
+        <v>1672</v>
       </c>
       <c r="D285" s="4" t="s">
-        <v>2609</v>
+        <v>1935</v>
       </c>
       <c r="E285" s="4" t="s">
-        <v>2610</v>
+        <v>2395</v>
       </c>
       <c r="F285" s="4" t="s">
-        <v>2611</v>
+        <v>81</v>
       </c>
       <c r="G285" s="4" t="s">
-        <v>2612</v>
+        <v>1936</v>
       </c>
       <c r="H285" s="4" t="s">
-        <v>2613</v>
+        <v>118</v>
       </c>
       <c r="I285" s="4" t="s">
-        <v>2614</v>
+        <v>81</v>
       </c>
       <c r="J285" s="4" t="s">
-        <v>2608</v>
+        <v>1938</v>
       </c>
       <c r="K285" s="4" t="s">
-        <v>2607</v>
+        <v>2397</v>
       </c>
       <c r="L285" s="4" t="s">
-        <v>2606</v>
+        <v>209</v>
       </c>
       <c r="M285" s="4" t="s">
-        <v>2605</v>
+        <v>962</v>
       </c>
       <c r="N285" s="4" t="s">
-        <v>2604</v>
+        <v>246</v>
       </c>
       <c r="O285" s="4" t="s">
-        <v>2603</v>
+        <v>290</v>
       </c>
       <c r="P285" s="4" t="s">
-        <v>2602</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="286" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A286" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B286" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C286" s="4" t="s">
+        <v>1673</v>
+      </c>
+      <c r="D286" s="4" t="s">
+        <v>1940</v>
+      </c>
+      <c r="E286" s="4" t="s">
+        <v>2399</v>
+      </c>
+      <c r="F286" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="G286" s="4" t="s">
+        <v>1941</v>
+      </c>
+      <c r="H286" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="I286" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="J286" s="4" t="s">
+        <v>1939</v>
+      </c>
+      <c r="K286" s="4" t="s">
+        <v>2398</v>
+      </c>
+      <c r="L286" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="M286" s="4" t="s">
+        <v>963</v>
+      </c>
+      <c r="N286" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="O286" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="P286" s="4" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="287" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="288" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A288" s="4" t="s">
+        <v>2583</v>
+      </c>
+      <c r="B288" s="4" t="s">
+        <v>2585</v>
+      </c>
+      <c r="C288" s="4" t="s">
+        <v>2587</v>
+      </c>
+      <c r="D288" s="4" t="s">
+        <v>2609</v>
+      </c>
+      <c r="E288" s="4" t="s">
+        <v>2610</v>
+      </c>
+      <c r="F288" s="4" t="s">
+        <v>2611</v>
+      </c>
+      <c r="G288" s="4" t="s">
+        <v>2612</v>
+      </c>
+      <c r="H288" s="4" t="s">
+        <v>2613</v>
+      </c>
+      <c r="I288" s="4" t="s">
+        <v>2614</v>
+      </c>
+      <c r="J288" s="4" t="s">
+        <v>2608</v>
+      </c>
+      <c r="K288" s="4" t="s">
+        <v>2607</v>
+      </c>
+      <c r="L288" s="4" t="s">
+        <v>2606</v>
+      </c>
+      <c r="M288" s="4" t="s">
+        <v>2605</v>
+      </c>
+      <c r="N288" s="4" t="s">
+        <v>2604</v>
+      </c>
+      <c r="O288" s="4" t="s">
+        <v>2603</v>
+      </c>
+      <c r="P288" s="4" t="s">
+        <v>2602</v>
+      </c>
+    </row>
+    <row r="289" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A289" s="4" t="s">
         <v>2582</v>
       </c>
-      <c r="B286" s="4" t="s">
+      <c r="B289" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C286" s="4" t="s">
+      <c r="C289" s="4" t="s">
         <v>1671</v>
       </c>
-      <c r="D286" s="4" t="s">
+      <c r="D289" s="4" t="s">
         <v>1942</v>
       </c>
-      <c r="E286" s="4" t="s">
+      <c r="E289" s="4" t="s">
         <v>2400</v>
       </c>
-      <c r="F286" s="4" t="s">
+      <c r="F289" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="G286" s="4" t="s">
+      <c r="G289" s="4" t="s">
         <v>1943</v>
       </c>
-      <c r="H286" s="4" t="s">
+      <c r="H289" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="I286" s="4" t="s">
+      <c r="I289" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="J286" s="4" t="s">
+      <c r="J289" s="4" t="s">
         <v>1944</v>
       </c>
-      <c r="K286" s="4" t="s">
+      <c r="K289" s="4" t="s">
         <v>2401</v>
       </c>
-      <c r="L286" s="4" t="s">
+      <c r="L289" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="M286" s="4" t="s">
+      <c r="M289" s="4" t="s">
         <v>964</v>
       </c>
-      <c r="N286" s="4" t="s">
+      <c r="N289" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="O286" s="4" t="s">
+      <c r="O289" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="P286" s="4" t="s">
+      <c r="P289" s="4" t="s">
         <v>1027</v>
       </c>
     </row>
-    <row r="287" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A287" s="4" t="s">
+    <row r="290" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A290" s="4" t="s">
         <v>2584</v>
       </c>
-      <c r="B287" s="4" t="s">
+      <c r="B290" s="4" t="s">
         <v>2586</v>
       </c>
-      <c r="C287" s="4" t="s">
+      <c r="C290" s="4" t="s">
         <v>2588</v>
       </c>
-      <c r="D287" s="4" t="s">
+      <c r="D290" s="4" t="s">
         <v>2589</v>
       </c>
-      <c r="E287" s="4" t="s">
+      <c r="E290" s="4" t="s">
         <v>2590</v>
       </c>
-      <c r="F287" s="4" t="s">
+      <c r="F290" s="4" t="s">
         <v>2591</v>
       </c>
-      <c r="G287" s="4" t="s">
+      <c r="G290" s="4" t="s">
         <v>2592</v>
       </c>
-      <c r="H287" s="5" t="s">
+      <c r="H290" s="5" t="s">
         <v>2593</v>
       </c>
-      <c r="I287" s="4" t="s">
+      <c r="I290" s="4" t="s">
         <v>2594</v>
       </c>
-      <c r="J287" s="4" t="s">
+      <c r="J290" s="4" t="s">
         <v>2595</v>
       </c>
-      <c r="K287" s="4" t="s">
+      <c r="K290" s="4" t="s">
         <v>2596</v>
       </c>
-      <c r="L287" s="4" t="s">
+      <c r="L290" s="4" t="s">
         <v>2597</v>
       </c>
-      <c r="M287" s="4" t="s">
+      <c r="M290" s="4" t="s">
         <v>2598</v>
       </c>
-      <c r="N287" s="4" t="s">
+      <c r="N290" s="4" t="s">
         <v>2599</v>
       </c>
-      <c r="O287" s="4" t="s">
+      <c r="O290" s="4" t="s">
         <v>2600</v>
       </c>
-      <c r="P287" s="4" t="s">
+      <c r="P290" s="4" t="s">
         <v>2601</v>
       </c>
     </row>

</xml_diff>

<commit_message>
II Core, II Windows 1.2.6: Print Screen, Save to .pdf - II Core: localization updated II Windows - implemented ScreenshotPdf: AssemblePdf(), SavePdf(), PrintPdf() - Screenshot.GetBitmap(UIElement) ties into saving/printing pdf - Save and Print screen functions implemented into: (#105)   - DeviceECG, DeviceMonitor, DeviceIABP, DeviceDefib
</commit_message>
<xml_diff>
--- a/II Core/Localization Strings.xlsx
+++ b/II Core/Localization Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibi\Documents\Infirmary Integrated\II Core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778CF6CE-3599-4AF1-80D1-F5797065E6DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A61F96-78B1-4830-9712-F08754E69885}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="203" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="203" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8316" uniqueCount="3383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8380" uniqueCount="3415">
   <si>
     <t>Temperature</t>
   </si>
@@ -10174,6 +10174,102 @@
   </si>
   <si>
     <t>החל שינויים באופן אוטומטי</t>
+  </si>
+  <si>
+    <t>MENU:MenuSaveScreen</t>
+  </si>
+  <si>
+    <t>MENU:MenuPrintScreen</t>
+  </si>
+  <si>
+    <t>Save Screen</t>
+  </si>
+  <si>
+    <t>Print Screen</t>
+  </si>
+  <si>
+    <t>Сохранить изображение экрана</t>
+  </si>
+  <si>
+    <t>Salvar imagem da tela</t>
+  </si>
+  <si>
+    <t>Guardar imagen de pantalla</t>
+  </si>
+  <si>
+    <t>Enregistrer l'image de l'écran</t>
+  </si>
+  <si>
+    <t>Salva immagine sullo schermo</t>
+  </si>
+  <si>
+    <t>화면 이미지 저장</t>
+  </si>
+  <si>
+    <t>Hifadhi picha ya skrini</t>
+  </si>
+  <si>
+    <t>שמור את תמונת המסך</t>
+  </si>
+  <si>
+    <t>स्क्रीन की छवि सहेजें</t>
+  </si>
+  <si>
+    <t>የማያ ገጹን ምስል ያስቀምጡ</t>
+  </si>
+  <si>
+    <t>حفظ صورة من الشاشة</t>
+  </si>
+  <si>
+    <t>保存屏幕图像</t>
+  </si>
+  <si>
+    <t>Bild des Bildschirms speichern</t>
+  </si>
+  <si>
+    <t>تصویر صفحه را ذخیره کنید</t>
+  </si>
+  <si>
+    <t>تصویری از صفحه را چاپ کنید</t>
+  </si>
+  <si>
+    <t>የማያ ገጹን ምስል ያትሙ</t>
+  </si>
+  <si>
+    <t>طباعة صورة من الشاشة</t>
+  </si>
+  <si>
+    <t>打印屏幕图像</t>
+  </si>
+  <si>
+    <t>Drucken Sie ein Bild des Bildschirms</t>
+  </si>
+  <si>
+    <t>Imprime una imagen de la pantalla</t>
+  </si>
+  <si>
+    <t>Imprimer une image de l'écran</t>
+  </si>
+  <si>
+    <t>הדפס תמונה של המסך</t>
+  </si>
+  <si>
+    <t>स्क्रीन की एक छवि प्रिंट करें</t>
+  </si>
+  <si>
+    <t>Stampa un'immagine dello schermo</t>
+  </si>
+  <si>
+    <t>화면 이미지 인쇄</t>
+  </si>
+  <si>
+    <t>Imprimir uma imagem da tela</t>
+  </si>
+  <si>
+    <t>Распечатать изображение экрана</t>
+  </si>
+  <si>
+    <t>Chapisha picha ya skrini</t>
   </si>
 </sst>
 </file>
@@ -10551,11 +10647,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P292"/>
+  <dimension ref="A1:P294"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <pane ySplit="1" topLeftCell="A212" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A220" sqref="A220:XFD221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="60.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20298,3309 +20394,3409 @@
     </row>
     <row r="220" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A220" s="4" t="s">
-        <v>1029</v>
+        <v>3383</v>
       </c>
       <c r="B220" s="4" t="s">
-        <v>77</v>
+        <v>3385</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>1560</v>
+        <v>3396</v>
       </c>
       <c r="D220" s="4" t="s">
-        <v>1962</v>
+        <v>3397</v>
       </c>
       <c r="E220" s="4" t="s">
-        <v>2216</v>
+        <v>3398</v>
       </c>
       <c r="F220" s="4" t="s">
-        <v>331</v>
+        <v>3399</v>
       </c>
       <c r="G220" s="4" t="s">
-        <v>1976</v>
+        <v>3400</v>
       </c>
       <c r="H220" s="4" t="s">
-        <v>171</v>
+        <v>3389</v>
       </c>
       <c r="I220" s="4" t="s">
-        <v>160</v>
+        <v>3390</v>
       </c>
       <c r="J220" s="4" t="s">
-        <v>1990</v>
+        <v>3394</v>
       </c>
       <c r="K220" s="4" t="s">
-        <v>2230</v>
+        <v>3395</v>
       </c>
       <c r="L220" s="4" t="s">
-        <v>207</v>
+        <v>3391</v>
       </c>
       <c r="M220" s="4" t="s">
-        <v>862</v>
+        <v>3392</v>
       </c>
       <c r="N220" s="4" t="s">
-        <v>245</v>
+        <v>3388</v>
       </c>
       <c r="O220" s="4" t="s">
-        <v>288</v>
+        <v>3387</v>
       </c>
       <c r="P220" s="4" t="s">
-        <v>938</v>
+        <v>3393</v>
       </c>
     </row>
     <row r="221" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A221" s="4" t="s">
-        <v>1030</v>
+        <v>3384</v>
       </c>
       <c r="B221" s="4" t="s">
-        <v>45</v>
+        <v>3386</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>1495</v>
+        <v>3402</v>
       </c>
       <c r="D221" s="4" t="s">
-        <v>1709</v>
+        <v>3403</v>
       </c>
       <c r="E221" s="4" t="s">
-        <v>2126</v>
+        <v>3404</v>
       </c>
       <c r="F221" s="4" t="s">
-        <v>348</v>
+        <v>3405</v>
       </c>
       <c r="G221" s="4" t="s">
-        <v>1718</v>
+        <v>3401</v>
       </c>
       <c r="H221" s="4" t="s">
-        <v>349</v>
+        <v>3406</v>
       </c>
       <c r="I221" s="4" t="s">
-        <v>350</v>
+        <v>3407</v>
       </c>
       <c r="J221" s="4" t="s">
-        <v>1727</v>
+        <v>3408</v>
       </c>
       <c r="K221" s="4" t="s">
-        <v>2133</v>
+        <v>3409</v>
       </c>
       <c r="L221" s="4" t="s">
-        <v>351</v>
+        <v>3410</v>
       </c>
       <c r="M221" s="4" t="s">
-        <v>821</v>
+        <v>3411</v>
       </c>
       <c r="N221" s="4" t="s">
-        <v>765</v>
+        <v>3412</v>
       </c>
       <c r="O221" s="4" t="s">
-        <v>255</v>
+        <v>3413</v>
       </c>
       <c r="P221" s="4" t="s">
-        <v>903</v>
+        <v>3414</v>
       </c>
     </row>
     <row r="222" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A222" s="4" t="s">
-        <v>1033</v>
+        <v>1029</v>
       </c>
       <c r="B222" s="4" t="s">
-        <v>702</v>
+        <v>77</v>
       </c>
       <c r="C222" s="4" t="s">
-        <v>1563</v>
+        <v>1560</v>
       </c>
       <c r="D222" s="4" t="s">
-        <v>1965</v>
+        <v>1962</v>
       </c>
       <c r="E222" s="4" t="s">
-        <v>2219</v>
+        <v>2216</v>
       </c>
       <c r="F222" s="4" t="s">
-        <v>779</v>
+        <v>331</v>
       </c>
       <c r="G222" s="4" t="s">
-        <v>1979</v>
+        <v>1976</v>
       </c>
       <c r="H222" s="4" t="s">
-        <v>774</v>
+        <v>171</v>
       </c>
       <c r="I222" s="4" t="s">
-        <v>775</v>
+        <v>160</v>
       </c>
       <c r="J222" s="4" t="s">
-        <v>1993</v>
+        <v>1990</v>
       </c>
       <c r="K222" s="4" t="s">
-        <v>2233</v>
+        <v>2230</v>
       </c>
       <c r="L222" s="4" t="s">
-        <v>776</v>
+        <v>207</v>
       </c>
       <c r="M222" s="4" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="N222" s="4" t="s">
-        <v>777</v>
+        <v>245</v>
       </c>
       <c r="O222" s="4" t="s">
-        <v>778</v>
+        <v>288</v>
       </c>
       <c r="P222" s="4" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
     </row>
     <row r="223" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A223" s="4" t="s">
-        <v>1052</v>
+        <v>1030</v>
       </c>
       <c r="B223" s="4" t="s">
-        <v>1051</v>
+        <v>45</v>
       </c>
       <c r="C223" s="4" t="s">
-        <v>1564</v>
+        <v>1495</v>
       </c>
       <c r="D223" s="4" t="s">
-        <v>1966</v>
+        <v>1709</v>
       </c>
       <c r="E223" s="4" t="s">
-        <v>2220</v>
+        <v>2126</v>
       </c>
       <c r="F223" s="4" t="s">
-        <v>1071</v>
+        <v>348</v>
       </c>
       <c r="G223" s="4" t="s">
-        <v>1980</v>
+        <v>1718</v>
       </c>
       <c r="H223" s="4" t="s">
-        <v>1072</v>
+        <v>349</v>
       </c>
       <c r="I223" s="4" t="s">
-        <v>1073</v>
+        <v>350</v>
       </c>
       <c r="J223" s="4" t="s">
-        <v>1994</v>
+        <v>1727</v>
       </c>
       <c r="K223" s="4" t="s">
-        <v>2234</v>
+        <v>2133</v>
       </c>
       <c r="L223" s="4" t="s">
-        <v>1074</v>
+        <v>351</v>
       </c>
       <c r="M223" s="4" t="s">
-        <v>1075</v>
+        <v>821</v>
       </c>
       <c r="N223" s="4" t="s">
-        <v>1076</v>
+        <v>765</v>
       </c>
       <c r="O223" s="4" t="s">
-        <v>1077</v>
+        <v>255</v>
       </c>
       <c r="P223" s="4" t="s">
-        <v>1078</v>
+        <v>903</v>
       </c>
     </row>
     <row r="224" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A224" s="4" t="s">
-        <v>3273</v>
+        <v>1033</v>
       </c>
       <c r="B224" s="4" t="s">
-        <v>3274</v>
+        <v>702</v>
       </c>
       <c r="C224" s="4" t="s">
-        <v>3298</v>
+        <v>1563</v>
       </c>
       <c r="D224" s="4" t="s">
-        <v>3299</v>
+        <v>1965</v>
       </c>
       <c r="E224" s="4" t="s">
-        <v>3300</v>
+        <v>2219</v>
       </c>
       <c r="F224" s="4" t="s">
-        <v>3301</v>
+        <v>779</v>
       </c>
       <c r="G224" s="4" t="s">
-        <v>3302</v>
+        <v>1979</v>
       </c>
       <c r="H224" s="4" t="s">
-        <v>3290</v>
+        <v>774</v>
       </c>
       <c r="I224" s="4" t="s">
-        <v>3289</v>
+        <v>775</v>
       </c>
       <c r="J224" s="4" t="s">
-        <v>3291</v>
+        <v>1993</v>
       </c>
       <c r="K224" s="4" t="s">
-        <v>3292</v>
+        <v>2233</v>
       </c>
       <c r="L224" s="4" t="s">
-        <v>3293</v>
+        <v>776</v>
       </c>
       <c r="M224" s="4" t="s">
-        <v>3294</v>
+        <v>865</v>
       </c>
       <c r="N224" s="4" t="s">
-        <v>3295</v>
+        <v>777</v>
       </c>
       <c r="O224" s="4" t="s">
-        <v>3296</v>
+        <v>778</v>
       </c>
       <c r="P224" s="4" t="s">
-        <v>3297</v>
+        <v>941</v>
+      </c>
+    </row>
+    <row r="225" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A225" s="4" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B225" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C225" s="4" t="s">
+        <v>1564</v>
+      </c>
+      <c r="D225" s="4" t="s">
+        <v>1966</v>
+      </c>
+      <c r="E225" s="4" t="s">
+        <v>2220</v>
+      </c>
+      <c r="F225" s="4" t="s">
+        <v>1071</v>
+      </c>
+      <c r="G225" s="4" t="s">
+        <v>1980</v>
+      </c>
+      <c r="H225" s="4" t="s">
+        <v>1072</v>
+      </c>
+      <c r="I225" s="4" t="s">
+        <v>1073</v>
+      </c>
+      <c r="J225" s="4" t="s">
+        <v>1994</v>
+      </c>
+      <c r="K225" s="4" t="s">
+        <v>2234</v>
+      </c>
+      <c r="L225" s="4" t="s">
+        <v>1074</v>
+      </c>
+      <c r="M225" s="4" t="s">
+        <v>1075</v>
+      </c>
+      <c r="N225" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="O225" s="4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="P225" s="4" t="s">
+        <v>1078</v>
       </c>
     </row>
     <row r="226" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A226" s="4" t="s">
-        <v>445</v>
+        <v>3273</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>442</v>
+        <v>3274</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>1565</v>
+        <v>3298</v>
       </c>
       <c r="D226" s="4" t="s">
-        <v>1739</v>
+        <v>3299</v>
       </c>
       <c r="E226" s="4" t="s">
-        <v>2045</v>
+        <v>3300</v>
       </c>
       <c r="F226" s="4" t="s">
-        <v>636</v>
+        <v>3301</v>
       </c>
       <c r="G226" s="4" t="s">
-        <v>1748</v>
+        <v>3302</v>
       </c>
       <c r="H226" s="4" t="s">
-        <v>639</v>
+        <v>3290</v>
       </c>
       <c r="I226" s="4" t="s">
-        <v>658</v>
+        <v>3289</v>
       </c>
       <c r="J226" s="4" t="s">
-        <v>1946</v>
-      </c>
-      <c r="K226" s="5" t="s">
-        <v>2054</v>
+        <v>3291</v>
+      </c>
+      <c r="K226" s="4" t="s">
+        <v>3292</v>
       </c>
       <c r="L226" s="4" t="s">
-        <v>685</v>
+        <v>3293</v>
       </c>
       <c r="M226" s="4" t="s">
-        <v>867</v>
+        <v>3294</v>
       </c>
       <c r="N226" s="4" t="s">
-        <v>643</v>
+        <v>3295</v>
       </c>
       <c r="O226" s="4" t="s">
-        <v>688</v>
+        <v>3296</v>
       </c>
       <c r="P226" s="4" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="227" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="B227" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C227" s="4" t="s">
-        <v>1513</v>
-      </c>
-      <c r="D227" s="4" t="s">
-        <v>1765</v>
-      </c>
-      <c r="E227" s="4" t="s">
-        <v>2064</v>
-      </c>
-      <c r="F227" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="G227" s="4" t="s">
-        <v>1781</v>
-      </c>
-      <c r="H227" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="I227" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="J227" s="4" t="s">
-        <v>1805</v>
-      </c>
-      <c r="K227" s="4" t="s">
-        <v>2081</v>
-      </c>
-      <c r="L227" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="M227" s="4" t="s">
-        <v>838</v>
-      </c>
-      <c r="N227" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="O227" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="P227" s="4" t="s">
-        <v>918</v>
+        <v>3297</v>
       </c>
     </row>
     <row r="228" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A228" s="4" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>50</v>
+        <v>442</v>
       </c>
       <c r="C228" s="4" t="s">
-        <v>1511</v>
+        <v>1565</v>
       </c>
       <c r="D228" s="4" t="s">
-        <v>1764</v>
+        <v>1739</v>
       </c>
       <c r="E228" s="4" t="s">
-        <v>2062</v>
+        <v>2045</v>
       </c>
       <c r="F228" s="4" t="s">
-        <v>309</v>
+        <v>636</v>
       </c>
       <c r="G228" s="4" t="s">
-        <v>1780</v>
+        <v>1748</v>
       </c>
       <c r="H228" s="4" t="s">
-        <v>99</v>
+        <v>639</v>
       </c>
       <c r="I228" s="4" t="s">
-        <v>139</v>
+        <v>658</v>
       </c>
       <c r="J228" s="4" t="s">
-        <v>1803</v>
-      </c>
-      <c r="K228" s="4" t="s">
-        <v>2079</v>
+        <v>1946</v>
+      </c>
+      <c r="K228" s="5" t="s">
+        <v>2054</v>
       </c>
       <c r="L228" s="4" t="s">
-        <v>190</v>
+        <v>685</v>
       </c>
       <c r="M228" s="4" t="s">
-        <v>836</v>
+        <v>867</v>
       </c>
       <c r="N228" s="4" t="s">
-        <v>225</v>
+        <v>643</v>
       </c>
       <c r="O228" s="4" t="s">
-        <v>268</v>
+        <v>688</v>
       </c>
       <c r="P228" s="4" t="s">
-        <v>916</v>
+        <v>442</v>
       </c>
     </row>
     <row r="229" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A229" s="4" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>443</v>
+        <v>0</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>1566</v>
+        <v>1513</v>
       </c>
       <c r="D229" s="4" t="s">
-        <v>1995</v>
+        <v>1765</v>
       </c>
       <c r="E229" s="4" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="F229" s="4" t="s">
-        <v>637</v>
+        <v>311</v>
       </c>
       <c r="G229" s="4" t="s">
-        <v>1998</v>
+        <v>1781</v>
       </c>
       <c r="H229" s="4" t="s">
-        <v>640</v>
+        <v>101</v>
       </c>
       <c r="I229" s="4" t="s">
-        <v>659</v>
+        <v>141</v>
       </c>
       <c r="J229" s="4" t="s">
-        <v>2001</v>
+        <v>1805</v>
       </c>
       <c r="K229" s="4" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
       <c r="L229" s="4" t="s">
-        <v>673</v>
+        <v>101</v>
       </c>
       <c r="M229" s="4" t="s">
-        <v>868</v>
+        <v>838</v>
       </c>
       <c r="N229" s="4" t="s">
-        <v>644</v>
+        <v>101</v>
       </c>
       <c r="O229" s="4" t="s">
-        <v>610</v>
+        <v>270</v>
       </c>
       <c r="P229" s="4" t="s">
-        <v>942</v>
+        <v>918</v>
       </c>
     </row>
     <row r="230" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A230" s="4" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C230" s="4" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="D230" s="4" t="s">
-        <v>1799</v>
+        <v>1764</v>
       </c>
       <c r="E230" s="4" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="F230" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G230" s="4" t="s">
-        <v>1800</v>
+        <v>1780</v>
       </c>
       <c r="H230" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I230" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J230" s="4" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="K230" s="4" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
       <c r="L230" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M230" s="4" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="N230" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O230" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="P230" s="4" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="231" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A231" s="4" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B231" s="4" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C231" s="4" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="D231" s="4" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="E231" s="4" t="s">
-        <v>2235</v>
+        <v>2065</v>
       </c>
       <c r="F231" s="4" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G231" s="4" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="H231" s="4" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I231" s="4" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="J231" s="4" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="K231" s="4" t="s">
-        <v>2238</v>
+        <v>2082</v>
       </c>
       <c r="L231" s="4" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="M231" s="4" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="N231" s="4" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="O231" s="4" t="s">
-        <v>689</v>
+        <v>610</v>
       </c>
       <c r="P231" s="4" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="232" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A232" s="4" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B232" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C232" s="4" t="s">
-        <v>1515</v>
+        <v>1512</v>
       </c>
       <c r="D232" s="4" t="s">
-        <v>1767</v>
+        <v>1799</v>
       </c>
       <c r="E232" s="4" t="s">
-        <v>2066</v>
+        <v>2063</v>
       </c>
       <c r="F232" s="4" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="G232" s="4" t="s">
-        <v>1779</v>
+        <v>1800</v>
       </c>
       <c r="H232" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I232" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="J232" s="4" t="s">
-        <v>1807</v>
+        <v>1804</v>
       </c>
       <c r="K232" s="4" t="s">
-        <v>2083</v>
+        <v>2080</v>
       </c>
       <c r="L232" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M232" s="4" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="N232" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O232" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="P232" s="4" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
     </row>
     <row r="233" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A233" s="4" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B233" s="4" t="s">
-        <v>54</v>
+        <v>444</v>
       </c>
       <c r="C233" s="4" t="s">
-        <v>1516</v>
+        <v>1567</v>
       </c>
       <c r="D233" s="4" t="s">
-        <v>1768</v>
+        <v>1996</v>
       </c>
       <c r="E233" s="4" t="s">
-        <v>2067</v>
+        <v>2235</v>
       </c>
       <c r="F233" s="4" t="s">
-        <v>314</v>
+        <v>638</v>
       </c>
       <c r="G233" s="4" t="s">
-        <v>1783</v>
+        <v>1999</v>
       </c>
       <c r="H233" s="4" t="s">
-        <v>103</v>
+        <v>641</v>
       </c>
       <c r="I233" s="4" t="s">
-        <v>144</v>
+        <v>660</v>
       </c>
       <c r="J233" s="4" t="s">
-        <v>1808</v>
+        <v>2002</v>
       </c>
       <c r="K233" s="4" t="s">
-        <v>2084</v>
+        <v>2238</v>
       </c>
       <c r="L233" s="4" t="s">
-        <v>193</v>
+        <v>674</v>
       </c>
       <c r="M233" s="4" t="s">
-        <v>840</v>
+        <v>869</v>
       </c>
       <c r="N233" s="4" t="s">
-        <v>228</v>
+        <v>645</v>
       </c>
       <c r="O233" s="4" t="s">
-        <v>272</v>
+        <v>689</v>
       </c>
       <c r="P233" s="4" t="s">
-        <v>920</v>
+        <v>943</v>
       </c>
     </row>
     <row r="234" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A234" s="4" t="s">
-        <v>703</v>
+        <v>451</v>
       </c>
       <c r="B234" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C234" s="4" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
       <c r="D234" s="4" t="s">
-        <v>1769</v>
+        <v>1767</v>
       </c>
       <c r="E234" s="4" t="s">
-        <v>2068</v>
+        <v>2066</v>
       </c>
       <c r="F234" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G234" s="4" t="s">
-        <v>1784</v>
+        <v>1779</v>
       </c>
       <c r="H234" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I234" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J234" s="4" t="s">
-        <v>1809</v>
+        <v>1807</v>
       </c>
       <c r="K234" s="4" t="s">
-        <v>2085</v>
+        <v>2083</v>
       </c>
       <c r="L234" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="M234" s="4" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="N234" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="O234" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="P234" s="4" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
     <row r="235" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A235" s="4" t="s">
-        <v>2363</v>
+        <v>452</v>
       </c>
       <c r="B235" s="4" t="s">
-        <v>2365</v>
+        <v>54</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>2370</v>
+        <v>1516</v>
       </c>
       <c r="D235" s="4" t="s">
-        <v>2366</v>
+        <v>1768</v>
       </c>
       <c r="E235" s="4" t="s">
-        <v>2371</v>
+        <v>2067</v>
       </c>
       <c r="F235" s="4" t="s">
-        <v>2372</v>
+        <v>314</v>
       </c>
       <c r="G235" s="4" t="s">
-        <v>2369</v>
+        <v>1783</v>
       </c>
       <c r="H235" s="4" t="s">
-        <v>2367</v>
+        <v>103</v>
       </c>
       <c r="I235" s="4" t="s">
-        <v>2368</v>
+        <v>144</v>
       </c>
       <c r="J235" s="4" t="s">
-        <v>2373</v>
+        <v>1808</v>
       </c>
       <c r="K235" s="4" t="s">
-        <v>2374</v>
+        <v>2084</v>
       </c>
       <c r="L235" s="4" t="s">
-        <v>2375</v>
+        <v>193</v>
       </c>
       <c r="M235" s="4" t="s">
-        <v>2376</v>
+        <v>840</v>
       </c>
       <c r="N235" s="4" t="s">
-        <v>2377</v>
+        <v>228</v>
       </c>
       <c r="O235" s="4" t="s">
-        <v>2378</v>
+        <v>272</v>
       </c>
       <c r="P235" s="4" t="s">
-        <v>2379</v>
+        <v>920</v>
       </c>
     </row>
     <row r="236" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A236" s="4" t="s">
-        <v>2383</v>
+        <v>703</v>
       </c>
       <c r="B236" s="4" t="s">
-        <v>2381</v>
+        <v>55</v>
       </c>
       <c r="C236" s="4" t="s">
-        <v>2386</v>
+        <v>1517</v>
       </c>
       <c r="D236" s="4" t="s">
-        <v>2387</v>
+        <v>1769</v>
       </c>
       <c r="E236" s="4" t="s">
-        <v>2388</v>
+        <v>2068</v>
       </c>
       <c r="F236" s="4" t="s">
-        <v>2389</v>
+        <v>315</v>
       </c>
       <c r="G236" s="4" t="s">
-        <v>2390</v>
+        <v>1784</v>
       </c>
       <c r="H236" s="4" t="s">
-        <v>2391</v>
+        <v>104</v>
       </c>
       <c r="I236" s="4" t="s">
-        <v>2392</v>
+        <v>145</v>
       </c>
       <c r="J236" s="4" t="s">
-        <v>2393</v>
+        <v>1809</v>
       </c>
       <c r="K236" s="4" t="s">
-        <v>2394</v>
+        <v>2085</v>
       </c>
       <c r="L236" s="4" t="s">
-        <v>2395</v>
+        <v>194</v>
       </c>
       <c r="M236" s="4" t="s">
-        <v>2396</v>
+        <v>841</v>
       </c>
       <c r="N236" s="4" t="s">
-        <v>2397</v>
+        <v>229</v>
       </c>
       <c r="O236" s="4" t="s">
-        <v>2385</v>
+        <v>273</v>
       </c>
       <c r="P236" s="4" t="s">
-        <v>2384</v>
+        <v>921</v>
       </c>
     </row>
     <row r="237" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A237" s="4" t="s">
-        <v>1214</v>
+        <v>2363</v>
       </c>
       <c r="B237" s="4" t="s">
-        <v>1061</v>
+        <v>2365</v>
       </c>
       <c r="C237" s="4" t="s">
-        <v>1568</v>
+        <v>2370</v>
       </c>
       <c r="D237" s="4" t="s">
-        <v>1907</v>
+        <v>2366</v>
       </c>
       <c r="E237" s="4" t="s">
-        <v>2236</v>
+        <v>2371</v>
       </c>
       <c r="F237" s="4" t="s">
-        <v>1190</v>
+        <v>2372</v>
       </c>
       <c r="G237" s="4" t="s">
-        <v>1922</v>
+        <v>2369</v>
       </c>
       <c r="H237" s="4" t="s">
-        <v>1191</v>
+        <v>2367</v>
       </c>
       <c r="I237" s="4" t="s">
-        <v>1192</v>
+        <v>2368</v>
       </c>
       <c r="J237" s="4" t="s">
-        <v>1938</v>
+        <v>2373</v>
       </c>
       <c r="K237" s="4" t="s">
-        <v>2239</v>
+        <v>2374</v>
       </c>
       <c r="L237" s="4" t="s">
-        <v>1193</v>
+        <v>2375</v>
       </c>
       <c r="M237" s="4" t="s">
-        <v>1194</v>
+        <v>2376</v>
       </c>
       <c r="N237" s="4" t="s">
-        <v>1195</v>
+        <v>2377</v>
       </c>
       <c r="O237" s="4" t="s">
-        <v>1196</v>
+        <v>2378</v>
       </c>
       <c r="P237" s="4" t="s">
-        <v>1197</v>
+        <v>2379</v>
       </c>
     </row>
     <row r="238" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A238" s="4" t="s">
-        <v>1240</v>
+        <v>2383</v>
       </c>
       <c r="B238" s="4" t="s">
-        <v>1239</v>
+        <v>2381</v>
       </c>
       <c r="C238" s="4" t="s">
-        <v>1569</v>
+        <v>2386</v>
       </c>
       <c r="D238" s="4" t="s">
-        <v>1997</v>
+        <v>2387</v>
       </c>
       <c r="E238" s="4" t="s">
-        <v>2237</v>
+        <v>2388</v>
       </c>
       <c r="F238" s="4" t="s">
-        <v>1282</v>
+        <v>2389</v>
       </c>
       <c r="G238" s="4" t="s">
-        <v>2000</v>
+        <v>2390</v>
       </c>
       <c r="H238" s="4" t="s">
-        <v>1307</v>
+        <v>2391</v>
       </c>
       <c r="I238" s="4" t="s">
-        <v>1308</v>
+        <v>2392</v>
       </c>
       <c r="J238" s="4" t="s">
-        <v>2003</v>
+        <v>2393</v>
       </c>
       <c r="K238" s="4" t="s">
-        <v>2240</v>
+        <v>2394</v>
       </c>
       <c r="L238" s="4" t="s">
-        <v>1309</v>
+        <v>2395</v>
       </c>
       <c r="M238" s="4" t="s">
-        <v>1310</v>
+        <v>2396</v>
       </c>
       <c r="N238" s="4" t="s">
-        <v>1311</v>
+        <v>2397</v>
       </c>
       <c r="O238" s="4" t="s">
-        <v>1312</v>
+        <v>2385</v>
       </c>
       <c r="P238" s="4" t="s">
-        <v>1313</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="239" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A239" s="4" t="s">
-        <v>1053</v>
+        <v>1214</v>
       </c>
       <c r="B239" s="4" t="s">
-        <v>3248</v>
+        <v>1061</v>
       </c>
       <c r="C239" s="4" t="s">
-        <v>1564</v>
+        <v>1568</v>
       </c>
       <c r="D239" s="4" t="s">
-        <v>3254</v>
+        <v>1907</v>
       </c>
       <c r="E239" s="4" t="s">
-        <v>2220</v>
+        <v>2236</v>
       </c>
       <c r="F239" s="4" t="s">
-        <v>3252</v>
+        <v>1190</v>
       </c>
       <c r="G239" s="4" t="s">
-        <v>3254</v>
+        <v>1922</v>
       </c>
       <c r="H239" s="4" t="s">
-        <v>3246</v>
+        <v>1191</v>
       </c>
       <c r="I239" s="4" t="s">
-        <v>3247</v>
+        <v>1192</v>
       </c>
       <c r="J239" s="4" t="s">
-        <v>3253</v>
+        <v>1938</v>
       </c>
       <c r="K239" s="4" t="s">
-        <v>2234</v>
+        <v>2239</v>
       </c>
       <c r="L239" s="4" t="s">
-        <v>3248</v>
+        <v>1193</v>
       </c>
       <c r="M239" s="4" t="s">
-        <v>3251</v>
+        <v>1194</v>
       </c>
       <c r="N239" s="4" t="s">
-        <v>3248</v>
+        <v>1195</v>
       </c>
       <c r="O239" s="4" t="s">
-        <v>3250</v>
+        <v>1196</v>
       </c>
       <c r="P239" s="4" t="s">
-        <v>3249</v>
-      </c>
-    </row>
-    <row r="240" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="240" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A240" s="4" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B240" s="4" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C240" s="4" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D240" s="4" t="s">
+        <v>1997</v>
+      </c>
+      <c r="E240" s="4" t="s">
+        <v>2237</v>
+      </c>
+      <c r="F240" s="4" t="s">
+        <v>1282</v>
+      </c>
+      <c r="G240" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="H240" s="4" t="s">
+        <v>1307</v>
+      </c>
+      <c r="I240" s="4" t="s">
+        <v>1308</v>
+      </c>
+      <c r="J240" s="4" t="s">
+        <v>2003</v>
+      </c>
+      <c r="K240" s="4" t="s">
+        <v>2240</v>
+      </c>
+      <c r="L240" s="4" t="s">
+        <v>1309</v>
+      </c>
+      <c r="M240" s="4" t="s">
+        <v>1310</v>
+      </c>
+      <c r="N240" s="4" t="s">
+        <v>1311</v>
+      </c>
+      <c r="O240" s="4" t="s">
+        <v>1312</v>
+      </c>
+      <c r="P240" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
     <row r="241" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A241" s="4" t="s">
-        <v>699</v>
+        <v>1053</v>
       </c>
       <c r="B241" s="4" t="s">
-        <v>442</v>
+        <v>3248</v>
       </c>
       <c r="C241" s="4" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="D241" s="4" t="s">
-        <v>1739</v>
+        <v>3254</v>
       </c>
       <c r="E241" s="4" t="s">
-        <v>2045</v>
+        <v>2220</v>
       </c>
       <c r="F241" s="4" t="s">
-        <v>636</v>
+        <v>3252</v>
       </c>
       <c r="G241" s="4" t="s">
-        <v>1748</v>
+        <v>3254</v>
       </c>
       <c r="H241" s="4" t="s">
-        <v>639</v>
+        <v>3246</v>
       </c>
       <c r="I241" s="4" t="s">
-        <v>658</v>
+        <v>3247</v>
       </c>
       <c r="J241" s="4" t="s">
-        <v>1946</v>
-      </c>
-      <c r="K241" s="5" t="s">
-        <v>2054</v>
+        <v>3253</v>
+      </c>
+      <c r="K241" s="4" t="s">
+        <v>2234</v>
       </c>
       <c r="L241" s="4" t="s">
-        <v>685</v>
+        <v>3248</v>
       </c>
       <c r="M241" s="4" t="s">
-        <v>867</v>
+        <v>3251</v>
       </c>
       <c r="N241" s="4" t="s">
-        <v>643</v>
+        <v>3248</v>
       </c>
       <c r="O241" s="4" t="s">
-        <v>688</v>
+        <v>3250</v>
       </c>
       <c r="P241" s="4" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="242" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A242" s="4" t="s">
-        <v>3271</v>
-      </c>
-      <c r="B242" s="4" t="s">
-        <v>1042</v>
-      </c>
-      <c r="C242" s="4" t="s">
-        <v>1600</v>
-      </c>
-      <c r="D242" s="4" t="s">
-        <v>1914</v>
-      </c>
-      <c r="E242" s="4" t="s">
-        <v>2200</v>
-      </c>
-      <c r="F242" s="4" t="s">
-        <v>1103</v>
-      </c>
-      <c r="G242" s="4" t="s">
-        <v>1930</v>
-      </c>
-      <c r="H242" s="4" t="s">
-        <v>1104</v>
-      </c>
-      <c r="I242" s="4" t="s">
-        <v>1095</v>
-      </c>
-      <c r="J242" s="4" t="s">
-        <v>1947</v>
-      </c>
-      <c r="K242" s="4" t="s">
-        <v>2201</v>
-      </c>
-      <c r="L242" s="4" t="s">
-        <v>1099</v>
-      </c>
-      <c r="M242" s="4" t="s">
-        <v>1096</v>
-      </c>
-      <c r="N242" s="4" t="s">
-        <v>1104</v>
-      </c>
-      <c r="O242" s="4" t="s">
-        <v>1107</v>
-      </c>
-      <c r="P242" s="4" t="s">
-        <v>1108</v>
-      </c>
-    </row>
+        <v>3249</v>
+      </c>
+    </row>
+    <row r="242" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="243" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A243" s="4" t="s">
-        <v>3272</v>
+        <v>699</v>
       </c>
       <c r="B243" s="4" t="s">
-        <v>3276</v>
+        <v>442</v>
       </c>
       <c r="C243" s="4" t="s">
-        <v>3283</v>
+        <v>1565</v>
       </c>
       <c r="D243" s="4" t="s">
-        <v>3284</v>
+        <v>1739</v>
       </c>
       <c r="E243" s="4" t="s">
-        <v>3285</v>
+        <v>2045</v>
       </c>
       <c r="F243" s="4" t="s">
-        <v>3282</v>
+        <v>636</v>
       </c>
       <c r="G243" s="4" t="s">
-        <v>3284</v>
+        <v>1748</v>
       </c>
       <c r="H243" s="4" t="s">
-        <v>3281</v>
+        <v>639</v>
       </c>
       <c r="I243" s="4" t="s">
-        <v>3280</v>
+        <v>658</v>
       </c>
       <c r="J243" s="4" t="s">
-        <v>3286</v>
-      </c>
-      <c r="K243" s="4" t="s">
-        <v>3287</v>
+        <v>1946</v>
+      </c>
+      <c r="K243" s="5" t="s">
+        <v>2054</v>
       </c>
       <c r="L243" s="4" t="s">
-        <v>3278</v>
+        <v>685</v>
       </c>
       <c r="M243" s="4" t="s">
-        <v>3288</v>
+        <v>867</v>
       </c>
       <c r="N243" s="4" t="s">
-        <v>3279</v>
+        <v>643</v>
       </c>
       <c r="O243" s="4" t="s">
-        <v>3277</v>
+        <v>688</v>
       </c>
       <c r="P243" s="4" t="s">
-        <v>3275</v>
+        <v>442</v>
       </c>
     </row>
     <row r="244" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K244" s="5"/>
+      <c r="A244" s="4" t="s">
+        <v>3271</v>
+      </c>
+      <c r="B244" s="4" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C244" s="4" t="s">
+        <v>1600</v>
+      </c>
+      <c r="D244" s="4" t="s">
+        <v>1914</v>
+      </c>
+      <c r="E244" s="4" t="s">
+        <v>2200</v>
+      </c>
+      <c r="F244" s="4" t="s">
+        <v>1103</v>
+      </c>
+      <c r="G244" s="4" t="s">
+        <v>1930</v>
+      </c>
+      <c r="H244" s="4" t="s">
+        <v>1104</v>
+      </c>
+      <c r="I244" s="4" t="s">
+        <v>1095</v>
+      </c>
+      <c r="J244" s="4" t="s">
+        <v>1947</v>
+      </c>
+      <c r="K244" s="4" t="s">
+        <v>2201</v>
+      </c>
+      <c r="L244" s="4" t="s">
+        <v>1099</v>
+      </c>
+      <c r="M244" s="4" t="s">
+        <v>1096</v>
+      </c>
+      <c r="N244" s="4" t="s">
+        <v>1104</v>
+      </c>
+      <c r="O244" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="P244" s="4" t="s">
+        <v>1108</v>
+      </c>
     </row>
     <row r="245" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A245" s="4" t="s">
-        <v>465</v>
+        <v>3272</v>
       </c>
       <c r="B245" s="4" t="s">
-        <v>51</v>
+        <v>3276</v>
       </c>
       <c r="C245" s="4" t="s">
-        <v>1512</v>
+        <v>3283</v>
       </c>
       <c r="D245" s="4" t="s">
-        <v>1799</v>
+        <v>3284</v>
       </c>
       <c r="E245" s="4" t="s">
-        <v>2063</v>
+        <v>3285</v>
       </c>
       <c r="F245" s="4" t="s">
-        <v>310</v>
+        <v>3282</v>
       </c>
       <c r="G245" s="4" t="s">
-        <v>1800</v>
+        <v>3284</v>
       </c>
       <c r="H245" s="4" t="s">
-        <v>100</v>
+        <v>3281</v>
       </c>
       <c r="I245" s="4" t="s">
-        <v>140</v>
+        <v>3280</v>
       </c>
       <c r="J245" s="4" t="s">
-        <v>1804</v>
+        <v>3286</v>
       </c>
       <c r="K245" s="4" t="s">
-        <v>2080</v>
+        <v>3287</v>
       </c>
       <c r="L245" s="4" t="s">
-        <v>191</v>
+        <v>3278</v>
       </c>
       <c r="M245" s="4" t="s">
-        <v>837</v>
+        <v>3288</v>
       </c>
       <c r="N245" s="4" t="s">
-        <v>226</v>
+        <v>3279</v>
       </c>
       <c r="O245" s="4" t="s">
-        <v>269</v>
+        <v>3277</v>
       </c>
       <c r="P245" s="4" t="s">
-        <v>954</v>
+        <v>3275</v>
       </c>
     </row>
     <row r="246" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A246" s="4" t="s">
-        <v>466</v>
-      </c>
-      <c r="B246" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C246" s="4" t="s">
-        <v>1516</v>
-      </c>
-      <c r="D246" s="4" t="s">
-        <v>1768</v>
-      </c>
-      <c r="E246" s="4" t="s">
-        <v>2067</v>
-      </c>
-      <c r="F246" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="G246" s="4" t="s">
-        <v>1783</v>
-      </c>
-      <c r="H246" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="I246" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="J246" s="4" t="s">
-        <v>1808</v>
-      </c>
-      <c r="K246" s="4" t="s">
-        <v>2084</v>
-      </c>
-      <c r="L246" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="M246" s="4" t="s">
-        <v>840</v>
-      </c>
-      <c r="N246" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="O246" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="P246" s="4" t="s">
-        <v>920</v>
-      </c>
+      <c r="K246" s="5"/>
     </row>
     <row r="247" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A247" s="4" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B247" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C247" s="4" t="s">
-        <v>1515</v>
+        <v>1512</v>
       </c>
       <c r="D247" s="4" t="s">
-        <v>1767</v>
+        <v>1799</v>
       </c>
       <c r="E247" s="4" t="s">
-        <v>2066</v>
+        <v>2063</v>
       </c>
       <c r="F247" s="4" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="G247" s="4" t="s">
-        <v>1779</v>
+        <v>1800</v>
       </c>
       <c r="H247" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I247" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="J247" s="4" t="s">
-        <v>1807</v>
+        <v>1804</v>
       </c>
       <c r="K247" s="4" t="s">
-        <v>2083</v>
+        <v>2080</v>
       </c>
       <c r="L247" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M247" s="4" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="N247" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O247" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="P247" s="4" t="s">
-        <v>919</v>
+        <v>954</v>
       </c>
     </row>
     <row r="248" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A248" s="4" t="s">
-        <v>482</v>
+        <v>466</v>
       </c>
       <c r="B248" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C248" s="4" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="D248" s="4" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="E248" s="4" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="F248" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G248" s="4" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="H248" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I248" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J248" s="4" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="K248" s="4" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
       <c r="L248" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M248" s="4" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="N248" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="O248" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P248" s="4" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="249" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A249" s="4" t="s">
-        <v>2364</v>
+        <v>467</v>
       </c>
       <c r="B249" s="4" t="s">
-        <v>2365</v>
+        <v>53</v>
       </c>
       <c r="C249" s="4" t="s">
-        <v>2370</v>
+        <v>1515</v>
       </c>
       <c r="D249" s="4" t="s">
-        <v>2366</v>
+        <v>1767</v>
       </c>
       <c r="E249" s="4" t="s">
-        <v>2371</v>
+        <v>2066</v>
       </c>
       <c r="F249" s="4" t="s">
-        <v>2372</v>
+        <v>313</v>
       </c>
       <c r="G249" s="4" t="s">
-        <v>2369</v>
+        <v>1779</v>
       </c>
       <c r="H249" s="4" t="s">
-        <v>2367</v>
+        <v>102</v>
       </c>
       <c r="I249" s="4" t="s">
-        <v>2368</v>
+        <v>143</v>
       </c>
       <c r="J249" s="4" t="s">
-        <v>2373</v>
+        <v>1807</v>
       </c>
       <c r="K249" s="4" t="s">
-        <v>2374</v>
+        <v>2083</v>
       </c>
       <c r="L249" s="4" t="s">
-        <v>2375</v>
+        <v>192</v>
       </c>
       <c r="M249" s="4" t="s">
-        <v>2376</v>
+        <v>839</v>
       </c>
       <c r="N249" s="4" t="s">
-        <v>2377</v>
+        <v>227</v>
       </c>
       <c r="O249" s="4" t="s">
-        <v>2378</v>
+        <v>271</v>
       </c>
       <c r="P249" s="4" t="s">
-        <v>2379</v>
+        <v>919</v>
       </c>
     </row>
     <row r="250" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A250" s="4" t="s">
-        <v>2382</v>
+        <v>482</v>
       </c>
       <c r="B250" s="4" t="s">
-        <v>2381</v>
+        <v>55</v>
       </c>
       <c r="C250" s="4" t="s">
-        <v>2386</v>
+        <v>1517</v>
       </c>
       <c r="D250" s="4" t="s">
-        <v>2387</v>
+        <v>1769</v>
       </c>
       <c r="E250" s="4" t="s">
-        <v>2388</v>
+        <v>2068</v>
       </c>
       <c r="F250" s="4" t="s">
-        <v>2389</v>
+        <v>315</v>
       </c>
       <c r="G250" s="4" t="s">
-        <v>2390</v>
+        <v>1784</v>
       </c>
       <c r="H250" s="4" t="s">
-        <v>2391</v>
+        <v>104</v>
       </c>
       <c r="I250" s="4" t="s">
-        <v>2392</v>
+        <v>145</v>
       </c>
       <c r="J250" s="4" t="s">
-        <v>2393</v>
+        <v>1809</v>
       </c>
       <c r="K250" s="4" t="s">
-        <v>2394</v>
+        <v>2085</v>
       </c>
       <c r="L250" s="4" t="s">
-        <v>2395</v>
+        <v>194</v>
       </c>
       <c r="M250" s="4" t="s">
-        <v>2396</v>
+        <v>841</v>
       </c>
       <c r="N250" s="4" t="s">
-        <v>2397</v>
+        <v>229</v>
       </c>
       <c r="O250" s="4" t="s">
-        <v>2385</v>
+        <v>273</v>
       </c>
       <c r="P250" s="4" t="s">
-        <v>2384</v>
+        <v>921</v>
       </c>
     </row>
     <row r="251" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A251" s="4" t="s">
-        <v>1043</v>
+        <v>2364</v>
       </c>
       <c r="B251" s="4" t="s">
-        <v>1044</v>
+        <v>2365</v>
       </c>
       <c r="C251" s="4" t="s">
-        <v>1570</v>
+        <v>2370</v>
       </c>
       <c r="D251" s="4" t="s">
-        <v>1742</v>
+        <v>2366</v>
       </c>
       <c r="E251" s="4" t="s">
-        <v>2048</v>
+        <v>2371</v>
       </c>
       <c r="F251" s="4" t="s">
-        <v>304</v>
+        <v>2372</v>
       </c>
       <c r="G251" s="4" t="s">
-        <v>1751</v>
+        <v>2369</v>
       </c>
       <c r="H251" s="4" t="s">
-        <v>94</v>
+        <v>2367</v>
       </c>
       <c r="I251" s="4" t="s">
-        <v>134</v>
+        <v>2368</v>
       </c>
       <c r="J251" s="4" t="s">
-        <v>1735</v>
+        <v>2373</v>
       </c>
       <c r="K251" s="4" t="s">
-        <v>2241</v>
+        <v>2374</v>
       </c>
       <c r="L251" s="4" t="s">
-        <v>185</v>
+        <v>2375</v>
       </c>
       <c r="M251" s="4" t="s">
-        <v>831</v>
+        <v>2376</v>
       </c>
       <c r="N251" s="4" t="s">
-        <v>221</v>
+        <v>2377</v>
       </c>
       <c r="O251" s="4" t="s">
-        <v>263</v>
+        <v>2378</v>
       </c>
       <c r="P251" s="4" t="s">
-        <v>911</v>
+        <v>2379</v>
       </c>
     </row>
     <row r="252" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A252" s="4" t="s">
-        <v>468</v>
+        <v>2382</v>
       </c>
       <c r="B252" s="4" t="s">
-        <v>50</v>
+        <v>2381</v>
       </c>
       <c r="C252" s="4" t="s">
-        <v>1511</v>
+        <v>2386</v>
       </c>
       <c r="D252" s="4" t="s">
-        <v>1764</v>
+        <v>2387</v>
       </c>
       <c r="E252" s="4" t="s">
-        <v>2062</v>
+        <v>2388</v>
       </c>
       <c r="F252" s="4" t="s">
-        <v>309</v>
+        <v>2389</v>
       </c>
       <c r="G252" s="4" t="s">
-        <v>1780</v>
+        <v>2390</v>
       </c>
       <c r="H252" s="4" t="s">
-        <v>99</v>
+        <v>2391</v>
       </c>
       <c r="I252" s="4" t="s">
-        <v>139</v>
+        <v>2392</v>
       </c>
       <c r="J252" s="4" t="s">
-        <v>1803</v>
+        <v>2393</v>
       </c>
       <c r="K252" s="4" t="s">
-        <v>2079</v>
+        <v>2394</v>
       </c>
       <c r="L252" s="4" t="s">
-        <v>190</v>
+        <v>2395</v>
       </c>
       <c r="M252" s="4" t="s">
-        <v>836</v>
+        <v>2396</v>
       </c>
       <c r="N252" s="4" t="s">
-        <v>225</v>
+        <v>2397</v>
       </c>
       <c r="O252" s="4" t="s">
-        <v>268</v>
+        <v>2385</v>
       </c>
       <c r="P252" s="4" t="s">
-        <v>916</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="253" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A253" s="4" t="s">
-        <v>469</v>
+        <v>1043</v>
       </c>
       <c r="B253" s="4" t="s">
-        <v>443</v>
+        <v>1044</v>
       </c>
       <c r="C253" s="4" t="s">
-        <v>1566</v>
+        <v>1570</v>
       </c>
       <c r="D253" s="4" t="s">
-        <v>1995</v>
+        <v>1742</v>
       </c>
       <c r="E253" s="4" t="s">
-        <v>2065</v>
+        <v>2048</v>
       </c>
       <c r="F253" s="4" t="s">
-        <v>637</v>
+        <v>304</v>
       </c>
       <c r="G253" s="4" t="s">
-        <v>1998</v>
+        <v>1751</v>
       </c>
       <c r="H253" s="4" t="s">
-        <v>642</v>
+        <v>94</v>
       </c>
       <c r="I253" s="4" t="s">
-        <v>659</v>
+        <v>134</v>
       </c>
       <c r="J253" s="4" t="s">
-        <v>2001</v>
+        <v>1735</v>
       </c>
       <c r="K253" s="4" t="s">
-        <v>2082</v>
+        <v>2241</v>
       </c>
       <c r="L253" s="4" t="s">
-        <v>673</v>
+        <v>185</v>
       </c>
       <c r="M253" s="4" t="s">
-        <v>870</v>
+        <v>831</v>
       </c>
       <c r="N253" s="4" t="s">
-        <v>644</v>
+        <v>221</v>
       </c>
       <c r="O253" s="4" t="s">
-        <v>610</v>
+        <v>263</v>
       </c>
       <c r="P253" s="4" t="s">
-        <v>953</v>
+        <v>911</v>
       </c>
     </row>
     <row r="254" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A254" s="4" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B254" s="4" t="s">
-        <v>453</v>
+        <v>50</v>
       </c>
       <c r="C254" s="4" t="s">
-        <v>1578</v>
+        <v>1511</v>
       </c>
       <c r="D254" s="4" t="s">
-        <v>2004</v>
+        <v>1764</v>
       </c>
       <c r="E254" s="4" t="s">
-        <v>2312</v>
+        <v>2062</v>
       </c>
       <c r="F254" s="4" t="s">
-        <v>722</v>
+        <v>309</v>
       </c>
       <c r="G254" s="4" t="s">
-        <v>2016</v>
+        <v>1780</v>
       </c>
       <c r="H254" s="4" t="s">
-        <v>734</v>
+        <v>99</v>
       </c>
       <c r="I254" s="4" t="s">
-        <v>672</v>
+        <v>139</v>
       </c>
       <c r="J254" s="4" t="s">
-        <v>2028</v>
+        <v>1803</v>
       </c>
       <c r="K254" s="4" t="s">
-        <v>2324</v>
+        <v>2079</v>
       </c>
       <c r="L254" s="4" t="s">
-        <v>675</v>
+        <v>190</v>
       </c>
       <c r="M254" s="4" t="s">
-        <v>871</v>
+        <v>836</v>
       </c>
       <c r="N254" s="4" t="s">
-        <v>646</v>
+        <v>225</v>
       </c>
       <c r="O254" s="4" t="s">
-        <v>758</v>
+        <v>268</v>
       </c>
       <c r="P254" s="4" t="s">
-        <v>967</v>
+        <v>916</v>
       </c>
     </row>
     <row r="255" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A255" s="4" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B255" s="4" t="s">
-        <v>454</v>
+        <v>443</v>
       </c>
       <c r="C255" s="4" t="s">
-        <v>1579</v>
+        <v>1566</v>
       </c>
       <c r="D255" s="4" t="s">
-        <v>2005</v>
+        <v>1995</v>
       </c>
       <c r="E255" s="4" t="s">
-        <v>2313</v>
+        <v>2065</v>
       </c>
       <c r="F255" s="4" t="s">
-        <v>725</v>
+        <v>637</v>
       </c>
       <c r="G255" s="4" t="s">
-        <v>2017</v>
+        <v>1998</v>
       </c>
       <c r="H255" s="4" t="s">
-        <v>735</v>
+        <v>642</v>
       </c>
       <c r="I255" s="4" t="s">
-        <v>671</v>
+        <v>659</v>
       </c>
       <c r="J255" s="4" t="s">
-        <v>2029</v>
+        <v>2001</v>
       </c>
       <c r="K255" s="4" t="s">
-        <v>2325</v>
+        <v>2082</v>
       </c>
       <c r="L255" s="4" t="s">
-        <v>686</v>
+        <v>673</v>
       </c>
       <c r="M255" s="4" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="N255" s="4" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="O255" s="4" t="s">
-        <v>759</v>
+        <v>610</v>
       </c>
       <c r="P255" s="4" t="s">
-        <v>968</v>
+        <v>953</v>
       </c>
     </row>
     <row r="256" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A256" s="4" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B256" s="4" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C256" s="4" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
       <c r="D256" s="4" t="s">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="E256" s="4" t="s">
-        <v>2314</v>
+        <v>2312</v>
       </c>
       <c r="F256" s="4" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="G256" s="4" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="H256" s="4" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="I256" s="4" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="J256" s="4" t="s">
-        <v>2030</v>
+        <v>2028</v>
       </c>
       <c r="K256" s="4" t="s">
-        <v>2326</v>
+        <v>2324</v>
       </c>
       <c r="L256" s="4" t="s">
-        <v>687</v>
+        <v>675</v>
       </c>
       <c r="M256" s="4" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="N256" s="4" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="O256" s="4" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="P256" s="4" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
     </row>
     <row r="257" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A257" s="4" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B257" s="4" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C257" s="4" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
       <c r="D257" s="4" t="s">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="E257" s="4" t="s">
-        <v>2315</v>
+        <v>2313</v>
       </c>
       <c r="F257" s="4" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="G257" s="4" t="s">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="H257" s="4" t="s">
-        <v>745</v>
+        <v>735</v>
       </c>
       <c r="I257" s="4" t="s">
-        <v>661</v>
+        <v>671</v>
       </c>
       <c r="J257" s="4" t="s">
-        <v>2031</v>
+        <v>2029</v>
       </c>
       <c r="K257" s="4" t="s">
-        <v>2327</v>
+        <v>2325</v>
       </c>
       <c r="L257" s="4" t="s">
-        <v>676</v>
+        <v>686</v>
       </c>
       <c r="M257" s="4" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="N257" s="4" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="O257" s="4" t="s">
-        <v>690</v>
+        <v>759</v>
       </c>
       <c r="P257" s="4" t="s">
-        <v>958</v>
+        <v>968</v>
       </c>
     </row>
     <row r="258" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A258" s="4" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B258" s="4" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C258" s="4" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="D258" s="4" t="s">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="E258" s="4" t="s">
-        <v>2316</v>
+        <v>2314</v>
       </c>
       <c r="F258" s="4" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="G258" s="4" t="s">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="H258" s="4" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="I258" s="4" t="s">
-        <v>662</v>
+        <v>670</v>
       </c>
       <c r="J258" s="4" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="K258" s="4" t="s">
-        <v>2328</v>
+        <v>2326</v>
       </c>
       <c r="L258" s="4" t="s">
-        <v>677</v>
+        <v>687</v>
       </c>
       <c r="M258" s="4" t="s">
-        <v>978</v>
+        <v>873</v>
       </c>
       <c r="N258" s="4" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="O258" s="4" t="s">
-        <v>691</v>
+        <v>760</v>
       </c>
       <c r="P258" s="4" t="s">
-        <v>959</v>
+        <v>969</v>
       </c>
     </row>
     <row r="259" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A259" s="4" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B259" s="4" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C259" s="4" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
       <c r="D259" s="4" t="s">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="E259" s="4" t="s">
-        <v>2317</v>
+        <v>2315</v>
       </c>
       <c r="F259" s="4" t="s">
-        <v>723</v>
+        <v>727</v>
       </c>
       <c r="G259" s="4" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="H259" s="4" t="s">
-        <v>738</v>
+        <v>745</v>
       </c>
       <c r="I259" s="4" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="J259" s="4" t="s">
-        <v>2033</v>
+        <v>2031</v>
       </c>
       <c r="K259" s="4" t="s">
-        <v>2329</v>
+        <v>2327</v>
       </c>
       <c r="L259" s="4" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="M259" s="4" t="s">
-        <v>979</v>
+        <v>874</v>
       </c>
       <c r="N259" s="4" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="O259" s="4" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="P259" s="4" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
     </row>
     <row r="260" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A260" s="4" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B260" s="4" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C260" s="4" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="D260" s="4" t="s">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="E260" s="4" t="s">
-        <v>2318</v>
+        <v>2316</v>
       </c>
       <c r="F260" s="4" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G260" s="4" t="s">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="H260" s="4" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="I260" s="4" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="J260" s="4" t="s">
-        <v>2034</v>
+        <v>2032</v>
       </c>
       <c r="K260" s="4" t="s">
-        <v>2330</v>
+        <v>2328</v>
       </c>
       <c r="L260" s="4" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="M260" s="4" t="s">
-        <v>875</v>
+        <v>978</v>
       </c>
       <c r="N260" s="4" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="O260" s="4" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="P260" s="4" t="s">
-        <v>964</v>
+        <v>959</v>
       </c>
     </row>
     <row r="261" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A261" s="4" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B261" s="4" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C261" s="4" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="D261" s="4" t="s">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="E261" s="4" t="s">
-        <v>2319</v>
+        <v>2317</v>
       </c>
       <c r="F261" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="G261" s="4" t="s">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="H261" s="4" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="I261" s="4" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="J261" s="4" t="s">
-        <v>2035</v>
+        <v>2033</v>
       </c>
       <c r="K261" s="4" t="s">
-        <v>2331</v>
+        <v>2329</v>
       </c>
       <c r="L261" s="4" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="M261" s="4" t="s">
-        <v>876</v>
+        <v>979</v>
       </c>
       <c r="N261" s="4" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="O261" s="4" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="P261" s="4" t="s">
-        <v>965</v>
+        <v>960</v>
       </c>
     </row>
     <row r="262" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A262" s="4" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B262" s="4" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C262" s="4" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="D262" s="4" t="s">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="E262" s="4" t="s">
-        <v>2320</v>
+        <v>2318</v>
       </c>
       <c r="F262" s="4" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G262" s="4" t="s">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="H262" s="4" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="I262" s="4" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="J262" s="4" t="s">
-        <v>2036</v>
+        <v>2034</v>
       </c>
       <c r="K262" s="4" t="s">
-        <v>2332</v>
+        <v>2330</v>
       </c>
       <c r="L262" s="4" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="M262" s="4" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="N262" s="4" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="O262" s="4" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="P262" s="4" t="s">
-        <v>961</v>
+        <v>964</v>
       </c>
     </row>
     <row r="263" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A263" s="4" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B263" s="4" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C263" s="4" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="D263" s="4" t="s">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="E263" s="4" t="s">
-        <v>2321</v>
+        <v>2319</v>
       </c>
       <c r="F263" s="4" t="s">
-        <v>731</v>
+        <v>724</v>
       </c>
       <c r="G263" s="4" t="s">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="H263" s="4" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="I263" s="4" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="J263" s="4" t="s">
-        <v>2037</v>
+        <v>2035</v>
       </c>
       <c r="K263" s="4" t="s">
-        <v>2333</v>
+        <v>2331</v>
       </c>
       <c r="L263" s="4" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="M263" s="4" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="N263" s="4" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="O263" s="4" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="P263" s="4" t="s">
-        <v>962</v>
+        <v>965</v>
       </c>
     </row>
     <row r="264" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A264" s="4" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B264" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C264" s="4" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
       <c r="D264" s="4" t="s">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="E264" s="4" t="s">
-        <v>2322</v>
+        <v>2320</v>
       </c>
       <c r="F264" s="4" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="G264" s="4" t="s">
-        <v>2026</v>
+        <v>2024</v>
       </c>
       <c r="H264" s="4" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="I264" s="4" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="J264" s="4" t="s">
-        <v>2038</v>
+        <v>2036</v>
       </c>
       <c r="K264" s="4" t="s">
-        <v>2334</v>
+        <v>2332</v>
       </c>
       <c r="L264" s="4" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="M264" s="4" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="N264" s="4" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="O264" s="4" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="P264" s="4" t="s">
-        <v>966</v>
+        <v>961</v>
       </c>
     </row>
     <row r="265" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A265" s="4" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B265" s="4" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C265" s="4" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
       <c r="D265" s="4" t="s">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="E265" s="4" t="s">
-        <v>2323</v>
+        <v>2321</v>
       </c>
       <c r="F265" s="4" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="G265" s="4" t="s">
-        <v>2027</v>
+        <v>2025</v>
       </c>
       <c r="H265" s="4" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="I265" s="4" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="J265" s="4" t="s">
-        <v>2039</v>
+        <v>2037</v>
       </c>
       <c r="K265" s="4" t="s">
-        <v>2335</v>
+        <v>2333</v>
       </c>
       <c r="L265" s="4" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="M265" s="4" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="N265" s="4" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="O265" s="4" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="P265" s="4" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="266" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A266" s="4" t="s">
-        <v>710</v>
+        <v>480</v>
       </c>
       <c r="B266" s="4" t="s">
-        <v>746</v>
+        <v>463</v>
       </c>
       <c r="C266" s="4" t="s">
-        <v>746</v>
+        <v>1588</v>
       </c>
       <c r="D266" s="4" t="s">
-        <v>746</v>
+        <v>2014</v>
       </c>
       <c r="E266" s="4" t="s">
-        <v>746</v>
+        <v>2322</v>
       </c>
       <c r="F266" s="4" t="s">
-        <v>746</v>
+        <v>732</v>
       </c>
       <c r="G266" s="4" t="s">
-        <v>746</v>
+        <v>2026</v>
       </c>
       <c r="H266" s="4" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="I266" s="4" t="s">
-        <v>746</v>
+        <v>668</v>
       </c>
       <c r="J266" s="4" t="s">
-        <v>746</v>
+        <v>2038</v>
       </c>
       <c r="K266" s="4" t="s">
-        <v>746</v>
+        <v>2334</v>
       </c>
       <c r="L266" s="4" t="s">
-        <v>746</v>
+        <v>683</v>
       </c>
       <c r="M266" s="4" t="s">
-        <v>746</v>
+        <v>879</v>
       </c>
       <c r="N266" s="4" t="s">
-        <v>746</v>
+        <v>656</v>
       </c>
       <c r="O266" s="4" t="s">
-        <v>746</v>
+        <v>697</v>
       </c>
       <c r="P266" s="4" t="s">
-        <v>746</v>
+        <v>966</v>
       </c>
     </row>
     <row r="267" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A267" s="4" t="s">
-        <v>711</v>
+        <v>481</v>
       </c>
       <c r="B267" s="4" t="s">
-        <v>747</v>
+        <v>464</v>
       </c>
       <c r="C267" s="4" t="s">
-        <v>747</v>
+        <v>1589</v>
       </c>
       <c r="D267" s="4" t="s">
-        <v>747</v>
+        <v>2015</v>
       </c>
       <c r="E267" s="4" t="s">
-        <v>747</v>
+        <v>2323</v>
       </c>
       <c r="F267" s="4" t="s">
-        <v>747</v>
+        <v>733</v>
       </c>
       <c r="G267" s="4" t="s">
-        <v>747</v>
+        <v>2027</v>
       </c>
       <c r="H267" s="4" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="I267" s="4" t="s">
-        <v>747</v>
+        <v>669</v>
       </c>
       <c r="J267" s="4" t="s">
-        <v>747</v>
+        <v>2039</v>
       </c>
       <c r="K267" s="4" t="s">
-        <v>747</v>
+        <v>2335</v>
       </c>
       <c r="L267" s="4" t="s">
-        <v>747</v>
+        <v>684</v>
       </c>
       <c r="M267" s="4" t="s">
-        <v>747</v>
+        <v>880</v>
       </c>
       <c r="N267" s="4" t="s">
-        <v>747</v>
+        <v>657</v>
       </c>
       <c r="O267" s="4" t="s">
-        <v>747</v>
+        <v>698</v>
       </c>
       <c r="P267" s="4" t="s">
-        <v>747</v>
+        <v>963</v>
       </c>
     </row>
     <row r="268" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A268" s="4" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B268" s="4" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C268" s="4" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D268" s="4" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="E268" s="4" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="F268" s="4" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="G268" s="4" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="H268" s="4" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="I268" s="4" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="J268" s="4" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="K268" s="4" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="L268" s="4" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="M268" s="4" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="N268" s="4" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="O268" s="4" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="P268" s="4" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="269" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A269" s="4" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B269" s="4" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="C269" s="4" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="D269" s="4" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E269" s="4" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="F269" s="4" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="G269" s="4" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="H269" s="4" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="I269" s="4" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="J269" s="4" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="K269" s="4" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="L269" s="4" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="M269" s="4" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="N269" s="4" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="O269" s="4" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="P269" s="4" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
     </row>
     <row r="270" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A270" s="4" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B270" s="4" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="C270" s="4" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="D270" s="4" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="E270" s="4" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="F270" s="4" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="G270" s="4" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="H270" s="4" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="I270" s="4" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="J270" s="4" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="K270" s="4" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="L270" s="4" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="M270" s="4" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="N270" s="4" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="O270" s="4" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="P270" s="4" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
     </row>
     <row r="271" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A271" s="4" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B271" s="4" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C271" s="4" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="D271" s="4" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="E271" s="4" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="F271" s="4" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="G271" s="4" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="H271" s="4" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="I271" s="4" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="J271" s="4" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="K271" s="4" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="L271" s="4" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="M271" s="4" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="N271" s="4" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="O271" s="4" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="P271" s="4" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
     </row>
     <row r="272" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A272" s="4" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="B272" s="4" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="C272" s="4" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="D272" s="4" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="E272" s="4" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="F272" s="4" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="G272" s="4" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="H272" s="4" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="I272" s="4" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="J272" s="4" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="K272" s="4" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="L272" s="4" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="M272" s="4" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="N272" s="4" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="O272" s="4" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="P272" s="4" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="273" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A273" s="4" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B273" s="4" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="C273" s="4" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="D273" s="4" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="E273" s="4" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="F273" s="4" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="G273" s="4" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="H273" s="4" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="I273" s="4" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="J273" s="4" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="K273" s="4" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="L273" s="4" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="M273" s="4" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="N273" s="4" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="O273" s="4" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="P273" s="4" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
     </row>
     <row r="274" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A274" s="4" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B274" s="4" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="C274" s="4" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="D274" s="4" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="E274" s="4" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="F274" s="4" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="G274" s="4" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="H274" s="4" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="I274" s="4" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="J274" s="4" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="K274" s="4" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="L274" s="4" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="M274" s="4" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="N274" s="4" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="O274" s="4" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="P274" s="4" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="275" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A275" s="4" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B275" s="4" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="C275" s="4" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="D275" s="4" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="E275" s="4" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="F275" s="4" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="G275" s="4" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="H275" s="4" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="I275" s="4" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="J275" s="4" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="K275" s="4" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="L275" s="4" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="M275" s="4" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="N275" s="4" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="O275" s="4" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="P275" s="4" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="276" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A276" s="4" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="B276" s="4" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="C276" s="4" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="D276" s="4" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="E276" s="4" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="F276" s="4" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="G276" s="4" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="H276" s="4" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="I276" s="4" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="J276" s="4" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="K276" s="4" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="L276" s="4" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="M276" s="4" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="N276" s="4" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="O276" s="4" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="P276" s="4" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="277" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A277" s="4" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="B277" s="4" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="C277" s="4" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="D277" s="4" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E277" s="4" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F277" s="4" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="G277" s="4" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="H277" s="4" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="I277" s="4" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="J277" s="4" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="K277" s="4" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="L277" s="4" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="M277" s="4" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="N277" s="4" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="O277" s="4" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="P277" s="4" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="278" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>755</v>
+      </c>
+    </row>
+    <row r="278" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A278" s="4" t="s">
+        <v>720</v>
+      </c>
+      <c r="B278" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="C278" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="D278" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="E278" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="F278" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="G278" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="H278" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="I278" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="J278" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="K278" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="L278" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="M278" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="N278" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="O278" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="P278" s="4" t="s">
+        <v>756</v>
+      </c>
+    </row>
     <row r="279" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A279" s="4" t="s">
-        <v>1002</v>
+        <v>721</v>
       </c>
       <c r="B279" s="4" t="s">
-        <v>1006</v>
+        <v>757</v>
       </c>
       <c r="C279" s="4" t="s">
-        <v>1571</v>
+        <v>757</v>
       </c>
       <c r="D279" s="4" t="s">
-        <v>1837</v>
+        <v>757</v>
       </c>
       <c r="E279" s="4" t="s">
-        <v>2242</v>
+        <v>757</v>
       </c>
       <c r="F279" s="4" t="s">
-        <v>1127</v>
+        <v>757</v>
       </c>
       <c r="G279" s="4" t="s">
-        <v>1841</v>
+        <v>757</v>
       </c>
       <c r="H279" s="4" t="s">
-        <v>1126</v>
+        <v>757</v>
       </c>
       <c r="I279" s="4" t="s">
-        <v>1006</v>
+        <v>757</v>
       </c>
       <c r="J279" s="4" t="s">
-        <v>1845</v>
+        <v>757</v>
       </c>
       <c r="K279" s="4" t="s">
-        <v>2246</v>
+        <v>757</v>
       </c>
       <c r="L279" s="4" t="s">
-        <v>1144</v>
+        <v>757</v>
       </c>
       <c r="M279" s="4" t="s">
-        <v>1143</v>
+        <v>757</v>
       </c>
       <c r="N279" s="4" t="s">
-        <v>1126</v>
+        <v>757</v>
       </c>
       <c r="O279" s="4" t="s">
-        <v>1145</v>
+        <v>757</v>
       </c>
       <c r="P279" s="4" t="s">
-        <v>1146</v>
-      </c>
-    </row>
-    <row r="280" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A280" s="4" t="s">
-        <v>1003</v>
-      </c>
-      <c r="B280" s="4" t="s">
-        <v>1007</v>
-      </c>
-      <c r="C280" s="4" t="s">
-        <v>1572</v>
-      </c>
-      <c r="D280" s="4" t="s">
-        <v>1838</v>
-      </c>
-      <c r="E280" s="4" t="s">
-        <v>2243</v>
-      </c>
-      <c r="F280" s="4" t="s">
-        <v>1129</v>
-      </c>
-      <c r="G280" s="4" t="s">
-        <v>1842</v>
-      </c>
-      <c r="H280" s="4" t="s">
-        <v>1130</v>
-      </c>
-      <c r="I280" s="4" t="s">
-        <v>1128</v>
-      </c>
-      <c r="J280" s="4" t="s">
-        <v>1846</v>
-      </c>
-      <c r="K280" s="4" t="s">
-        <v>2247</v>
-      </c>
-      <c r="L280" s="4" t="s">
-        <v>1140</v>
-      </c>
-      <c r="M280" s="4" t="s">
-        <v>1141</v>
-      </c>
-      <c r="N280" s="4" t="s">
-        <v>1142</v>
-      </c>
-      <c r="O280" s="4" t="s">
-        <v>1152</v>
-      </c>
-      <c r="P280" s="4" t="s">
-        <v>1151</v>
-      </c>
-    </row>
+        <v>757</v>
+      </c>
+    </row>
+    <row r="280" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="281" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A281" s="4" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="B281" s="4" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="C281" s="4" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
       <c r="D281" s="4" t="s">
-        <v>1839</v>
+        <v>1837</v>
       </c>
       <c r="E281" s="4" t="s">
-        <v>2244</v>
+        <v>2242</v>
       </c>
       <c r="F281" s="4" t="s">
-        <v>1132</v>
+        <v>1127</v>
       </c>
       <c r="G281" s="4" t="s">
-        <v>1843</v>
+        <v>1841</v>
       </c>
       <c r="H281" s="4" t="s">
-        <v>1131</v>
+        <v>1126</v>
       </c>
       <c r="I281" s="4" t="s">
-        <v>1133</v>
+        <v>1006</v>
       </c>
       <c r="J281" s="4" t="s">
-        <v>1847</v>
+        <v>1845</v>
       </c>
       <c r="K281" s="4" t="s">
-        <v>2248</v>
+        <v>2246</v>
       </c>
       <c r="L281" s="4" t="s">
-        <v>1138</v>
+        <v>1144</v>
       </c>
       <c r="M281" s="4" t="s">
-        <v>1139</v>
+        <v>1143</v>
       </c>
       <c r="N281" s="4" t="s">
-        <v>1131</v>
+        <v>1126</v>
       </c>
       <c r="O281" s="4" t="s">
-        <v>1149</v>
+        <v>1145</v>
       </c>
       <c r="P281" s="4" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="282" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A282" s="4" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="B282" s="4" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="C282" s="4" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
       <c r="D282" s="4" t="s">
-        <v>1840</v>
+        <v>1838</v>
       </c>
       <c r="E282" s="4" t="s">
-        <v>2245</v>
+        <v>2243</v>
       </c>
       <c r="F282" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="G282" s="4" t="s">
-        <v>1844</v>
+        <v>1842</v>
       </c>
       <c r="H282" s="4" t="s">
-        <v>1135</v>
+        <v>1130</v>
       </c>
       <c r="I282" s="4" t="s">
-        <v>1134</v>
+        <v>1128</v>
       </c>
       <c r="J282" s="4" t="s">
-        <v>1848</v>
+        <v>1846</v>
       </c>
       <c r="K282" s="4" t="s">
-        <v>2249</v>
+        <v>2247</v>
       </c>
       <c r="L282" s="4" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="M282" s="4" t="s">
-        <v>1137</v>
+        <v>1141</v>
       </c>
       <c r="N282" s="4" t="s">
-        <v>1135</v>
+        <v>1142</v>
       </c>
       <c r="O282" s="4" t="s">
-        <v>1148</v>
+        <v>1152</v>
       </c>
       <c r="P282" s="4" t="s">
-        <v>1147</v>
-      </c>
-    </row>
-    <row r="283" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="283" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A283" s="4" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B283" s="4" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C283" s="4" t="s">
+        <v>1573</v>
+      </c>
+      <c r="D283" s="4" t="s">
+        <v>1839</v>
+      </c>
+      <c r="E283" s="4" t="s">
+        <v>2244</v>
+      </c>
+      <c r="F283" s="4" t="s">
+        <v>1132</v>
+      </c>
+      <c r="G283" s="4" t="s">
+        <v>1843</v>
+      </c>
+      <c r="H283" s="4" t="s">
+        <v>1131</v>
+      </c>
+      <c r="I283" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="J283" s="4" t="s">
+        <v>1847</v>
+      </c>
+      <c r="K283" s="4" t="s">
+        <v>2248</v>
+      </c>
+      <c r="L283" s="4" t="s">
+        <v>1138</v>
+      </c>
+      <c r="M283" s="4" t="s">
+        <v>1139</v>
+      </c>
+      <c r="N283" s="4" t="s">
+        <v>1131</v>
+      </c>
+      <c r="O283" s="4" t="s">
+        <v>1149</v>
+      </c>
+      <c r="P283" s="4" t="s">
+        <v>1150</v>
+      </c>
+    </row>
     <row r="284" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A284" s="4" t="s">
-        <v>2447</v>
+        <v>1005</v>
       </c>
       <c r="B284" s="4" t="s">
-        <v>2448</v>
+        <v>1009</v>
       </c>
       <c r="C284" s="4" t="s">
-        <v>2455</v>
+        <v>1574</v>
       </c>
       <c r="D284" s="4" t="s">
-        <v>2454</v>
+        <v>1840</v>
       </c>
       <c r="E284" s="4" t="s">
-        <v>2453</v>
+        <v>2245</v>
       </c>
       <c r="F284" s="4" t="s">
-        <v>2452</v>
+        <v>1136</v>
       </c>
       <c r="G284" s="4" t="s">
-        <v>2451</v>
+        <v>1844</v>
       </c>
       <c r="H284" s="4" t="s">
-        <v>2450</v>
+        <v>1135</v>
       </c>
       <c r="I284" s="4" t="s">
-        <v>2449</v>
+        <v>1134</v>
       </c>
       <c r="J284" s="4" t="s">
-        <v>2456</v>
+        <v>1848</v>
       </c>
       <c r="K284" s="4" t="s">
-        <v>2457</v>
+        <v>2249</v>
       </c>
       <c r="L284" s="4" t="s">
-        <v>2458</v>
+        <v>1135</v>
       </c>
       <c r="M284" s="4" t="s">
-        <v>2459</v>
+        <v>1137</v>
       </c>
       <c r="N284" s="4" t="s">
-        <v>2460</v>
+        <v>1135</v>
       </c>
       <c r="O284" s="4" t="s">
-        <v>2461</v>
+        <v>1148</v>
       </c>
       <c r="P284" s="4" t="s">
-        <v>2462</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="285" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="286" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A286" s="4" t="s">
-        <v>40</v>
+        <v>2447</v>
       </c>
       <c r="B286" s="4" t="s">
-        <v>79</v>
+        <v>2448</v>
       </c>
       <c r="C286" s="4" t="s">
-        <v>1499</v>
+        <v>2455</v>
       </c>
       <c r="D286" s="4" t="s">
-        <v>1713</v>
+        <v>2454</v>
       </c>
       <c r="E286" s="4" t="s">
-        <v>2250</v>
+        <v>2453</v>
       </c>
       <c r="F286" s="4" t="s">
-        <v>300</v>
+        <v>2452</v>
       </c>
       <c r="G286" s="4" t="s">
-        <v>1722</v>
+        <v>2451</v>
       </c>
       <c r="H286" s="4" t="s">
-        <v>116</v>
+        <v>2450</v>
       </c>
       <c r="I286" s="4" t="s">
-        <v>128</v>
+        <v>2449</v>
       </c>
       <c r="J286" s="4" t="s">
-        <v>1829</v>
+        <v>2456</v>
       </c>
       <c r="K286" s="4" t="s">
-        <v>2252</v>
+        <v>2457</v>
       </c>
       <c r="L286" s="4" t="s">
-        <v>179</v>
+        <v>2458</v>
       </c>
       <c r="M286" s="4" t="s">
-        <v>825</v>
+        <v>2459</v>
       </c>
       <c r="N286" s="4" t="s">
-        <v>219</v>
+        <v>2460</v>
       </c>
       <c r="O286" s="4" t="s">
-        <v>257</v>
+        <v>2461</v>
       </c>
       <c r="P286" s="4" t="s">
-        <v>907</v>
-      </c>
-    </row>
-    <row r="287" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A287" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B287" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C287" s="4" t="s">
-        <v>1576</v>
-      </c>
-      <c r="D287" s="4" t="s">
-        <v>1827</v>
-      </c>
-      <c r="E287" s="4" t="s">
-        <v>2251</v>
-      </c>
-      <c r="F287" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G287" s="4" t="s">
-        <v>1828</v>
-      </c>
-      <c r="H287" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="I287" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J287" s="4" t="s">
-        <v>1830</v>
-      </c>
-      <c r="K287" s="4" t="s">
-        <v>2253</v>
-      </c>
-      <c r="L287" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="M287" s="4" t="s">
-        <v>881</v>
-      </c>
-      <c r="N287" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="O287" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="P287" s="4" t="s">
-        <v>944</v>
-      </c>
-    </row>
+        <v>2462</v>
+      </c>
+    </row>
+    <row r="287" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="288" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A288" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B288" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C288" s="4" t="s">
-        <v>1577</v>
+        <v>1499</v>
       </c>
       <c r="D288" s="4" t="s">
-        <v>1832</v>
+        <v>1713</v>
       </c>
       <c r="E288" s="4" t="s">
-        <v>2255</v>
+        <v>2250</v>
       </c>
       <c r="F288" s="4" t="s">
-        <v>333</v>
+        <v>300</v>
       </c>
       <c r="G288" s="4" t="s">
-        <v>1833</v>
+        <v>1722</v>
       </c>
       <c r="H288" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I288" s="4" t="s">
-        <v>162</v>
+        <v>128</v>
       </c>
       <c r="J288" s="4" t="s">
-        <v>1831</v>
+        <v>1829</v>
       </c>
       <c r="K288" s="4" t="s">
-        <v>2254</v>
+        <v>2252</v>
       </c>
       <c r="L288" s="4" t="s">
-        <v>210</v>
+        <v>179</v>
       </c>
       <c r="M288" s="4" t="s">
-        <v>882</v>
+        <v>825</v>
       </c>
       <c r="N288" s="4" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
       <c r="O288" s="4" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="P288" s="4" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="289" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>907</v>
+      </c>
+    </row>
+    <row r="289" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A289" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B289" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C289" s="4" t="s">
+        <v>1576</v>
+      </c>
+      <c r="D289" s="4" t="s">
+        <v>1827</v>
+      </c>
+      <c r="E289" s="4" t="s">
+        <v>2251</v>
+      </c>
+      <c r="F289" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G289" s="4" t="s">
+        <v>1828</v>
+      </c>
+      <c r="H289" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="I289" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J289" s="4" t="s">
+        <v>1830</v>
+      </c>
+      <c r="K289" s="4" t="s">
+        <v>2253</v>
+      </c>
+      <c r="L289" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M289" s="4" t="s">
+        <v>881</v>
+      </c>
+      <c r="N289" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="O289" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="P289" s="4" t="s">
+        <v>944</v>
+      </c>
+    </row>
     <row r="290" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A290" s="4" t="s">
-        <v>2415</v>
+        <v>39</v>
       </c>
       <c r="B290" s="4" t="s">
-        <v>2417</v>
+        <v>82</v>
       </c>
       <c r="C290" s="4" t="s">
-        <v>2419</v>
+        <v>1577</v>
       </c>
       <c r="D290" s="4" t="s">
-        <v>2441</v>
+        <v>1832</v>
       </c>
       <c r="E290" s="4" t="s">
-        <v>2442</v>
+        <v>2255</v>
       </c>
       <c r="F290" s="4" t="s">
-        <v>2443</v>
+        <v>333</v>
       </c>
       <c r="G290" s="4" t="s">
-        <v>2444</v>
+        <v>1833</v>
       </c>
       <c r="H290" s="4" t="s">
-        <v>2445</v>
+        <v>119</v>
       </c>
       <c r="I290" s="4" t="s">
-        <v>2446</v>
+        <v>162</v>
       </c>
       <c r="J290" s="4" t="s">
-        <v>2440</v>
+        <v>1831</v>
       </c>
       <c r="K290" s="4" t="s">
-        <v>2439</v>
+        <v>2254</v>
       </c>
       <c r="L290" s="4" t="s">
-        <v>2438</v>
+        <v>210</v>
       </c>
       <c r="M290" s="4" t="s">
-        <v>2437</v>
+        <v>882</v>
       </c>
       <c r="N290" s="4" t="s">
-        <v>2436</v>
+        <v>247</v>
       </c>
       <c r="O290" s="4" t="s">
-        <v>2435</v>
+        <v>291</v>
       </c>
       <c r="P290" s="4" t="s">
-        <v>2434</v>
-      </c>
-    </row>
-    <row r="291" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A291" s="4" t="s">
-        <v>2414</v>
-      </c>
-      <c r="B291" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C291" s="4" t="s">
-        <v>1575</v>
-      </c>
-      <c r="D291" s="4" t="s">
-        <v>1834</v>
-      </c>
-      <c r="E291" s="4" t="s">
-        <v>2256</v>
-      </c>
-      <c r="F291" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="G291" s="4" t="s">
-        <v>1835</v>
-      </c>
-      <c r="H291" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="I291" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="J291" s="4" t="s">
-        <v>1836</v>
-      </c>
-      <c r="K291" s="4" t="s">
-        <v>2257</v>
-      </c>
-      <c r="L291" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="M291" s="4" t="s">
-        <v>883</v>
-      </c>
-      <c r="N291" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="O291" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="P291" s="4" t="s">
-        <v>946</v>
-      </c>
-    </row>
+        <v>945</v>
+      </c>
+    </row>
+    <row r="291" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="292" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A292" s="4" t="s">
+        <v>2415</v>
+      </c>
+      <c r="B292" s="4" t="s">
+        <v>2417</v>
+      </c>
+      <c r="C292" s="4" t="s">
+        <v>2419</v>
+      </c>
+      <c r="D292" s="4" t="s">
+        <v>2441</v>
+      </c>
+      <c r="E292" s="4" t="s">
+        <v>2442</v>
+      </c>
+      <c r="F292" s="4" t="s">
+        <v>2443</v>
+      </c>
+      <c r="G292" s="4" t="s">
+        <v>2444</v>
+      </c>
+      <c r="H292" s="4" t="s">
+        <v>2445</v>
+      </c>
+      <c r="I292" s="4" t="s">
+        <v>2446</v>
+      </c>
+      <c r="J292" s="4" t="s">
+        <v>2440</v>
+      </c>
+      <c r="K292" s="4" t="s">
+        <v>2439</v>
+      </c>
+      <c r="L292" s="4" t="s">
+        <v>2438</v>
+      </c>
+      <c r="M292" s="4" t="s">
+        <v>2437</v>
+      </c>
+      <c r="N292" s="4" t="s">
+        <v>2436</v>
+      </c>
+      <c r="O292" s="4" t="s">
+        <v>2435</v>
+      </c>
+      <c r="P292" s="4" t="s">
+        <v>2434</v>
+      </c>
+    </row>
+    <row r="293" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A293" s="4" t="s">
+        <v>2414</v>
+      </c>
+      <c r="B293" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C293" s="4" t="s">
+        <v>1575</v>
+      </c>
+      <c r="D293" s="4" t="s">
+        <v>1834</v>
+      </c>
+      <c r="E293" s="4" t="s">
+        <v>2256</v>
+      </c>
+      <c r="F293" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="G293" s="4" t="s">
+        <v>1835</v>
+      </c>
+      <c r="H293" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I293" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="J293" s="4" t="s">
+        <v>1836</v>
+      </c>
+      <c r="K293" s="4" t="s">
+        <v>2257</v>
+      </c>
+      <c r="L293" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="M293" s="4" t="s">
+        <v>883</v>
+      </c>
+      <c r="N293" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="O293" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="P293" s="4" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="294" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A294" s="4" t="s">
         <v>2416</v>
       </c>
-      <c r="B292" s="4" t="s">
+      <c r="B294" s="4" t="s">
         <v>2418</v>
       </c>
-      <c r="C292" s="4" t="s">
+      <c r="C294" s="4" t="s">
         <v>2420</v>
       </c>
-      <c r="D292" s="4" t="s">
+      <c r="D294" s="4" t="s">
         <v>2421</v>
       </c>
-      <c r="E292" s="4" t="s">
+      <c r="E294" s="4" t="s">
         <v>2422</v>
       </c>
-      <c r="F292" s="4" t="s">
+      <c r="F294" s="4" t="s">
         <v>2423</v>
       </c>
-      <c r="G292" s="4" t="s">
+      <c r="G294" s="4" t="s">
         <v>2424</v>
       </c>
-      <c r="H292" s="5" t="s">
+      <c r="H294" s="5" t="s">
         <v>2425</v>
       </c>
-      <c r="I292" s="4" t="s">
+      <c r="I294" s="4" t="s">
         <v>2426</v>
       </c>
-      <c r="J292" s="4" t="s">
+      <c r="J294" s="4" t="s">
         <v>2427</v>
       </c>
-      <c r="K292" s="4" t="s">
+      <c r="K294" s="4" t="s">
         <v>2428</v>
       </c>
-      <c r="L292" s="4" t="s">
+      <c r="L294" s="4" t="s">
         <v>2429</v>
       </c>
-      <c r="M292" s="4" t="s">
+      <c r="M294" s="4" t="s">
         <v>2430</v>
       </c>
-      <c r="N292" s="4" t="s">
+      <c r="N294" s="4" t="s">
         <v>2431</v>
       </c>
-      <c r="O292" s="4" t="s">
+      <c r="O294" s="4" t="s">
         <v>2432</v>
       </c>
-      <c r="P292" s="4" t="s">
+      <c r="P294" s="4" t="s">
         <v>2433</v>
       </c>
     </row>

</xml_diff>

<commit_message>
II Server, II Core, II Windows: v1.3.0; Self-Installation II Windows - Window state, size, position persistant (#113)   - Saved on change, restored on load, edge case checking added - If update exists, prompts various options (#102)   - Option to download and bootstrap open installer   - Option to mute notification persists until newer version II Server: version.php posts http paths, hash for upgrading - MySQL table updated with fields, data II Core - Localization updated - Get_LatestVersion_Windows() relays upgrade paths, hash - File.MD5Hash() computes file hash
</commit_message>
<xml_diff>
--- a/II Core/Localization Strings.xlsx
+++ b/II Core/Localization Strings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibi\Documents\Infirmary Integrated\II Core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A61F96-78B1-4830-9712-F08754E69885}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588F1AC0-3FDF-4E46-9010-FAC476DA22BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="203" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="203" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8380" uniqueCount="3415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4302" uniqueCount="3527">
   <si>
     <t>Temperature</t>
   </si>
@@ -10270,6 +10270,342 @@
   </si>
   <si>
     <t>Chapisha picha ya skrini</t>
+  </si>
+  <si>
+    <t>UPGRADE:UpdateAvailable</t>
+  </si>
+  <si>
+    <t>A new version of Infirmary Integrated is available. Would you like to upgrade now?</t>
+  </si>
+  <si>
+    <t>UPGRADE:DownloadInstall</t>
+  </si>
+  <si>
+    <t>UPGRADE:OpenDownloadPage</t>
+  </si>
+  <si>
+    <t>UPGRADE:Later</t>
+  </si>
+  <si>
+    <t>UPGRADE:Mute</t>
+  </si>
+  <si>
+    <t>Download and Install Now</t>
+  </si>
+  <si>
+    <t>Open Download Website</t>
+  </si>
+  <si>
+    <t>Remind Me Later</t>
+  </si>
+  <si>
+    <t>Don't Remind Me</t>
+  </si>
+  <si>
+    <t>UPGRADE:Upgrade</t>
+  </si>
+  <si>
+    <t>Upgrade Infirmary Integrated</t>
+  </si>
+  <si>
+    <t>UPGRADE:Downloading</t>
+  </si>
+  <si>
+    <t>Download in process. The installer will run when it is finished downloading.</t>
+  </si>
+  <si>
+    <t>שדרג</t>
+  </si>
+  <si>
+    <t>अपग्रेड</t>
+  </si>
+  <si>
+    <t>አሻሽል</t>
+  </si>
+  <si>
+    <t>تطوير</t>
+  </si>
+  <si>
+    <t>升级</t>
+  </si>
+  <si>
+    <t>Aktualisierung</t>
+  </si>
+  <si>
+    <t>ارتقا</t>
+  </si>
+  <si>
+    <t>Mejorar</t>
+  </si>
+  <si>
+    <t>Améliorer</t>
+  </si>
+  <si>
+    <t>Aggiornamento</t>
+  </si>
+  <si>
+    <t>업그레이드</t>
+  </si>
+  <si>
+    <t>Melhorar</t>
+  </si>
+  <si>
+    <t>Обновить</t>
+  </si>
+  <si>
+    <t>Boresha</t>
+  </si>
+  <si>
+    <t>Toleo jipya la programu hiyo linapatikana. Je! Ungependa kusasisha sasa?</t>
+  </si>
+  <si>
+    <t>Доступна новая версия программы. Хотите обновить сейчас?</t>
+  </si>
+  <si>
+    <t>Una nueva versión del programa está disponible. ¿Desea actualizar ahora?</t>
+  </si>
+  <si>
+    <t>Une nouvelle version du programme est disponible. Voulez-vous mettre à jour maintenant?</t>
+  </si>
+  <si>
+    <t>È disponibile una nuova versione del programma. Vuoi aggiornare ora?</t>
+  </si>
+  <si>
+    <t>Uma nova versão do programa está disponível. Deseja atualizar agora?</t>
+  </si>
+  <si>
+    <t>새로운 버전의 프로그램을 사용할 수 있습니다. 지금 업그레이드 하시겠습니까?</t>
+  </si>
+  <si>
+    <t>कार्यक्रम का एक नया संस्करण उपलब्ध है। क्या आप अभी अपग्रेड करना चाहते हैं?</t>
+  </si>
+  <si>
+    <t>Eine neue Version des Programms ist verfügbar. Möchten Sie jetzt ein Upgrade durchführen?</t>
+  </si>
+  <si>
+    <t>نسخه جدیدی از برنامه موجود است. آیا اکنون می خواهید بروزرسانی کنید؟</t>
+  </si>
+  <si>
+    <t>גרסה חדשה של האפליקציה זמינה. האם ברצונך לעדכן עכשיו?</t>
+  </si>
+  <si>
+    <t>የመተግበሪያው አዲስ ስሪት ይገኛል። አሁን ማዘመን ይፈልጋሉ?</t>
+  </si>
+  <si>
+    <t>يتوفر إصدار جديد من البرنامج. هل ترغب في تحديث الآن؟</t>
+  </si>
+  <si>
+    <t>该程序有新版本。 您要现在更新吗？</t>
+  </si>
+  <si>
+    <t>立即下载并安装</t>
+  </si>
+  <si>
+    <t>تحميل وتثبيت الآن</t>
+  </si>
+  <si>
+    <t>አሁን ያውርዱ እና ይጫኑ</t>
+  </si>
+  <si>
+    <t>Jetzt herunterladen und installieren</t>
+  </si>
+  <si>
+    <t>اکنون بارگیری و نصب کنید</t>
+  </si>
+  <si>
+    <t>Descargue e instale ahora</t>
+  </si>
+  <si>
+    <t>Téléchargez et installez maintenant</t>
+  </si>
+  <si>
+    <t>הורד והתקן כעת</t>
+  </si>
+  <si>
+    <t>अभी डाउनलोड करें और इंस्टॉल करें</t>
+  </si>
+  <si>
+    <t>Scarica e installa ora</t>
+  </si>
+  <si>
+    <t>지금 다운로드하여 설치</t>
+  </si>
+  <si>
+    <t>Baixe e instale agora</t>
+  </si>
+  <si>
+    <t>Скачать и установить сейчас</t>
+  </si>
+  <si>
+    <t>Pakua na usanikishe sasa</t>
+  </si>
+  <si>
+    <t>Fungua tovuti</t>
+  </si>
+  <si>
+    <t>Открытый сайт</t>
+  </si>
+  <si>
+    <t>ድር ጣቢያ ይክፈቱ</t>
+  </si>
+  <si>
+    <t>افتح الموقع</t>
+  </si>
+  <si>
+    <t>开启网站</t>
+  </si>
+  <si>
+    <t>Webseite öffnen</t>
+  </si>
+  <si>
+    <t>باز کردن وب سایت</t>
+  </si>
+  <si>
+    <t>Abrir sitio web</t>
+  </si>
+  <si>
+    <t>Site ouvert</t>
+  </si>
+  <si>
+    <t>אתר פתוח</t>
+  </si>
+  <si>
+    <t>वेबसाइट खोलें</t>
+  </si>
+  <si>
+    <t>Apri il sito web</t>
+  </si>
+  <si>
+    <t>웹 사이트 열기</t>
+  </si>
+  <si>
+    <t>Abrir site</t>
+  </si>
+  <si>
+    <t>Lembre-me mais tarde</t>
+  </si>
+  <si>
+    <t>Ricordamelo più tardi</t>
+  </si>
+  <si>
+    <t>나중에 상기시켜 줘</t>
+  </si>
+  <si>
+    <t>Напомни мне позже</t>
+  </si>
+  <si>
+    <t>Nikumbushe baadaye</t>
+  </si>
+  <si>
+    <t>መጨረሻ ላይ አስታውሰኝ</t>
+  </si>
+  <si>
+    <t>ذكرني لاحقا</t>
+  </si>
+  <si>
+    <t>稍后提醒我</t>
+  </si>
+  <si>
+    <t>Erinnere mich später</t>
+  </si>
+  <si>
+    <t>بعدا به من یادآوری کن</t>
+  </si>
+  <si>
+    <t>Recuérdame más tarde</t>
+  </si>
+  <si>
+    <t>Rappelle-moi plus tard</t>
+  </si>
+  <si>
+    <t>תזכרו לי אחר כך</t>
+  </si>
+  <si>
+    <t>मुझे बाद में याद दिलाना</t>
+  </si>
+  <si>
+    <t>मुझे फिर से मत बताना</t>
+  </si>
+  <si>
+    <t>אל תגיד לי שוב</t>
+  </si>
+  <si>
+    <t>Non dirmelo più</t>
+  </si>
+  <si>
+    <t>다시 말 하지마</t>
+  </si>
+  <si>
+    <t>Não me diga de novo</t>
+  </si>
+  <si>
+    <t>Не говори мне снова</t>
+  </si>
+  <si>
+    <t>Usiniambie tena</t>
+  </si>
+  <si>
+    <t>لا تقل لي مرة أخرى</t>
+  </si>
+  <si>
+    <t>ድጋሜ አትነግረኝ</t>
+  </si>
+  <si>
+    <t>不要再告诉我</t>
+  </si>
+  <si>
+    <t>Sag es mir nicht noch einmal</t>
+  </si>
+  <si>
+    <t>دیگر به من نگو</t>
+  </si>
+  <si>
+    <t>No me digas mas</t>
+  </si>
+  <si>
+    <t>Ne me dis plus</t>
+  </si>
+  <si>
+    <t>Le téléchargement est en cours. Le programme d'installation s'exécutera une fois le téléchargement terminé.</t>
+  </si>
+  <si>
+    <t>La descarga está en progreso. El instalador se ejecutará una vez que se complete la descarga.</t>
+  </si>
+  <si>
+    <t>ההורדה מתבצעת. המתקין יפעל לאחר סיום ההורדה.</t>
+  </si>
+  <si>
+    <t>डाउनलोड प्रगति पर है। डाउनलोड पूरा होने के बाद इंस्टॉलर चलेगा।</t>
+  </si>
+  <si>
+    <t>A transferência está em processo. O instalador será executado quando terminar a transferência.</t>
+  </si>
+  <si>
+    <t>Il trasferimento è in corso. Il programma di installazione verrà eseguito al termine del trasferimento.</t>
+  </si>
+  <si>
+    <t>다운로드가 진행 중입니다. 다운로드가 완료되면 설치 관리자가 실행됩니다.</t>
+  </si>
+  <si>
+    <t>Загрузка продолжается. Когда загрузка будет завершена, установщик запустится.</t>
+  </si>
+  <si>
+    <t>Upakuaji unaendelea. Kisakinishi kitaendesha wakati imekamilika kupakua.</t>
+  </si>
+  <si>
+    <t>ማውረዱ በሂደት ላይ ነው። ጫኝው መጫኑን ሲያጠናቅቅ ይሠራል።</t>
+  </si>
+  <si>
+    <t>التنزيل قيد التنفيذ. سيتم تشغيل المثبت عند الانتهاء من التنزيل.</t>
+  </si>
+  <si>
+    <t>正在下载。 下载完成后，安装程序将运行。</t>
+  </si>
+  <si>
+    <t>Der herunterladen wird ausgeführt. Das Installationsprogramm wird ausgeführt, wenn der herunterladen abgeschlossen ist.</t>
+  </si>
+  <si>
+    <t>بارگیری در حال انجام است. پس از اتمام بارگیری ، نصب خواهد شد.</t>
   </si>
 </sst>
 </file>
@@ -10647,11 +10983,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P294"/>
+  <dimension ref="A1:P302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A212" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A220" sqref="A220:XFD221"/>
+      <pane ySplit="1" topLeftCell="A281" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D294" sqref="D294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="60.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23800,6 +24136,356 @@
         <v>2433</v>
       </c>
     </row>
+    <row r="296" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A296" s="4" t="s">
+        <v>3425</v>
+      </c>
+      <c r="B296" s="4" t="s">
+        <v>3426</v>
+      </c>
+      <c r="C296" s="4" t="s">
+        <v>3431</v>
+      </c>
+      <c r="D296" s="4" t="s">
+        <v>3432</v>
+      </c>
+      <c r="E296" s="4" t="s">
+        <v>3433</v>
+      </c>
+      <c r="F296" s="4" t="s">
+        <v>3434</v>
+      </c>
+      <c r="G296" s="4" t="s">
+        <v>3435</v>
+      </c>
+      <c r="H296" s="4" t="s">
+        <v>3436</v>
+      </c>
+      <c r="I296" s="4" t="s">
+        <v>3437</v>
+      </c>
+      <c r="J296" s="4" t="s">
+        <v>3429</v>
+      </c>
+      <c r="K296" s="4" t="s">
+        <v>3430</v>
+      </c>
+      <c r="L296" s="4" t="s">
+        <v>3438</v>
+      </c>
+      <c r="M296" s="4" t="s">
+        <v>3439</v>
+      </c>
+      <c r="N296" s="4" t="s">
+        <v>3440</v>
+      </c>
+      <c r="O296" s="4" t="s">
+        <v>3441</v>
+      </c>
+      <c r="P296" s="4" t="s">
+        <v>3442</v>
+      </c>
+    </row>
+    <row r="297" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A297" s="4" t="s">
+        <v>3415</v>
+      </c>
+      <c r="B297" s="4" t="s">
+        <v>3416</v>
+      </c>
+      <c r="C297" s="4" t="s">
+        <v>3454</v>
+      </c>
+      <c r="D297" s="4" t="s">
+        <v>3455</v>
+      </c>
+      <c r="E297" s="4" t="s">
+        <v>3456</v>
+      </c>
+      <c r="F297" s="4" t="s">
+        <v>3451</v>
+      </c>
+      <c r="G297" s="4" t="s">
+        <v>3452</v>
+      </c>
+      <c r="H297" s="4" t="s">
+        <v>3445</v>
+      </c>
+      <c r="I297" s="4" t="s">
+        <v>3446</v>
+      </c>
+      <c r="J297" s="4" t="s">
+        <v>3453</v>
+      </c>
+      <c r="K297" s="4" t="s">
+        <v>3450</v>
+      </c>
+      <c r="L297" s="4" t="s">
+        <v>3447</v>
+      </c>
+      <c r="M297" s="4" t="s">
+        <v>3449</v>
+      </c>
+      <c r="N297" s="4" t="s">
+        <v>3448</v>
+      </c>
+      <c r="O297" s="4" t="s">
+        <v>3444</v>
+      </c>
+      <c r="P297" s="4" t="s">
+        <v>3443</v>
+      </c>
+    </row>
+    <row r="298" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A298" s="4" t="s">
+        <v>3417</v>
+      </c>
+      <c r="B298" s="4" t="s">
+        <v>3421</v>
+      </c>
+      <c r="C298" s="4" t="s">
+        <v>3459</v>
+      </c>
+      <c r="D298" s="4" t="s">
+        <v>3458</v>
+      </c>
+      <c r="E298" s="4" t="s">
+        <v>3457</v>
+      </c>
+      <c r="F298" s="4" t="s">
+        <v>3460</v>
+      </c>
+      <c r="G298" s="4" t="s">
+        <v>3461</v>
+      </c>
+      <c r="H298" s="4" t="s">
+        <v>3462</v>
+      </c>
+      <c r="I298" s="4" t="s">
+        <v>3463</v>
+      </c>
+      <c r="J298" s="4" t="s">
+        <v>3464</v>
+      </c>
+      <c r="K298" s="4" t="s">
+        <v>3465</v>
+      </c>
+      <c r="L298" s="4" t="s">
+        <v>3466</v>
+      </c>
+      <c r="M298" s="4" t="s">
+        <v>3467</v>
+      </c>
+      <c r="N298" s="4" t="s">
+        <v>3468</v>
+      </c>
+      <c r="O298" s="4" t="s">
+        <v>3469</v>
+      </c>
+      <c r="P298" s="4" t="s">
+        <v>3470</v>
+      </c>
+    </row>
+    <row r="299" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A299" s="4" t="s">
+        <v>3418</v>
+      </c>
+      <c r="B299" s="4" t="s">
+        <v>3422</v>
+      </c>
+      <c r="C299" s="4" t="s">
+        <v>3473</v>
+      </c>
+      <c r="D299" s="4" t="s">
+        <v>3474</v>
+      </c>
+      <c r="E299" s="4" t="s">
+        <v>3475</v>
+      </c>
+      <c r="F299" s="4" t="s">
+        <v>3476</v>
+      </c>
+      <c r="G299" s="4" t="s">
+        <v>3477</v>
+      </c>
+      <c r="H299" s="4" t="s">
+        <v>3478</v>
+      </c>
+      <c r="I299" s="4" t="s">
+        <v>3479</v>
+      </c>
+      <c r="J299" s="4" t="s">
+        <v>3480</v>
+      </c>
+      <c r="K299" s="4" t="s">
+        <v>3481</v>
+      </c>
+      <c r="L299" s="4" t="s">
+        <v>3482</v>
+      </c>
+      <c r="M299" s="4" t="s">
+        <v>3483</v>
+      </c>
+      <c r="N299" s="4" t="s">
+        <v>3484</v>
+      </c>
+      <c r="O299" s="4" t="s">
+        <v>3472</v>
+      </c>
+      <c r="P299" s="4" t="s">
+        <v>3471</v>
+      </c>
+    </row>
+    <row r="300" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A300" s="4" t="s">
+        <v>3419</v>
+      </c>
+      <c r="B300" s="4" t="s">
+        <v>3423</v>
+      </c>
+      <c r="C300" s="4" t="s">
+        <v>3490</v>
+      </c>
+      <c r="D300" s="4" t="s">
+        <v>3491</v>
+      </c>
+      <c r="E300" s="4" t="s">
+        <v>3492</v>
+      </c>
+      <c r="F300" s="4" t="s">
+        <v>3493</v>
+      </c>
+      <c r="G300" s="4" t="s">
+        <v>3494</v>
+      </c>
+      <c r="H300" s="4" t="s">
+        <v>3495</v>
+      </c>
+      <c r="I300" s="4" t="s">
+        <v>3496</v>
+      </c>
+      <c r="J300" s="4" t="s">
+        <v>3497</v>
+      </c>
+      <c r="K300" s="4" t="s">
+        <v>3498</v>
+      </c>
+      <c r="L300" s="4" t="s">
+        <v>3486</v>
+      </c>
+      <c r="M300" s="4" t="s">
+        <v>3487</v>
+      </c>
+      <c r="N300" s="4" t="s">
+        <v>3485</v>
+      </c>
+      <c r="O300" s="4" t="s">
+        <v>3488</v>
+      </c>
+      <c r="P300" s="4" t="s">
+        <v>3489</v>
+      </c>
+    </row>
+    <row r="301" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A301" s="4" t="s">
+        <v>3420</v>
+      </c>
+      <c r="B301" s="4" t="s">
+        <v>3424</v>
+      </c>
+      <c r="C301" s="4" t="s">
+        <v>3507</v>
+      </c>
+      <c r="D301" s="4" t="s">
+        <v>3506</v>
+      </c>
+      <c r="E301" s="4" t="s">
+        <v>3508</v>
+      </c>
+      <c r="F301" s="4" t="s">
+        <v>3509</v>
+      </c>
+      <c r="G301" s="4" t="s">
+        <v>3510</v>
+      </c>
+      <c r="H301" s="4" t="s">
+        <v>3511</v>
+      </c>
+      <c r="I301" s="4" t="s">
+        <v>3512</v>
+      </c>
+      <c r="J301" s="4" t="s">
+        <v>3500</v>
+      </c>
+      <c r="K301" s="4" t="s">
+        <v>3499</v>
+      </c>
+      <c r="L301" s="4" t="s">
+        <v>3501</v>
+      </c>
+      <c r="M301" s="4" t="s">
+        <v>3502</v>
+      </c>
+      <c r="N301" s="4" t="s">
+        <v>3503</v>
+      </c>
+      <c r="O301" s="4" t="s">
+        <v>3504</v>
+      </c>
+      <c r="P301" s="4" t="s">
+        <v>3505</v>
+      </c>
+    </row>
+    <row r="302" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A302" s="4" t="s">
+        <v>3427</v>
+      </c>
+      <c r="B302" s="4" t="s">
+        <v>3428</v>
+      </c>
+      <c r="C302" s="4" t="s">
+        <v>3522</v>
+      </c>
+      <c r="D302" s="4" t="s">
+        <v>3523</v>
+      </c>
+      <c r="E302" s="4" t="s">
+        <v>3524</v>
+      </c>
+      <c r="F302" s="4" t="s">
+        <v>3525</v>
+      </c>
+      <c r="G302" s="4" t="s">
+        <v>3526</v>
+      </c>
+      <c r="H302" s="4" t="s">
+        <v>3514</v>
+      </c>
+      <c r="I302" s="4" t="s">
+        <v>3513</v>
+      </c>
+      <c r="J302" s="4" t="s">
+        <v>3515</v>
+      </c>
+      <c r="K302" s="4" t="s">
+        <v>3516</v>
+      </c>
+      <c r="L302" s="4" t="s">
+        <v>3518</v>
+      </c>
+      <c r="M302" s="4" t="s">
+        <v>3519</v>
+      </c>
+      <c r="N302" s="5" t="s">
+        <v>3517</v>
+      </c>
+      <c r="O302" s="4" t="s">
+        <v>3520</v>
+      </c>
+      <c r="P302" s="4" t="s">
+        <v>3521</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>